<commit_message>
cambios a 0114 y 0115
</commit_message>
<xml_diff>
--- a/03_ips_clean/00_ips_wide_norm_complete.xlsx
+++ b/03_ips_clean/00_ips_wide_norm_complete.xlsx
@@ -950,13 +950,13 @@
         <v>0.422256551002962</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0625332305408447</v>
+        <v>0.0669019166655314</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.123212775155093</v>
+        <v>0.126006753086738</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.0360054274476526</v>
+        <v>-0.0375403915665097</v>
       </c>
       <c r="S2" t="n">
         <v>-0.18882416799571</v>
@@ -1126,13 +1126,13 @@
         <v>0.980729453309989</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0597997673844625</v>
+        <v>0.0641516598826344</v>
       </c>
       <c r="Q3" t="n">
-        <v>-1.65161203171721</v>
+        <v>-1.68906405373724</v>
       </c>
       <c r="R3" t="n">
-        <v>0.141107996962751</v>
+        <v>0.143326428547803</v>
       </c>
       <c r="S3" t="n">
         <v>1.77604750729784</v>
@@ -1302,13 +1302,13 @@
         <v>0.0836960557978047</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.286603452372981</v>
+        <v>-0.284379763535628</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.675458387937445</v>
+        <v>-0.690775109984053</v>
       </c>
       <c r="R4" t="n">
-        <v>-1.94430407731597</v>
+        <v>-1.98627979276712</v>
       </c>
       <c r="S4" t="n">
         <v>1.12109028219999</v>
@@ -1478,13 +1478,13 @@
         <v>0.101108296213635</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.848490893002359</v>
+        <v>-0.849719282090128</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.320493426562984</v>
+        <v>-0.327760948619257</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.964820110969772</v>
+        <v>-0.98603855788766</v>
       </c>
       <c r="S5" t="n">
         <v>0.557827068615837</v>
@@ -1654,13 +1654,13 @@
         <v>0.820924051315604</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.249398000495473</v>
+        <v>-0.246945731857553</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.54307262065294</v>
+        <v>1.57806339854592</v>
       </c>
       <c r="R6" t="n">
-        <v>0.825555632940874</v>
+        <v>0.842278909796593</v>
       </c>
       <c r="S6" t="n">
         <v>1.08834242094509</v>
@@ -1830,13 +1830,13 @@
         <v>0.693876926431495</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.525142335047296</v>
+        <v>-0.524384161812572</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.143010945875753</v>
+        <v>-0.146253867936859</v>
       </c>
       <c r="R7" t="n">
-        <v>-1.84718031638735</v>
+        <v>-1.88709778070237</v>
       </c>
       <c r="S7" t="n">
         <v>-0.300166896262345</v>
@@ -2006,13 +2006,13 @@
         <v>-0.161169421836911</v>
       </c>
       <c r="P8" t="n">
-        <v>-1.75325633317396</v>
+        <v>-1.76004334588915</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.123212775155093</v>
+        <v>0.126006753086738</v>
       </c>
       <c r="R8" t="n">
-        <v>0.0513143311985523</v>
+        <v>0.0516298513558593</v>
       </c>
       <c r="S8" t="n">
         <v>0.904954397917697</v>
@@ -2182,13 +2182,13 @@
         <v>0.705127161654617</v>
       </c>
       <c r="P9" t="n">
-        <v>1.00614094110653</v>
+        <v>1.01630688681041</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.18810765927848</v>
+        <v>1.21504923718112</v>
       </c>
       <c r="R9" t="n">
-        <v>0.403158899090921</v>
+        <v>0.41093072525082</v>
       </c>
       <c r="S9" t="n">
         <v>1.02939627068629</v>
@@ -2358,13 +2358,13 @@
         <v>-0.61382666269609</v>
       </c>
       <c r="P10" t="n">
-        <v>-1.94815487051618</v>
+        <v>-1.95613928486334</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.7444014575604</v>
+        <v>0.76128153547513</v>
       </c>
       <c r="R10" t="n">
-        <v>0.388498708762072</v>
+        <v>0.395959855505197</v>
       </c>
       <c r="S10" t="n">
         <v>-0.215022456999624</v>
@@ -2534,13 +2534,13 @@
         <v>0.633241168403185</v>
       </c>
       <c r="P11" t="n">
-        <v>0.669127104480341</v>
+        <v>0.67722253224459</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.18810765927848</v>
+        <v>1.21504923718112</v>
       </c>
       <c r="R11" t="n">
-        <v>0.0284077838097264</v>
+        <v>0.0282378673783229</v>
       </c>
       <c r="S11" t="n">
         <v>-0.53595149729757</v>
@@ -2710,13 +2710,13 @@
         <v>0.666121465418268</v>
       </c>
       <c r="P12" t="n">
-        <v>0.106426517128875</v>
+        <v>0.111064871223932</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.566918976873169</v>
+        <v>0.579774454792732</v>
       </c>
       <c r="R12" t="n">
-        <v>0.290458685937897</v>
+        <v>0.29584216408134</v>
       </c>
       <c r="S12" t="n">
         <v>0.151753589055171</v>
@@ -2886,13 +2886,13 @@
         <v>0.452912018420414</v>
       </c>
       <c r="P13" t="n">
-        <v>0.0491181769779372</v>
+        <v>0.0534044447979595</v>
       </c>
       <c r="Q13" t="n">
-        <v>-1.91783575274806</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R13" t="n">
-        <v>0.935507060407239</v>
+        <v>0.954560432888768</v>
       </c>
       <c r="S13" t="n">
         <v>0.361339901086483</v>
@@ -3062,13 +3062,13 @@
         <v>-1.63843593801321</v>
       </c>
       <c r="P14" t="n">
-        <v>0.863627386663889</v>
+        <v>0.872917769292771</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.409234666906599</v>
+        <v>-0.418514488960456</v>
       </c>
       <c r="R14" t="n">
-        <v>-1.14623996628927</v>
+        <v>-1.17130307098975</v>
       </c>
       <c r="S14" t="n">
         <v>-1.07956599412878</v>
@@ -3238,13 +3238,13 @@
         <v>0.791309820419164</v>
       </c>
       <c r="P15" t="n">
-        <v>0.703060616917027</v>
+        <v>0.711364522608943</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.833142697904015</v>
+        <v>0.852035075816329</v>
       </c>
       <c r="R15" t="n">
-        <v>1.33408098497281</v>
+        <v>1.3615809540979</v>
       </c>
       <c r="S15" t="n">
         <v>0.538178351862902</v>
@@ -3414,13 +3414,13 @@
         <v>0.489924722878264</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.669871247469737</v>
+        <v>-0.670002247844483</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.143010945875753</v>
+        <v>-0.146253867936859</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.795311660292459</v>
+        <v>-0.81293787645389</v>
       </c>
       <c r="S16" t="n">
         <v>0.0469604330395157</v>
@@ -3590,13 +3590,13 @@
         <v>0.452448342782151</v>
       </c>
       <c r="P17" t="n">
-        <v>0.886743161789851</v>
+        <v>0.896175561220078</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.675458387937445</v>
+        <v>-0.690775109984053</v>
       </c>
       <c r="R17" t="n">
-        <v>0.742175800445547</v>
+        <v>0.75713208811836</v>
       </c>
       <c r="S17" t="n">
         <v>-1.32844973966597</v>
@@ -3766,13 +3766,13 @@
         <v>0.352806888517492</v>
       </c>
       <c r="P18" t="n">
-        <v>0.452145267662214</v>
+        <v>0.458907620232268</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.566918976873169</v>
+        <v>0.579774454792732</v>
       </c>
       <c r="R18" t="n">
-        <v>0.00000366504758191066</v>
+        <v>-0.00076819275382247</v>
       </c>
       <c r="S18" t="n">
         <v>-0.62109593656029</v>
@@ -3942,13 +3942,13 @@
         <v>0.13003108098284</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.433731741782896</v>
+        <v>-0.432411967650354</v>
       </c>
       <c r="Q19" t="n">
-        <v>-1.91783575274806</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R19" t="n">
-        <v>-0.144765714449799</v>
+        <v>-0.148605531491853</v>
       </c>
       <c r="S19" t="n">
         <v>-1.04681813287389</v>
@@ -4118,13 +4118,13 @@
         <v>0.628230217645815</v>
       </c>
       <c r="P20" t="n">
-        <v>0.502451039486188</v>
+        <v>0.509522456526923</v>
       </c>
       <c r="Q20" t="n">
-        <v>1.45433138030932</v>
+        <v>1.48730985820472</v>
       </c>
       <c r="R20" t="n">
-        <v>0.675288682070174</v>
+        <v>0.688827494903954</v>
       </c>
       <c r="S20" t="n">
         <v>0.970450120427482</v>
@@ -4294,13 +4294,13 @@
         <v>0.748570315095748</v>
       </c>
       <c r="P21" t="n">
-        <v>-4.50807621951825</v>
+        <v>-4.53178806847232</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.566918976873169</v>
+        <v>0.579774454792732</v>
       </c>
       <c r="R21" t="n">
-        <v>-0.912593182923249</v>
+        <v>-0.932704834418877</v>
       </c>
       <c r="S21" t="n">
         <v>-0.0250848617212482</v>
@@ -4470,13 +4470,13 @@
         <v>0.300484753336637</v>
       </c>
       <c r="P22" t="n">
-        <v>0.851399289652306</v>
+        <v>0.86061454630273</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.211954015498708</v>
+        <v>0.216760293427937</v>
       </c>
       <c r="R22" t="n">
-        <v>1.23054339077532</v>
+        <v>1.25584918651944</v>
       </c>
       <c r="S22" t="n">
         <v>-0.483554919289742</v>
@@ -4646,13 +4646,13 @@
         <v>0.708474574376465</v>
       </c>
       <c r="P23" t="n">
-        <v>0.579473519268888</v>
+        <v>0.587018140697139</v>
       </c>
       <c r="Q23" t="n">
-        <v>-0.143010945875753</v>
+        <v>-0.146253867936859</v>
       </c>
       <c r="R23" t="n">
-        <v>0.631308111083628</v>
+        <v>0.643914885667083</v>
       </c>
       <c r="S23" t="n">
         <v>0.191051022561042</v>
@@ -4822,13 +4822,13 @@
         <v>0.843013721415667</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.860590991552887</v>
+        <v>-0.861893720232677</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.389436496185939</v>
+        <v>0.398267374110335</v>
       </c>
       <c r="R24" t="n">
-        <v>1.06286746388911</v>
+        <v>1.08461986380387</v>
       </c>
       <c r="S24" t="n">
         <v>1.28482958847445</v>
@@ -4998,13 +4998,13 @@
         <v>0.73139397982921</v>
       </c>
       <c r="P25" t="n">
-        <v>-0.470033395508338</v>
+        <v>-0.46893664849548</v>
       </c>
       <c r="Q25" t="n">
-        <v>-1.20790582999914</v>
+        <v>-1.23529635203125</v>
       </c>
       <c r="R25" t="n">
-        <v>-0.284037522573861</v>
+        <v>-0.290828794075275</v>
       </c>
       <c r="S25" t="n">
         <v>0.610223646623665</v>
@@ -5174,13 +5174,13 @@
         <v>0.725911218773256</v>
       </c>
       <c r="P26" t="n">
-        <v>0.508173623202598</v>
+        <v>0.515280198183329</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.92188393824763</v>
+        <v>0.942788616157528</v>
       </c>
       <c r="R26" t="n">
-        <v>0.0623094739451889</v>
+        <v>0.0628580036650769</v>
       </c>
       <c r="S26" t="n">
         <v>0.073158722043429</v>
@@ -5350,13 +5350,13 @@
         <v>-0.362693429284501</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.0242351267606668</v>
+        <v>-0.020399520945631</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.0344715348114776</v>
+        <v>0.0352532127455389</v>
       </c>
       <c r="R27" t="n">
-        <v>-1.29925570284663</v>
+        <v>-1.32756152395969</v>
       </c>
       <c r="S27" t="n">
         <v>-0.0119857172192911</v>
@@ -5526,13 +5526,13 @@
         <v>0.293342521575321</v>
       </c>
       <c r="P28" t="n">
-        <v>-0.276107239047984</v>
+        <v>-0.273819064436975</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.833142697904015</v>
+        <v>0.852035075816329</v>
       </c>
       <c r="R28" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S28" t="n">
         <v>0.511980062858988</v>
@@ -5702,13 +5702,13 @@
         <v>0.494545209940255</v>
       </c>
       <c r="P29" t="n">
-        <v>0.711710868351421</v>
+        <v>0.720067918747888</v>
       </c>
       <c r="Q29" t="n">
-        <v>-1.82909451240444</v>
+        <v>-1.87057113441964</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.317022950813771</v>
+        <v>-0.324513251002927</v>
       </c>
       <c r="S29" t="n">
         <v>-1.21710701139933</v>
@@ -5878,13 +5878,13 @@
         <v>0.324408789338953</v>
       </c>
       <c r="P30" t="n">
-        <v>-0.266015731732477</v>
+        <v>-0.263665557747366</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.123212775155093</v>
+        <v>0.126006753086738</v>
       </c>
       <c r="R30" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S30" t="n">
         <v>-1.08611556637976</v>
@@ -6054,13 +6054,13 @@
         <v>0.866929622757662</v>
       </c>
       <c r="P31" t="n">
-        <v>0.422957204801574</v>
+        <v>0.429540234147452</v>
       </c>
       <c r="Q31" t="n">
-        <v>1.01062517859125</v>
+        <v>1.03354215649873</v>
       </c>
       <c r="R31" t="n">
-        <v>1.38722417491489</v>
+        <v>1.41585035692579</v>
       </c>
       <c r="S31" t="n">
         <v>0.728115947141277</v>
@@ -6230,13 +6230,13 @@
         <v>0.621661479437087</v>
       </c>
       <c r="P32" t="n">
-        <v>0.792005627093407</v>
+        <v>0.800855985836197</v>
       </c>
       <c r="Q32" t="n">
-        <v>1.27684889962209</v>
+        <v>1.30580277752232</v>
       </c>
       <c r="R32" t="n">
-        <v>1.11784317762229</v>
+        <v>1.14076062534996</v>
       </c>
       <c r="S32" t="n">
         <v>-0.666942942317139</v>
@@ -6406,13 +6406,13 @@
         <v>1.0073419945482</v>
       </c>
       <c r="P33" t="n">
-        <v>0.314297036438038</v>
+        <v>0.320212488362844</v>
       </c>
       <c r="Q33" t="n">
-        <v>0.92188393824763</v>
+        <v>0.942788616157528</v>
       </c>
       <c r="R33" t="n">
-        <v>1.0903553207557</v>
+        <v>1.11269024457691</v>
       </c>
       <c r="S33" t="n">
         <v>2.39170729888981</v>
@@ -6582,13 +6582,13 @@
         <v>0.262386071726014</v>
       </c>
       <c r="P34" t="n">
-        <v>0.562364504813988</v>
+        <v>0.569804013283931</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.211954015498708</v>
+        <v>0.216760293427937</v>
       </c>
       <c r="R34" t="n">
-        <v>0.0558956406763179</v>
+        <v>0.0563082481513669</v>
       </c>
       <c r="S34" t="n">
         <v>-0.693141231321054</v>
@@ -6758,13 +6758,13 @@
         <v>0.304161619801461</v>
       </c>
       <c r="P35" t="n">
-        <v>0.135353829808903</v>
+        <v>0.140169905152587</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.123212775155093</v>
+        <v>0.126006753086738</v>
       </c>
       <c r="R35" t="n">
-        <v>0.238415010270484</v>
+        <v>0.242695576484378</v>
       </c>
       <c r="S35" t="n">
         <v>-0.136427589987883</v>
@@ -6932,13 +6932,13 @@
         <v>0.980111219125638</v>
       </c>
       <c r="P36" t="n">
-        <v>0.143511100433078</v>
+        <v>0.148377291746287</v>
       </c>
       <c r="Q36" t="n">
-        <v>-1.65161203171721</v>
+        <v>-1.68906405373724</v>
       </c>
       <c r="R36" t="n">
-        <v>0.471878541257399</v>
+        <v>0.481106677183429</v>
       </c>
       <c r="S36" t="n">
         <v>1.82189451305468</v>
@@ -7106,13 +7106,13 @@
         <v>-0.25860231582458</v>
       </c>
       <c r="P37" t="n">
-        <v>0.0281624183220916</v>
+        <v>0.0323199398726138</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.675458387937445</v>
+        <v>-0.690775109984053</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.969401420447537</v>
+        <v>-0.990716954683167</v>
       </c>
       <c r="S37" t="n">
         <v>0.885305681164761</v>
@@ -7280,13 +7280,13 @@
         <v>-0.195318725861978</v>
       </c>
       <c r="P38" t="n">
-        <v>-0.467965049023593</v>
+        <v>-0.46685559467342</v>
       </c>
       <c r="Q38" t="n">
-        <v>-0.320493426562984</v>
+        <v>-0.327760948619257</v>
       </c>
       <c r="R38" t="n">
-        <v>-1.75463786493649</v>
+        <v>-1.79259416543312</v>
       </c>
       <c r="S38" t="n">
         <v>1.71055178478805</v>
@@ -7454,13 +7454,13 @@
         <v>0.712920166241567</v>
       </c>
       <c r="P39" t="n">
-        <v>-0.142267702332242</v>
+        <v>-0.13915725536418</v>
       </c>
       <c r="Q39" t="n">
-        <v>1.54307262065294</v>
+        <v>1.57806339854592</v>
       </c>
       <c r="R39" t="n">
-        <v>1.27452396176186</v>
+        <v>1.30076179575631</v>
       </c>
       <c r="S39" t="n">
         <v>1.04249541518825</v>
@@ -7628,13 +7628,13 @@
         <v>0.774654103413132</v>
       </c>
       <c r="P40" t="n">
-        <v>-0.578874527213365</v>
+        <v>-0.578446469409299</v>
       </c>
       <c r="Q40" t="n">
-        <v>-0.143010945875753</v>
+        <v>-0.146253867936859</v>
       </c>
       <c r="R40" t="n">
-        <v>0.411405256150898</v>
+        <v>0.419351839482733</v>
       </c>
       <c r="S40" t="n">
         <v>0.944251831423568</v>
@@ -7802,13 +7802,13 @@
         <v>-2.27560761159001</v>
       </c>
       <c r="P41" t="n">
-        <v>-1.82711789605368</v>
+        <v>-1.83435869337463</v>
       </c>
       <c r="Q41" t="n">
-        <v>0.123212775155093</v>
+        <v>0.126006753086738</v>
       </c>
       <c r="R41" t="n">
-        <v>-0.316106688918218</v>
+        <v>-0.323577571643826</v>
       </c>
       <c r="S41" t="n">
         <v>-0.110229300983968</v>
@@ -7976,13 +7976,13 @@
         <v>0.701918038158217</v>
       </c>
       <c r="P42" t="n">
-        <v>0.978685101450939</v>
+        <v>0.988682366221351</v>
       </c>
       <c r="Q42" t="n">
-        <v>1.18810765927848</v>
+        <v>1.21504923718112</v>
       </c>
       <c r="R42" t="n">
-        <v>0.767831133521032</v>
+        <v>0.783331110173201</v>
       </c>
       <c r="S42" t="n">
         <v>0.859107392160847</v>
@@ -8150,13 +8150,13 @@
         <v>-0.874595401257201</v>
       </c>
       <c r="P43" t="n">
-        <v>-1.81448950677264</v>
+        <v>-1.82165271883236</v>
       </c>
       <c r="Q43" t="n">
-        <v>0.7444014575604</v>
+        <v>0.76128153547513</v>
       </c>
       <c r="R43" t="n">
-        <v>0.065974521527401</v>
+        <v>0.0666007211014827</v>
       </c>
       <c r="S43" t="n">
         <v>0.472682629353117</v>
@@ -8324,13 +8324,13 @@
         <v>0.543589077011985</v>
       </c>
       <c r="P44" t="n">
-        <v>0.702184319760572</v>
+        <v>0.710482841729965</v>
       </c>
       <c r="Q44" t="n">
-        <v>1.18810765927848</v>
+        <v>1.21504923718112</v>
       </c>
       <c r="R44" t="n">
-        <v>0.297788781102321</v>
+        <v>0.303327598954152</v>
       </c>
       <c r="S44" t="n">
         <v>-0.935475404607257</v>
@@ -8498,13 +8498,13 @@
         <v>0.635124342267359</v>
       </c>
       <c r="P45" t="n">
-        <v>0.0575433276704748</v>
+        <v>0.0618813572395922</v>
       </c>
       <c r="Q45" t="n">
-        <v>0.566918976873169</v>
+        <v>0.579774454792732</v>
       </c>
       <c r="R45" t="n">
-        <v>0.420567875106429</v>
+        <v>0.428708633073748</v>
       </c>
       <c r="S45" t="n">
         <v>0.872206536662804</v>
@@ -8672,13 +8672,13 @@
         <v>0.282649510584146</v>
       </c>
       <c r="P46" t="n">
-        <v>-0.0118973652851027</v>
+        <v>-0.00798595974407987</v>
       </c>
       <c r="Q46" t="n">
-        <v>-1.91783575274806</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R46" t="n">
-        <v>1.10318298729345</v>
+        <v>1.12578975560434</v>
       </c>
       <c r="S46" t="n">
         <v>0.701917658137364</v>
@@ -8846,13 +8846,13 @@
         <v>-1.81477096977866</v>
       </c>
       <c r="P47" t="n">
-        <v>0.791741481728153</v>
+        <v>0.800590217636334</v>
       </c>
       <c r="Q47" t="n">
-        <v>-0.409234666906599</v>
+        <v>-0.418514488960456</v>
       </c>
       <c r="R47" t="n">
-        <v>-1.70699224636774</v>
+        <v>-1.74393883875984</v>
       </c>
       <c r="S47" t="n">
         <v>-0.942024976858236</v>
@@ -9020,13 +9020,13 @@
         <v>0.81505489389443</v>
       </c>
       <c r="P48" t="n">
-        <v>0.768052259915925</v>
+        <v>0.776755455928092</v>
       </c>
       <c r="Q48" t="n">
-        <v>0.833142697904015</v>
+        <v>0.852035075816329</v>
       </c>
       <c r="R48" t="n">
-        <v>1.26902639038855</v>
+        <v>1.2951477196017</v>
       </c>
       <c r="S48" t="n">
         <v>0.898404825666718</v>
@@ -9194,13 +9194,13 @@
         <v>0.461807269480779</v>
       </c>
       <c r="P49" t="n">
-        <v>-0.163308001085708</v>
+        <v>-0.160326819777657</v>
       </c>
       <c r="Q49" t="n">
-        <v>-0.143010945875753</v>
+        <v>-0.146253867936859</v>
       </c>
       <c r="R49" t="n">
-        <v>-0.0870412150299569</v>
+        <v>-0.0896577318684609</v>
       </c>
       <c r="S49" t="n">
         <v>0.0797082942944081</v>
@@ -9368,13 +9368,13 @@
         <v>0.442324758013405</v>
       </c>
       <c r="P50" t="n">
-        <v>0.860282450753235</v>
+        <v>0.869552283039498</v>
       </c>
       <c r="Q50" t="n">
-        <v>-0.675458387937445</v>
+        <v>-0.690775109984053</v>
       </c>
       <c r="R50" t="n">
-        <v>0.59557389715706</v>
+        <v>0.607423390662127</v>
       </c>
       <c r="S50" t="n">
         <v>-1.32844973966597</v>
@@ -9542,13 +9542,13 @@
         <v>-0.121622770689255</v>
       </c>
       <c r="P51" t="n">
-        <v>0.215686614618895</v>
+        <v>0.220996231930336</v>
       </c>
       <c r="Q51" t="n">
-        <v>0.566918976873169</v>
+        <v>0.579774454792732</v>
       </c>
       <c r="R51" t="n">
-        <v>0.566253516499363</v>
+        <v>0.57748165117088</v>
       </c>
       <c r="S51" t="n">
         <v>-0.0905805842310331</v>
@@ -9718,13 +9718,13 @@
         <v>-0.253074814136863</v>
       </c>
       <c r="P52" t="n">
-        <v>-0.55850817261161</v>
+        <v>-0.557954989670279</v>
       </c>
       <c r="Q52" t="n">
-        <v>-1.91783575274806</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R52" t="n">
-        <v>0.683535039130152</v>
+        <v>0.697248609135867</v>
       </c>
       <c r="S52" t="n">
         <v>-0.915826687854322</v>
@@ -9894,13 +9894,13 @@
         <v>0.619212946680644</v>
       </c>
       <c r="P53" t="n">
-        <v>0.545909402921401</v>
+        <v>0.55324781588735</v>
       </c>
       <c r="Q53" t="n">
-        <v>1.45433138030932</v>
+        <v>1.48730985820472</v>
       </c>
       <c r="R53" t="n">
-        <v>1.22138077181979</v>
+        <v>1.24649239292842</v>
       </c>
       <c r="S53" t="n">
         <v>1.42892017799598</v>
@@ -10070,13 +10070,13 @@
         <v>0.636458426559906</v>
       </c>
       <c r="P54" t="n">
-        <v>-3.73795870952598</v>
+        <v>-3.75693917375107</v>
       </c>
       <c r="Q54" t="n">
-        <v>0.566918976873169</v>
+        <v>0.579774454792732</v>
       </c>
       <c r="R54" t="n">
-        <v>-1.25710765565119</v>
+        <v>-1.28452027344102</v>
       </c>
       <c r="S54" t="n">
         <v>-0.208472884748646</v>
@@ -10246,13 +10246,13 @@
         <v>0.318055619628716</v>
       </c>
       <c r="P55" t="n">
-        <v>0.773494061862328</v>
+        <v>0.782230690770505</v>
       </c>
       <c r="Q55" t="n">
-        <v>0.211954015498708</v>
+        <v>0.216760293427937</v>
       </c>
       <c r="R55" t="n">
-        <v>1.30476060431511</v>
+        <v>1.33163921460666</v>
       </c>
       <c r="S55" t="n">
         <v>-0.326365185266258</v>
@@ -10422,13 +10422,13 @@
         <v>0.647070090947876</v>
       </c>
       <c r="P56" t="n">
-        <v>0.687985657581973</v>
+        <v>0.696196946976425</v>
       </c>
       <c r="Q56" t="n">
-        <v>-0.143010945875753</v>
+        <v>-0.146253867936859</v>
       </c>
       <c r="R56" t="n">
-        <v>1.28093779503074</v>
+        <v>1.30731155127002</v>
       </c>
       <c r="S56" t="n">
         <v>0.125555300051257</v>
@@ -10598,13 +10598,13 @@
         <v>0.854536467759523</v>
       </c>
       <c r="P57" t="n">
-        <v>-1.24863037914744</v>
+        <v>-1.25231711235756</v>
       </c>
       <c r="Q57" t="n">
-        <v>0.389436496185939</v>
+        <v>0.398267374110335</v>
       </c>
       <c r="R57" t="n">
-        <v>0.841132085165275</v>
+        <v>0.858185458901318</v>
       </c>
       <c r="S57" t="n">
         <v>0.538178351862902</v>
@@ -10774,13 +10774,13 @@
         <v>0.616536643435231</v>
       </c>
       <c r="P58" t="n">
-        <v>-0.292584070122288</v>
+        <v>-0.290397124513237</v>
       </c>
       <c r="Q58" t="n">
-        <v>-1.20790582999914</v>
+        <v>-1.23529635203125</v>
       </c>
       <c r="R58" t="n">
-        <v>0.295039995415662</v>
+        <v>0.300520560876848</v>
       </c>
       <c r="S58" t="n">
         <v>0.754314236145192</v>
@@ -10950,13 +10950,13 @@
         <v>0.632671742180757</v>
       </c>
       <c r="P59" t="n">
-        <v>0.602240269413511</v>
+        <v>0.609924763332083</v>
       </c>
       <c r="Q59" t="n">
-        <v>0.92188393824763</v>
+        <v>0.942788616157528</v>
       </c>
       <c r="R59" t="n">
-        <v>-0.1603421666742</v>
+        <v>-0.164512080596578</v>
       </c>
       <c r="S59" t="n">
         <v>-0.116778873234946</v>
@@ -11126,13 +11126,13 @@
         <v>-0.619813772691909</v>
       </c>
       <c r="P60" t="n">
-        <v>0.162075970063058</v>
+        <v>0.167056218698069</v>
       </c>
       <c r="Q60" t="n">
-        <v>0.0344715348114776</v>
+        <v>0.0352532127455389</v>
       </c>
       <c r="R60" t="n">
-        <v>-0.112696548105442</v>
+        <v>-0.115856753923302</v>
       </c>
       <c r="S60" t="n">
         <v>-0.123328445485926</v>
@@ -11302,13 +11302,13 @@
         <v>0.310998801800763</v>
       </c>
       <c r="P61" t="n">
-        <v>-0.395506376438518</v>
+        <v>-0.393951756444788</v>
       </c>
       <c r="Q61" t="n">
-        <v>0.833142697904015</v>
+        <v>0.852035075816329</v>
       </c>
       <c r="R61" t="n">
-        <v>-1.67858812760559</v>
+        <v>-1.7149327786277</v>
       </c>
       <c r="S61" t="n">
         <v>1.24553215496858</v>
@@ -11478,13 +11478,13 @@
         <v>0.404783300634729</v>
       </c>
       <c r="P62" t="n">
-        <v>0.767454028381762</v>
+        <v>0.776153549028146</v>
       </c>
       <c r="Q62" t="n">
-        <v>-1.82909451240444</v>
+        <v>-1.87057113441964</v>
       </c>
       <c r="R62" t="n">
-        <v>-0.0677997152233431</v>
+        <v>-0.0700084653273303</v>
       </c>
       <c r="S62" t="n">
         <v>-1.15161128888955</v>
@@ -11654,13 +11654,13 @@
         <v>0.187551264108434</v>
       </c>
       <c r="P63" t="n">
-        <v>-0.240766422576618</v>
+        <v>-0.238261123958958</v>
       </c>
       <c r="Q63" t="n">
-        <v>0.123212775155093</v>
+        <v>0.126006753086738</v>
       </c>
       <c r="R63" t="n">
-        <v>-1.17464408505142</v>
+        <v>-1.20030913112189</v>
       </c>
       <c r="S63" t="n">
         <v>-1.04026856062291</v>
@@ -11830,13 +11830,13 @@
         <v>0.821094879182332</v>
       </c>
       <c r="P64" t="n">
-        <v>0.474905566956014</v>
+        <v>0.481807752384182</v>
       </c>
       <c r="Q64" t="n">
-        <v>1.01062517859125</v>
+        <v>1.03354215649873</v>
       </c>
       <c r="R64" t="n">
-        <v>1.53932364957669</v>
+        <v>1.57117313053663</v>
       </c>
       <c r="S64" t="n">
         <v>0.996648409431395</v>
@@ -12006,13 +12006,13 @@
         <v>0.485800450095818</v>
       </c>
       <c r="P65" t="n">
-        <v>0.877791417959126</v>
+        <v>0.88716882040057</v>
       </c>
       <c r="Q65" t="n">
-        <v>1.27684889962209</v>
+        <v>1.30580277752232</v>
       </c>
       <c r="R65" t="n">
-        <v>0.98406894087155</v>
+        <v>1.00415143892115</v>
       </c>
       <c r="S65" t="n">
         <v>-0.968223265862149</v>
@@ -12182,13 +12182,13 @@
         <v>0.997413641627143</v>
       </c>
       <c r="P66" t="n">
-        <v>0.232118968774371</v>
+        <v>0.237529541834127</v>
       </c>
       <c r="Q66" t="n">
-        <v>0.92188393824763</v>
+        <v>0.942788616157528</v>
       </c>
       <c r="R66" t="n">
-        <v>1.12150822520451</v>
+        <v>1.14450334278636</v>
       </c>
       <c r="S66" t="n">
         <v>2.54234746066232</v>
@@ -12358,13 +12358,13 @@
         <v>-0.351105605658082</v>
       </c>
       <c r="P67" t="n">
-        <v>0.660250733748699</v>
+        <v>0.668291627595223</v>
       </c>
       <c r="Q67" t="n">
-        <v>0.211954015498708</v>
+        <v>0.216760293427937</v>
       </c>
       <c r="R67" t="n">
-        <v>0.400410113404262</v>
+        <v>0.408123687173516</v>
       </c>
       <c r="S67" t="n">
         <v>-0.797934387336709</v>
@@ -12534,13 +12534,13 @@
         <v>0.0662838153819746</v>
       </c>
       <c r="P68" t="n">
-        <v>0.12482739934058</v>
+        <v>0.129578803265003</v>
       </c>
       <c r="Q68" t="n">
-        <v>0.389436496185939</v>
+        <v>0.398267374110335</v>
       </c>
       <c r="R68" t="n">
-        <v>0.140283361256753</v>
+        <v>0.142484317124611</v>
       </c>
       <c r="S68" t="n">
         <v>-0.260869462756473</v>
@@ -12708,13 +12708,13 @@
         <v>0.869821494501567</v>
       </c>
       <c r="P69" t="n">
-        <v>0.150554750494226</v>
+        <v>0.155464216006376</v>
       </c>
       <c r="Q69" t="n">
-        <v>-0.608902457679733</v>
+        <v>-0.622709954728153</v>
       </c>
       <c r="R69" t="n">
-        <v>-0.02473540613235</v>
+        <v>-0.0260315354495616</v>
       </c>
       <c r="S69" t="n">
         <v>1.74329964604294</v>
@@ -12882,13 +12882,13 @@
         <v>-1.42945244705181</v>
       </c>
       <c r="P70" t="n">
-        <v>-0.733798839601401</v>
+        <v>-0.734322593068041</v>
       </c>
       <c r="Q70" t="n">
-        <v>-0.426095502571886</v>
+        <v>-0.435757661625284</v>
       </c>
       <c r="R70" t="n">
-        <v>-1.17006277557365</v>
+        <v>-1.19563073432639</v>
       </c>
       <c r="S70" t="n">
         <v>0.806710814153019</v>
@@ -13056,13 +13056,13 @@
         <v>-2.93154187919583</v>
       </c>
       <c r="P71" t="n">
-        <v>-0.314298992064392</v>
+        <v>-0.31224545680991</v>
       </c>
       <c r="Q71" t="n">
-        <v>-1.04728418497719</v>
+        <v>-1.07103244401368</v>
       </c>
       <c r="R71" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S71" t="n">
         <v>0.616773218874644</v>
@@ -13230,13 +13230,13 @@
         <v>0.784366887835697</v>
       </c>
       <c r="P72" t="n">
-        <v>0.00485583381917229</v>
+        <v>0.00887016628936483</v>
       </c>
       <c r="Q72" t="n">
-        <v>1.51822507335672</v>
+        <v>1.55265240725038</v>
       </c>
       <c r="R72" t="n">
-        <v>1.1801489865199</v>
+        <v>1.20438682176886</v>
       </c>
       <c r="S72" t="n">
         <v>0.832909103156933</v>
@@ -13404,13 +13404,13 @@
         <v>0.755924048025396</v>
       </c>
       <c r="P73" t="n">
-        <v>-0.534603356574528</v>
+        <v>-0.533903309187084</v>
       </c>
       <c r="Q73" t="n">
-        <v>0.208404365884963</v>
+        <v>0.213130151814289</v>
       </c>
       <c r="R73" t="n">
-        <v>0.45996713661521</v>
+        <v>0.468942845515111</v>
       </c>
       <c r="S73" t="n">
         <v>0.911503970168675</v>
@@ -13578,13 +13578,13 @@
         <v>-3.59875078600573</v>
       </c>
       <c r="P74" t="n">
-        <v>-1.27998389077363</v>
+        <v>-1.28386325111426</v>
       </c>
       <c r="Q74" t="n">
-        <v>0.23236450077774</v>
+        <v>0.237633607706412</v>
       </c>
       <c r="R74" t="n">
-        <v>0.307867661953405</v>
+        <v>0.313620071904268</v>
       </c>
       <c r="S74" t="n">
         <v>-0.27396860725843</v>
@@ -13752,13 +13752,13 @@
         <v>0.679458241013575</v>
       </c>
       <c r="P75" t="n">
-        <v>0.934966327353578</v>
+        <v>0.944694996309131</v>
       </c>
       <c r="Q75" t="n">
-        <v>1.29282232288394</v>
+        <v>1.32213841478374</v>
       </c>
       <c r="R75" t="n">
-        <v>0.784323847640987</v>
+        <v>0.800173338637027</v>
       </c>
       <c r="S75" t="n">
         <v>0.603674074372686</v>
@@ -13926,13 +13926,13 @@
         <v>-1.36012073714098</v>
       </c>
       <c r="P76" t="n">
-        <v>-1.50326651125293</v>
+        <v>-1.5085176570251</v>
       </c>
       <c r="Q76" t="n">
-        <v>0.895261566144546</v>
+        <v>0.915562554055168</v>
       </c>
       <c r="R76" t="n">
-        <v>-0.522265615417652</v>
+        <v>-0.534105427441654</v>
       </c>
       <c r="S76" t="n">
         <v>-0.254319890505495</v>
@@ -14100,13 +14100,13 @@
         <v>0.524850886963929</v>
       </c>
       <c r="P77" t="n">
-        <v>0.669234392315072</v>
+        <v>0.677330479225511</v>
       </c>
       <c r="Q77" t="n">
-        <v>-0.89109960197243</v>
+        <v>-0.911306213013166</v>
       </c>
       <c r="R77" t="n">
-        <v>0.463632184197422</v>
+        <v>0.472685562951516</v>
       </c>
       <c r="S77" t="n">
         <v>-1.00752069936802</v>
@@ -14274,13 +14274,13 @@
         <v>0.671071406223236</v>
       </c>
       <c r="P78" t="n">
-        <v>0.0701302956988629</v>
+        <v>0.074545656048726</v>
       </c>
       <c r="Q78" t="n">
-        <v>0.290933719404525</v>
+        <v>0.297530944331604</v>
       </c>
       <c r="R78" t="n">
-        <v>-0.166755999943072</v>
+        <v>-0.171061836110288</v>
       </c>
       <c r="S78" t="n">
         <v>0.84600824765889</v>
@@ -14448,13 +14448,13 @@
         <v>-0.415845299818037</v>
       </c>
       <c r="P79" t="n">
-        <v>-0.00743066036827705</v>
+        <v>-0.00349181265231594</v>
       </c>
       <c r="Q79" t="n">
-        <v>-0.549445826649511</v>
+        <v>-0.56190508269955</v>
       </c>
       <c r="R79" t="n">
-        <v>0.872284989614079</v>
+        <v>0.889998557110767</v>
       </c>
       <c r="S79" t="n">
         <v>-0.31981561301528</v>
@@ -14622,13 +14622,13 @@
         <v>-1.84942462274359</v>
       </c>
       <c r="P80" t="n">
-        <v>0.738848579205926</v>
+        <v>0.747372356042255</v>
       </c>
       <c r="Q80" t="n">
-        <v>0.296258193825143</v>
+        <v>0.302976156752076</v>
       </c>
       <c r="R80" t="n">
-        <v>-1.04086984830067</v>
+        <v>-1.06369994469308</v>
       </c>
       <c r="S80" t="n">
         <v>-0.83723182084258</v>
@@ -14796,13 +14796,13 @@
         <v>0.689150688785339</v>
       </c>
       <c r="P81" t="n">
-        <v>0.756752066867376</v>
+        <v>0.765385837681271</v>
       </c>
       <c r="Q81" t="n">
-        <v>0.653885392409912</v>
+        <v>0.668712924327107</v>
       </c>
       <c r="R81" t="n">
-        <v>1.14074972501112</v>
+        <v>1.1641526093275</v>
       </c>
       <c r="S81" t="n">
         <v>0.996648409431395</v>
@@ -14970,13 +14970,13 @@
         <v>0.326568541654021</v>
       </c>
       <c r="P82" t="n">
-        <v>0.112229906239797</v>
+        <v>0.116903914720399</v>
       </c>
       <c r="Q82" t="n">
-        <v>0.463091725671139</v>
+        <v>0.473592812593529</v>
       </c>
       <c r="R82" t="n">
-        <v>0.208911377233676</v>
+        <v>0.212566701121311</v>
       </c>
       <c r="S82" t="n">
         <v>0.302393750827676</v>
@@ -15144,13 +15144,13 @@
         <v>0.376145228976738</v>
       </c>
       <c r="P83" t="n">
-        <v>0.857077396449888</v>
+        <v>0.866327537786666</v>
       </c>
       <c r="Q83" t="n">
-        <v>0.336191751979769</v>
+        <v>0.343815249905615</v>
       </c>
       <c r="R83" t="n">
-        <v>0.70094401514566</v>
+        <v>0.715026516958794</v>
       </c>
       <c r="S83" t="n">
         <v>-1.33499931191694</v>
@@ -15318,13 +15318,13 @@
         <v>-0.373764701980574</v>
       </c>
       <c r="P84" t="n">
-        <v>0.105016157428016</v>
+        <v>0.109645846670939</v>
       </c>
       <c r="Q84" t="n">
-        <v>0.763924530435995</v>
+        <v>0.781247314350194</v>
       </c>
       <c r="R84" t="n">
-        <v>0.635889420561394</v>
+        <v>0.648593282462591</v>
       </c>
       <c r="S84" t="n">
         <v>-0.477005347038763</v>
@@ -15494,13 +15494,13 @@
         <v>-0.226690043387625</v>
       </c>
       <c r="P85" t="n">
-        <v>-0.451632852815097</v>
+        <v>-0.450423058058779</v>
       </c>
       <c r="Q85" t="n">
-        <v>-1.2389652641194</v>
+        <v>-1.26706009115067</v>
       </c>
       <c r="R85" t="n">
-        <v>0.845713394643041</v>
+        <v>0.862863855696825</v>
       </c>
       <c r="S85" t="n">
         <v>-1.04681813287389</v>
@@ -15670,13 +15670,13 @@
         <v>-0.44453217943795</v>
       </c>
       <c r="P86" t="n">
-        <v>0.684864464339318</v>
+        <v>0.693056578002985</v>
       </c>
       <c r="Q86" t="n">
-        <v>1.63181386099655</v>
+        <v>1.66881693888712</v>
       </c>
       <c r="R86" t="n">
-        <v>0.973073798124913</v>
+        <v>0.992923286611928</v>
       </c>
       <c r="S86" t="n">
         <v>0.767413380647148</v>
@@ -15846,13 +15846,13 @@
         <v>0.61572317740319</v>
       </c>
       <c r="P87" t="n">
-        <v>-3.77122404962485</v>
+        <v>-3.79040888671526</v>
       </c>
       <c r="Q87" t="n">
-        <v>0.452442776829905</v>
+        <v>0.462702387752586</v>
       </c>
       <c r="R87" t="n">
-        <v>-1.64010512799236</v>
+        <v>-1.67563424554544</v>
       </c>
       <c r="S87" t="n">
         <v>-0.0512831507251616</v>
@@ -16022,13 +16022,13 @@
         <v>0.10140521131533</v>
       </c>
       <c r="P88" t="n">
-        <v>0.758423855785775</v>
+        <v>0.767067897599167</v>
       </c>
       <c r="Q88" t="n">
-        <v>0.818944099449037</v>
+        <v>0.837514509361737</v>
       </c>
       <c r="R88" t="n">
-        <v>1.21954824802868</v>
+        <v>1.24462103421022</v>
       </c>
       <c r="S88" t="n">
         <v>-0.247770318254516</v>
@@ -16198,13 +16198,13 @@
         <v>0.431326697260216</v>
       </c>
       <c r="P89" t="n">
-        <v>0.670680061936221</v>
+        <v>0.678785030632985</v>
       </c>
       <c r="Q89" t="n">
-        <v>0.5873294621522</v>
+        <v>0.600647769071208</v>
       </c>
       <c r="R89" t="n">
-        <v>1.26536134280633</v>
+        <v>1.29140500216529</v>
       </c>
       <c r="S89" t="n">
         <v>0.145204016804193</v>
@@ -16374,13 +16374,13 @@
         <v>0.706928988915587</v>
       </c>
       <c r="P90" t="n">
-        <v>-1.07140615450325</v>
+        <v>-1.07400407207263</v>
       </c>
       <c r="Q90" t="n">
-        <v>-0.423433265361577</v>
+        <v>-0.433035055415047</v>
       </c>
       <c r="R90" t="n">
-        <v>0.776077490581009</v>
+        <v>0.791752224405114</v>
       </c>
       <c r="S90" t="n">
         <v>1.04249541518825</v>
@@ -16550,13 +16550,13 @@
         <v>-0.0346266458926679</v>
       </c>
       <c r="P91" t="n">
-        <v>-0.0714427925975605</v>
+        <v>-0.0678972173640047</v>
       </c>
       <c r="Q91" t="n">
-        <v>0.800308438976877</v>
+        <v>0.818456265890085</v>
       </c>
       <c r="R91" t="n">
-        <v>-0.120942905165419</v>
+        <v>-0.124277868155215</v>
       </c>
       <c r="S91" t="n">
         <v>0.119005727800279</v>
@@ -16726,13 +16726,13 @@
         <v>0.382648889902903</v>
       </c>
       <c r="P92" t="n">
-        <v>0.589363013098114</v>
+        <v>0.596968392786596</v>
       </c>
       <c r="Q92" t="n">
-        <v>0.474628086915809</v>
+        <v>0.485390772837886</v>
       </c>
       <c r="R92" t="n">
-        <v>-0.0732972865966612</v>
+        <v>-0.0756225414819389</v>
       </c>
       <c r="S92" t="n">
         <v>-0.221572029250603</v>
@@ -16902,13 +16902,13 @@
         <v>-1.04937264557129</v>
       </c>
       <c r="P93" t="n">
-        <v>0.190880037540532</v>
+        <v>0.196037250240412</v>
       </c>
       <c r="Q93" t="n">
-        <v>0.978678332067544</v>
+        <v>1.0008708819759</v>
       </c>
       <c r="R93" t="n">
-        <v>-0.356422212322552</v>
+        <v>-0.36474746344429</v>
       </c>
       <c r="S93" t="n">
         <v>-0.27396860725843</v>
@@ -17078,13 +17078,13 @@
         <v>0.0731087953907957</v>
       </c>
       <c r="P94" t="n">
-        <v>-0.694231357767496</v>
+        <v>-0.694512019787852</v>
       </c>
       <c r="Q94" t="n">
-        <v>0.620163721079338</v>
+        <v>0.634226578997451</v>
       </c>
       <c r="R94" t="n">
-        <v>-0.553418519866456</v>
+        <v>-0.565918525651104</v>
       </c>
       <c r="S94" t="n">
         <v>0.84600824765889</v>
@@ -17254,13 +17254,13 @@
         <v>0.3821892815948</v>
       </c>
       <c r="P95" t="n">
-        <v>0.801679187179314</v>
+        <v>0.810588977546332</v>
       </c>
       <c r="Q95" t="n">
-        <v>-1.43952046729597</v>
+        <v>-1.47216309232178</v>
       </c>
       <c r="R95" t="n">
-        <v>-0.545172162806478</v>
+        <v>-0.557497411419191</v>
       </c>
       <c r="S95" t="n">
         <v>-1.21055743914835</v>
@@ -17430,13 +17430,13 @@
         <v>-0.257707503189335</v>
       </c>
       <c r="P96" t="n">
-        <v>-0.253834488268973</v>
+        <v>-0.251409476160386</v>
       </c>
       <c r="Q96" t="n">
-        <v>0.476402911722681</v>
+        <v>0.487205843644709</v>
       </c>
       <c r="R96" t="n">
-        <v>-1.01796330091185</v>
+        <v>-1.04030796071554</v>
       </c>
       <c r="S96" t="n">
         <v>-0.974772838113128</v>
@@ -17606,13 +17606,13 @@
         <v>0.733228345731462</v>
       </c>
       <c r="P97" t="n">
-        <v>0.266251439031159</v>
+        <v>0.271871712359302</v>
       </c>
       <c r="Q97" t="n">
-        <v>1.07185663442834</v>
+        <v>1.09616209933415</v>
       </c>
       <c r="R97" t="n">
-        <v>1.46052512655913</v>
+        <v>1.4907047056539</v>
       </c>
       <c r="S97" t="n">
         <v>0.734665519392256</v>
@@ -17782,13 +17782,13 @@
         <v>0.219426930573947</v>
       </c>
       <c r="P98" t="n">
-        <v>0.781902236631649</v>
+        <v>0.790690522993638</v>
       </c>
       <c r="Q98" t="n">
-        <v>1.30790833374236</v>
+        <v>1.33756651664174</v>
       </c>
       <c r="R98" t="n">
-        <v>0.352764494835504</v>
+        <v>0.35946836050024</v>
       </c>
       <c r="S98" t="n">
         <v>-1.28260273390912</v>
@@ -17958,13 +17958,13 @@
         <v>1.02123599437545</v>
       </c>
       <c r="P99" t="n">
-        <v>0.152595256464895</v>
+        <v>0.157517258270096</v>
       </c>
       <c r="Q99" t="n">
-        <v>1.26176288876368</v>
+        <v>1.29037467566432</v>
       </c>
       <c r="R99" t="n">
-        <v>1.22687834319311</v>
+        <v>1.25210646908303</v>
       </c>
       <c r="S99" t="n">
         <v>2.82397906745439</v>
@@ -18134,13 +18134,13 @@
         <v>-0.65123796550964</v>
       </c>
       <c r="P100" t="n">
-        <v>0.614045665936994</v>
+        <v>0.621802688881469</v>
       </c>
       <c r="Q100" t="n">
-        <v>0.471078437302065</v>
+        <v>0.481760631224238</v>
       </c>
       <c r="R100" t="n">
-        <v>-1.17830913263363</v>
+        <v>-1.2040518485583</v>
       </c>
       <c r="S100" t="n">
         <v>-0.922376260105301</v>
@@ -18310,13 +18310,13 @@
         <v>-0.0723999410904753</v>
       </c>
       <c r="P101" t="n">
-        <v>0.141951692126376</v>
+        <v>0.146808302874861</v>
       </c>
       <c r="Q101" t="n">
-        <v>-0.0542697055321378</v>
+        <v>-0.0555003275956601</v>
       </c>
       <c r="R101" t="n">
-        <v>0.0301486814112772</v>
+        <v>0.0300156581606157</v>
       </c>
       <c r="S101" t="n">
         <v>-0.594897647556377</v>
@@ -18486,13 +18486,13 @@
         <v>0.879208892511316</v>
       </c>
       <c r="P102" t="n">
-        <v>0.21375441503835</v>
+        <v>0.219052161460647</v>
       </c>
       <c r="Q102" t="n">
-        <v>-1.38183866107262</v>
+        <v>-1.4131732911</v>
       </c>
       <c r="R102" t="n">
-        <v>-0.355505950426999</v>
+        <v>-0.363811784085189</v>
       </c>
       <c r="S102" t="n">
         <v>0.616773218874644</v>
@@ -18662,13 +18662,13 @@
         <v>-2.2454483584521</v>
       </c>
       <c r="P103" t="n">
-        <v>-0.440133701946446</v>
+        <v>-0.438853259651136</v>
       </c>
       <c r="Q103" t="n">
-        <v>-1.61611553557977</v>
+        <v>-1.65276263760076</v>
       </c>
       <c r="R103" t="n">
-        <v>-1.7097410320544</v>
+        <v>-1.74674587683715</v>
       </c>
       <c r="S103" t="n">
         <v>-0.156076306740818</v>
@@ -18838,13 +18838,13 @@
         <v>0.0634814249015946</v>
       </c>
       <c r="P104" t="n">
-        <v>-0.23352551228769</v>
+        <v>-0.230975727559897</v>
       </c>
       <c r="Q104" t="n">
-        <v>-1.25138903776751</v>
+        <v>-1.27976558679843</v>
       </c>
       <c r="R104" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S104" t="n">
         <v>0.32859203983159</v>
@@ -19014,13 +19014,13 @@
         <v>0.785981617909298</v>
       </c>
       <c r="P105" t="n">
-        <v>-0.0629022056271481</v>
+        <v>-0.0593041594365709</v>
       </c>
       <c r="Q105" t="n">
-        <v>1.52798660979452</v>
+        <v>1.56263529668792</v>
       </c>
       <c r="R105" t="n">
-        <v>1.22138077181979</v>
+        <v>1.24649239292842</v>
       </c>
       <c r="S105" t="n">
         <v>0.819809958654977</v>
@@ -19190,13 +19190,13 @@
         <v>0.801291048632303</v>
       </c>
       <c r="P106" t="n">
-        <v>-0.304710651113034</v>
+        <v>-0.302598207796646</v>
       </c>
       <c r="Q106" t="n">
-        <v>0.529647655928851</v>
+        <v>0.541657967849429</v>
       </c>
       <c r="R106" t="n">
-        <v>-0.158509642883094</v>
+        <v>-0.162640721878375</v>
       </c>
       <c r="S106" t="n">
         <v>0.41373647909431</v>
@@ -19366,13 +19366,13 @@
         <v>-2.87784905375098</v>
       </c>
       <c r="P107" t="n">
-        <v>-1.07037062318702</v>
+        <v>-1.07296217874412</v>
       </c>
       <c r="Q107" t="n">
-        <v>-0.272573156777431</v>
+        <v>-0.278754036835009</v>
       </c>
       <c r="R107" t="n">
-        <v>-0.70826678021492</v>
+        <v>-0.724048337339251</v>
       </c>
       <c r="S107" t="n">
         <v>-0.666942942317139</v>
@@ -19542,13 +19542,13 @@
         <v>0.634217327641634</v>
       </c>
       <c r="P108" t="n">
-        <v>0.929775090033856</v>
+        <v>0.93947186549178</v>
       </c>
       <c r="Q108" t="n">
-        <v>1.21650485618843</v>
+        <v>1.24409037009031</v>
       </c>
       <c r="R108" t="n">
-        <v>0.795318990387623</v>
+        <v>0.811401490946245</v>
       </c>
       <c r="S108" t="n">
         <v>-0.0709318674780978</v>
@@ -19718,13 +19718,13 @@
         <v>-2.1309204758011</v>
       </c>
       <c r="P109" t="n">
-        <v>-1.23073605848453</v>
+        <v>-1.23431285403653</v>
       </c>
       <c r="Q109" t="n">
-        <v>0.261649110091133</v>
+        <v>0.267582276019008</v>
       </c>
       <c r="R109" t="n">
-        <v>-0.167672261838625</v>
+        <v>-0.171997515469389</v>
       </c>
       <c r="S109" t="n">
         <v>-0.693141231321054</v>
@@ -19894,13 +19894,13 @@
         <v>0.457316936983914</v>
       </c>
       <c r="P110" t="n">
-        <v>0.6938128129854</v>
+        <v>0.702059902778792</v>
       </c>
       <c r="Q110" t="n">
-        <v>-1.91783575274806</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R110" t="n">
-        <v>0.137442949380539</v>
+        <v>0.139583711111397</v>
       </c>
       <c r="S110" t="n">
         <v>-1.17780957789346</v>
@@ -20070,13 +20070,13 @@
         <v>0.723926361655077</v>
       </c>
       <c r="P111" t="n">
-        <v>-0.00492263747221518</v>
+        <v>-0.00096838117110132</v>
       </c>
       <c r="Q111" t="n">
-        <v>-0.0560445303390103</v>
+        <v>-0.0573153984024842</v>
       </c>
       <c r="R111" t="n">
-        <v>-0.0732972865966612</v>
+        <v>-0.0756225414819389</v>
       </c>
       <c r="S111" t="n">
         <v>0.649521080129536</v>
@@ -20246,13 +20246,13 @@
         <v>-1.22029812822368</v>
       </c>
       <c r="P112" t="n">
-        <v>0.0608760409164128</v>
+        <v>0.065234545735545</v>
       </c>
       <c r="Q112" t="n">
-        <v>-0.965642243861067</v>
+        <v>-0.987539186899773</v>
       </c>
       <c r="R112" t="n">
-        <v>0.704609062727872</v>
+        <v>0.7187692343952</v>
       </c>
       <c r="S112" t="n">
         <v>-0.830682248591602</v>
@@ -20422,13 +20422,13 @@
         <v>-1.53420653532784</v>
       </c>
       <c r="P113" t="n">
-        <v>0.677479937739975</v>
+        <v>0.685626682955412</v>
       </c>
       <c r="Q113" t="n">
-        <v>0.172907869747517</v>
+        <v>0.176828735677809</v>
       </c>
       <c r="R113" t="n">
-        <v>-1.1691465136781</v>
+        <v>-1.19469505496729</v>
       </c>
       <c r="S113" t="n">
         <v>-0.909277115603344</v>
@@ -20598,13 +20598,13 @@
         <v>0.659373764682491</v>
       </c>
       <c r="P114" t="n">
-        <v>0.774227761263761</v>
+        <v>0.782968897814082</v>
       </c>
       <c r="Q114" t="n">
-        <v>0.00518692549808421</v>
+        <v>0.00530454443294297</v>
       </c>
       <c r="R114" t="n">
-        <v>1.04912353545582</v>
+        <v>1.07058467341735</v>
       </c>
       <c r="S114" t="n">
         <v>0.45958348485116</v>
@@ -20774,13 +20774,13 @@
         <v>-0.327303589560573</v>
       </c>
       <c r="P115" t="n">
-        <v>0.098534410425347</v>
+        <v>0.103124277643205</v>
       </c>
       <c r="Q115" t="n">
-        <v>-0.0329718078496701</v>
+        <v>-0.0337194779137723</v>
       </c>
       <c r="R115" t="n">
-        <v>-0.260214713289482</v>
+        <v>-0.266501130738637</v>
       </c>
       <c r="S115" t="n">
         <v>-0.215022456999624</v>
@@ -20950,13 +20950,13 @@
         <v>0.362239027159003</v>
       </c>
       <c r="P116" t="n">
-        <v>0.851645101020487</v>
+        <v>0.860861867866613</v>
       </c>
       <c r="Q116" t="n">
-        <v>-1.74035327206083</v>
+        <v>-1.77981759407844</v>
       </c>
       <c r="R116" t="n">
-        <v>0.46912975557074</v>
+        <v>0.478299639106125</v>
       </c>
       <c r="S116" t="n">
         <v>-1.40704460667771</v>
@@ -21126,13 +21126,13 @@
         <v>-0.656684120594152</v>
       </c>
       <c r="P117" t="n">
-        <v>0.0589669285914424</v>
+        <v>0.0633137043630163</v>
       </c>
       <c r="Q117" t="n">
-        <v>0.52521059391167</v>
+        <v>0.537120290832369</v>
       </c>
       <c r="R117" t="n">
-        <v>0.852127227911912</v>
+        <v>0.869413611210535</v>
       </c>
       <c r="S117" t="n">
         <v>-0.758636953830839</v>
@@ -21302,13 +21302,13 @@
         <v>-0.555110684503396</v>
       </c>
       <c r="P118" t="n">
-        <v>-0.440042371479539</v>
+        <v>-0.438761368075606</v>
       </c>
       <c r="Q118" t="n">
-        <v>-1.24961421296064</v>
+        <v>-1.27795051599161</v>
       </c>
       <c r="R118" t="n">
-        <v>1.03537960702252</v>
+        <v>1.05654948303083</v>
       </c>
       <c r="S118" t="n">
         <v>-1.05336770512487</v>
@@ -21478,13 +21478,13 @@
         <v>-0.171191323351652</v>
       </c>
       <c r="P119" t="n">
-        <v>0.721336216815392</v>
+        <v>0.729752402637483</v>
       </c>
       <c r="Q119" t="n">
-        <v>1.63181386099655</v>
+        <v>1.66881693888712</v>
       </c>
       <c r="R119" t="n">
-        <v>0.546095754797195</v>
+        <v>0.556896705270648</v>
       </c>
       <c r="S119" t="n">
         <v>-0.863430109846494</v>
@@ -21654,13 +21654,13 @@
         <v>0.484364682549266</v>
       </c>
       <c r="P120" t="n">
-        <v>-3.90152852008991</v>
+        <v>-3.92151391108758</v>
       </c>
       <c r="Q120" t="n">
-        <v>0.250112748846463</v>
+        <v>0.255784315774652</v>
       </c>
       <c r="R120" t="n">
-        <v>-1.09767808582496</v>
+        <v>-1.12171206495737</v>
       </c>
       <c r="S120" t="n">
         <v>-0.313266040764301</v>
@@ -21830,13 +21830,13 @@
         <v>-0.00167720426486132</v>
       </c>
       <c r="P121" t="n">
-        <v>0.807492082807238</v>
+        <v>0.816437585965159</v>
       </c>
       <c r="Q121" t="n">
-        <v>0.669858815671763</v>
+        <v>0.685048561588523</v>
       </c>
       <c r="R121" t="n">
-        <v>0.89977284648067</v>
+        <v>0.918068937883811</v>
       </c>
       <c r="S121" t="n">
         <v>-0.411509624528978</v>
@@ -22006,13 +22006,13 @@
         <v>0.334048361818635</v>
       </c>
       <c r="P122" t="n">
-        <v>0.73444604327886</v>
+        <v>0.742942772176422</v>
       </c>
       <c r="Q122" t="n">
-        <v>0.405409919447789</v>
+        <v>0.41460301137175</v>
       </c>
       <c r="R122" t="n">
-        <v>1.17740020083324</v>
+        <v>1.20157978369155</v>
       </c>
       <c r="S122" t="n">
         <v>-0.725889092575946</v>
@@ -22182,13 +22182,13 @@
         <v>0.694385342701521</v>
       </c>
       <c r="P123" t="n">
-        <v>-1.21413360557842</v>
+        <v>-1.21760840034337</v>
       </c>
       <c r="Q123" t="n">
-        <v>-1.49808968592276</v>
+        <v>-1.53206042894697</v>
       </c>
       <c r="R123" t="n">
-        <v>0.227236615144737</v>
+        <v>0.23128028830334</v>
       </c>
       <c r="S123" t="n">
         <v>0.54472792411388</v>
@@ -22358,13 +22358,13 @@
         <v>-0.960952955218636</v>
       </c>
       <c r="P124" t="n">
-        <v>0.0883413870890033</v>
+        <v>0.0928686312469648</v>
       </c>
       <c r="Q124" t="n">
-        <v>-0.123487873000158</v>
+        <v>-0.126288089061795</v>
       </c>
       <c r="R124" t="n">
-        <v>-0.437053259131219</v>
+        <v>-0.447087247045219</v>
       </c>
       <c r="S124" t="n">
         <v>-0.195373740246688</v>
@@ -22534,13 +22534,13 @@
         <v>0.307614783107474</v>
       </c>
       <c r="P125" t="n">
-        <v>0.525221863852383</v>
+        <v>0.532433178414306</v>
       </c>
       <c r="Q125" t="n">
-        <v>-0.352440273086685</v>
+        <v>-0.360432223142089</v>
       </c>
       <c r="R125" t="n">
-        <v>-0.177751142689708</v>
+        <v>-0.182289988419506</v>
       </c>
       <c r="S125" t="n">
         <v>-0.719339520324967</v>
@@ -22710,13 +22710,13 @@
         <v>-0.472295775111498</v>
       </c>
       <c r="P126" t="n">
-        <v>0.221861776448268</v>
+        <v>0.227209332211956</v>
       </c>
       <c r="Q126" t="n">
-        <v>0.761262293225687</v>
+        <v>0.778524708139958</v>
       </c>
       <c r="R126" t="n">
-        <v>-0.246470784856186</v>
+        <v>-0.252465940352115</v>
       </c>
       <c r="S126" t="n">
         <v>-0.149526734489839</v>
@@ -22886,13 +22886,13 @@
         <v>-0.150797729928393</v>
       </c>
       <c r="P127" t="n">
-        <v>-0.672158243845515</v>
+        <v>-0.672303294880826</v>
       </c>
       <c r="Q127" t="n">
-        <v>0.842016821938377</v>
+        <v>0.861110429850449</v>
       </c>
       <c r="R127" t="n">
-        <v>0.281296066982366</v>
+        <v>0.286485370490326</v>
       </c>
       <c r="S127" t="n">
         <v>0.223798883815934</v>
@@ -23062,13 +23062,13 @@
         <v>0.198293083061531</v>
       </c>
       <c r="P128" t="n">
-        <v>0.840836530708299</v>
+        <v>0.849986892747557</v>
       </c>
       <c r="Q128" t="n">
-        <v>-1.71284348755431</v>
+        <v>-1.75168399657267</v>
       </c>
       <c r="R128" t="n">
-        <v>-1.18380670400695</v>
+        <v>-1.20966592471291</v>
       </c>
       <c r="S128" t="n">
         <v>-1.41359417892869</v>
@@ -23238,13 +23238,13 @@
         <v>-0.509686741274246</v>
       </c>
       <c r="P129" t="n">
-        <v>-0.0678924480159823</v>
+        <v>-0.0643250604668799</v>
       </c>
       <c r="Q129" t="n">
-        <v>0.159596683695975</v>
+        <v>0.163215704626629</v>
       </c>
       <c r="R129" t="n">
-        <v>-0.270293594140566</v>
+        <v>-0.276793603688753</v>
       </c>
       <c r="S129" t="n">
         <v>-1.05336770512487</v>
@@ -23414,13 +23414,13 @@
         <v>0.659503919247617</v>
       </c>
       <c r="P130" t="n">
-        <v>0.275622148646877</v>
+        <v>0.281299992971395</v>
       </c>
       <c r="Q130" t="n">
-        <v>0.879288142882695</v>
+        <v>0.899226916793752</v>
       </c>
       <c r="R130" t="n">
-        <v>1.46235765035024</v>
+        <v>1.49257606437211</v>
       </c>
       <c r="S130" t="n">
         <v>0.0993570110473433</v>
@@ -23590,13 +23590,13 @@
         <v>0.387074145117204</v>
       </c>
       <c r="P131" t="n">
-        <v>0.632430590780875</v>
+        <v>0.640300565517149</v>
       </c>
       <c r="Q131" t="n">
-        <v>1.11090278017953</v>
+        <v>1.13609365708428</v>
       </c>
       <c r="R131" t="n">
-        <v>0.408656470464239</v>
+        <v>0.416544801405429</v>
       </c>
       <c r="S131" t="n">
         <v>-1.21055743914835</v>
@@ -23766,13 +23766,13 @@
         <v>1.00948547754263</v>
       </c>
       <c r="P132" t="n">
-        <v>0.171031448596891</v>
+        <v>0.176066717165647</v>
       </c>
       <c r="Q132" t="n">
-        <v>1.33985518026606</v>
+        <v>1.37023779116457</v>
       </c>
       <c r="R132" t="n">
-        <v>1.32400210412173</v>
+        <v>1.35128848114779</v>
       </c>
       <c r="S132" t="n">
         <v>2.47685173815253</v>
@@ -23942,13 +23942,13 @@
         <v>-0.796156939117681</v>
       </c>
       <c r="P133" t="n">
-        <v>0.622976699141395</v>
+        <v>0.630788591834407</v>
       </c>
       <c r="Q133" t="n">
-        <v>0.449780539619597</v>
+        <v>0.45997978154235</v>
       </c>
       <c r="R133" t="n">
-        <v>-1.63644008041015</v>
+        <v>-1.67189152810903</v>
       </c>
       <c r="S133" t="n">
         <v>-1.2564044449052</v>
@@ -24118,13 +24118,13 @@
         <v>-0.0598725641970494</v>
       </c>
       <c r="P134" t="n">
-        <v>0.158952060672688</v>
+        <v>0.163913116889668</v>
       </c>
       <c r="Q134" t="n">
-        <v>-0.231752186219368</v>
+        <v>-0.237007408278058</v>
       </c>
       <c r="R134" t="n">
-        <v>-0.32444467216775</v>
+        <v>-0.332092253811649</v>
       </c>
       <c r="S134" t="n">
         <v>-0.562149786301484</v>
@@ -24294,13 +24294,13 @@
         <v>0.773328153780905</v>
       </c>
       <c r="P135" t="n">
-        <v>0.22815984396173</v>
+        <v>0.233546093275518</v>
       </c>
       <c r="Q135" t="n">
-        <v>-1.01178768883975</v>
+        <v>-1.0347310278772</v>
       </c>
       <c r="R135" t="n">
-        <v>-0.522265615417652</v>
+        <v>-0.534105427441654</v>
       </c>
       <c r="S135" t="n">
         <v>0.911503970168675</v>
@@ -24470,13 +24470,13 @@
         <v>-2.09041800206579</v>
       </c>
       <c r="P136" t="n">
-        <v>-0.0758741875940949</v>
+        <v>-0.0723558376012882</v>
       </c>
       <c r="Q136" t="n">
-        <v>-1.23009114008504</v>
+        <v>-1.25798473711655</v>
       </c>
       <c r="R136" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S136" t="n">
         <v>0.256546745070826</v>
@@ -24646,13 +24646,13 @@
         <v>0.581431516822516</v>
       </c>
       <c r="P137" t="n">
-        <v>-0.254356667667124</v>
+        <v>-0.251934863681451</v>
       </c>
       <c r="Q137" t="n">
-        <v>-1.22565407806786</v>
+        <v>-1.25344706009949</v>
       </c>
       <c r="R137" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S137" t="n">
         <v>1.44856889474891</v>
@@ -24822,13 +24822,13 @@
         <v>0.775093375070434</v>
       </c>
       <c r="P138" t="n">
-        <v>-0.103668187640164</v>
+        <v>-0.100320596142871</v>
       </c>
       <c r="Q138" t="n">
-        <v>1.59542995245567</v>
+        <v>1.63160798734723</v>
       </c>
       <c r="R138" t="n">
-        <v>-0.485615139595531</v>
+        <v>-0.496678253077596</v>
       </c>
       <c r="S138" t="n">
         <v>0.610223646623665</v>
@@ -24998,13 +24998,13 @@
         <v>0.726236605186072</v>
       </c>
       <c r="P139" t="n">
-        <v>-0.304117851874301</v>
+        <v>-0.30200176656662</v>
       </c>
       <c r="Q139" t="n">
-        <v>0.0531071952836367</v>
+        <v>0.0543114562171906</v>
       </c>
       <c r="R139" t="n">
-        <v>-0.525014401104312</v>
+        <v>-0.536912465518959</v>
       </c>
       <c r="S139" t="n">
         <v>0.865656964411826</v>
@@ -25174,13 +25174,13 @@
         <v>-3.24998535942862</v>
       </c>
       <c r="P140" t="n">
-        <v>-1.19332316082531</v>
+        <v>-1.19667010208839</v>
       </c>
       <c r="Q140" t="n">
-        <v>-0.510399680898321</v>
+        <v>-0.521973524949423</v>
       </c>
       <c r="R140" t="n">
-        <v>-1.79495338834083</v>
+        <v>-1.83376405723358</v>
       </c>
       <c r="S140" t="n">
         <v>-0.49010449154072</v>
@@ -25350,13 +25350,13 @@
         <v>0.67235668255386</v>
       </c>
       <c r="P141" t="n">
-        <v>0.915750261308999</v>
+        <v>0.925360872175683</v>
       </c>
       <c r="Q141" t="n">
-        <v>0.888162266917056</v>
+        <v>0.908302270827872</v>
       </c>
       <c r="R141" t="n">
-        <v>0.844797132747487</v>
+        <v>0.861928176337724</v>
       </c>
       <c r="S141" t="n">
         <v>0.0993570110473433</v>
@@ -25526,13 +25526,13 @@
         <v>-2.05333208566506</v>
       </c>
       <c r="P142" t="n">
-        <v>-1.40847804878684</v>
+        <v>-1.41314684098572</v>
       </c>
       <c r="Q142" t="n">
-        <v>-0.00901167295689425</v>
+        <v>-0.00921602202164887</v>
       </c>
       <c r="R142" t="n">
-        <v>-0.653291066481737</v>
+        <v>-0.667907575793163</v>
       </c>
       <c r="S142" t="n">
         <v>-0.686591659070075</v>
@@ -25702,13 +25702,13 @@
         <v>0.532233091204698</v>
       </c>
       <c r="P143" t="n">
-        <v>0.730274379907544</v>
+        <v>0.738745479282191</v>
       </c>
       <c r="Q143" t="n">
-        <v>-1.91783575274806</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R143" t="n">
-        <v>-0.615724328764062</v>
+        <v>-0.629544722070003</v>
       </c>
       <c r="S143" t="n">
         <v>-1.23675572815227</v>
@@ -25878,13 +25878,13 @@
         <v>0.734021475112701</v>
       </c>
       <c r="P144" t="n">
-        <v>0.0447703035236298</v>
+        <v>0.0490298592356968</v>
       </c>
       <c r="Q144" t="n">
-        <v>-0.196255690081922</v>
+        <v>-0.200705992141578</v>
       </c>
       <c r="R144" t="n">
-        <v>-0.3106091175449</v>
+        <v>-0.317963495489217</v>
       </c>
       <c r="S144" t="n">
         <v>0.367889473337461</v>
@@ -26054,13 +26054,13 @@
         <v>-1.52961451957697</v>
       </c>
       <c r="P145" t="n">
-        <v>0.0385598317739663</v>
+        <v>0.0427812320995958</v>
       </c>
       <c r="Q145" t="n">
-        <v>-1.09076739274556</v>
+        <v>-1.11550167878086</v>
       </c>
       <c r="R145" t="n">
-        <v>0.6377219443525</v>
+        <v>0.650464641180794</v>
       </c>
       <c r="S145" t="n">
         <v>-1.21055743914835</v>
@@ -26230,13 +26230,13 @@
         <v>-1.04388581718518</v>
       </c>
       <c r="P146" t="n">
-        <v>0.611517611451536</v>
+        <v>0.619259102742424</v>
       </c>
       <c r="Q146" t="n">
-        <v>-0.166971080768529</v>
+        <v>-0.170757323828983</v>
       </c>
       <c r="R146" t="n">
-        <v>-1.65843036590343</v>
+        <v>-1.69434783272747</v>
       </c>
       <c r="S146" t="n">
         <v>-0.942024976858236</v>
@@ -26406,13 +26406,13 @@
         <v>0.479536761649105</v>
       </c>
       <c r="P147" t="n">
-        <v>0.808880713326379</v>
+        <v>0.817834747838473</v>
       </c>
       <c r="Q147" t="n">
-        <v>-0.254824908708708</v>
+        <v>-0.26060332876677</v>
       </c>
       <c r="R147" t="n">
-        <v>0.690865134294576</v>
+        <v>0.704734044008678</v>
       </c>
       <c r="S147" t="n">
         <v>0.315492895329633</v>
@@ -26582,13 +26582,13 @@
         <v>-0.115359082242542</v>
       </c>
       <c r="P148" t="n">
-        <v>0.313648556171153</v>
+        <v>0.319560024016138</v>
       </c>
       <c r="Q148" t="n">
-        <v>-0.133249409437955</v>
+        <v>-0.136270978499327</v>
       </c>
       <c r="R148" t="n">
-        <v>0.0623094739451889</v>
+        <v>0.0628580036650769</v>
       </c>
       <c r="S148" t="n">
         <v>-0.483554919289742</v>
@@ -26758,13 +26758,13 @@
         <v>0.353534940616168</v>
       </c>
       <c r="P149" t="n">
-        <v>0.795057898087802</v>
+        <v>0.803927009122527</v>
       </c>
       <c r="Q149" t="n">
-        <v>-1.83086933721132</v>
+        <v>-1.87238620522646</v>
       </c>
       <c r="R149" t="n">
-        <v>-0.293200141529392</v>
+        <v>-0.300185587666289</v>
       </c>
       <c r="S149" t="n">
         <v>-1.21055743914835</v>
@@ -26934,13 +26934,13 @@
         <v>-0.971536148295485</v>
       </c>
       <c r="P150" t="n">
-        <v>0.129107708620484</v>
+        <v>0.133885409557635</v>
       </c>
       <c r="Q150" t="n">
-        <v>0.396535795413428</v>
+        <v>0.40552765733763</v>
       </c>
       <c r="R150" t="n">
-        <v>0.680786253443493</v>
+        <v>0.694441571058563</v>
       </c>
       <c r="S150" t="n">
         <v>-0.647294225564204</v>
@@ -27110,13 +27110,13 @@
         <v>-1.0114651284782</v>
       </c>
       <c r="P151" t="n">
-        <v>-0.551500851026146</v>
+        <v>-0.55090461707778</v>
       </c>
       <c r="Q151" t="n">
-        <v>-1.56730785339078</v>
+        <v>-1.6028481904131</v>
       </c>
       <c r="R151" t="n">
-        <v>-0.349092117158127</v>
+        <v>-0.357262028571478</v>
       </c>
       <c r="S151" t="n">
         <v>-1.19090872239542</v>
@@ -27286,13 +27286,13 @@
         <v>0.420340838497507</v>
       </c>
       <c r="P152" t="n">
-        <v>0.765180612744557</v>
+        <v>0.773866166166604</v>
       </c>
       <c r="Q152" t="n">
-        <v>1.63181386099655</v>
+        <v>1.66881693888712</v>
       </c>
       <c r="R152" t="n">
-        <v>0.676204943965727</v>
+        <v>0.689763174263055</v>
       </c>
       <c r="S152" t="n">
         <v>0.642971507878557</v>
@@ -27462,13 +27462,13 @@
         <v>0.392626050785882</v>
       </c>
       <c r="P153" t="n">
-        <v>-3.58897427267153</v>
+        <v>-3.60703941854554</v>
       </c>
       <c r="Q153" t="n">
-        <v>-0.415446553730652</v>
+        <v>-0.42486723678434</v>
       </c>
       <c r="R153" t="n">
-        <v>-1.26627027460672</v>
+        <v>-1.29387706703204</v>
       </c>
       <c r="S153" t="n">
         <v>-0.745537809328881</v>
@@ -27638,13 +27638,13 @@
         <v>-0.0307545475801543</v>
       </c>
       <c r="P154" t="n">
-        <v>0.725236265415238</v>
+        <v>0.733676412035711</v>
       </c>
       <c r="Q154" t="n">
-        <v>-0.031196983042798</v>
+        <v>-0.0319044071069485</v>
       </c>
       <c r="R154" t="n">
-        <v>1.02896577375365</v>
+        <v>1.04999972751712</v>
       </c>
       <c r="S154" t="n">
         <v>-0.0578327229761407</v>
@@ -27814,13 +27814,13 @@
         <v>0.326137404657039</v>
       </c>
       <c r="P155" t="n">
-        <v>0.739243778698415</v>
+        <v>0.747769983528939</v>
       </c>
       <c r="Q155" t="n">
-        <v>-0.231752186219368</v>
+        <v>-0.237007408278058</v>
       </c>
       <c r="R155" t="n">
-        <v>1.05370484493358</v>
+        <v>1.07526307021286</v>
       </c>
       <c r="S155" t="n">
         <v>-1.13851214438759</v>
@@ -27990,13 +27990,13 @@
         <v>0.711260695536204</v>
       </c>
       <c r="P156" t="n">
-        <v>-0.900642966235401</v>
+        <v>-0.90219176294886</v>
       </c>
       <c r="Q156" t="n">
-        <v>-0.127037522613903</v>
+        <v>-0.129918230675443</v>
       </c>
       <c r="R156" t="n">
-        <v>-1.20671325139578</v>
+        <v>-1.23305790869044</v>
       </c>
       <c r="S156" t="n">
         <v>0.54472792411388</v>
@@ -28166,13 +28166,13 @@
         <v>-0.692720665813553</v>
       </c>
       <c r="P157" t="n">
-        <v>-0.164852810098444</v>
+        <v>-0.161881119661172</v>
       </c>
       <c r="Q157" t="n">
-        <v>-1.03397299892565</v>
+        <v>-1.0574194129625</v>
       </c>
       <c r="R157" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S157" t="n">
         <v>-0.771736098332795</v>
@@ -28342,13 +28342,13 @@
         <v>0.372134841438778</v>
       </c>
       <c r="P158" t="n">
-        <v>0.468930381502136</v>
+        <v>0.475795857076493</v>
       </c>
       <c r="Q158" t="n">
-        <v>-0.149222832699806</v>
+        <v>-0.152606615760743</v>
       </c>
       <c r="R158" t="n">
-        <v>-0.694522851781624</v>
+        <v>-0.710013146952729</v>
       </c>
       <c r="S158" t="n">
         <v>-0.477005347038763</v>
@@ -28518,13 +28518,13 @@
         <v>-0.35366395632885</v>
       </c>
       <c r="P159" t="n">
-        <v>0.12922789815686</v>
+        <v>0.134006337504616</v>
       </c>
       <c r="Q159" t="n">
-        <v>0.103689702279497</v>
+        <v>0.106040974211674</v>
       </c>
       <c r="R159" t="n">
-        <v>-0.275791165513884</v>
+        <v>-0.282407679843362</v>
       </c>
       <c r="S159" t="n">
         <v>0.37443904558844</v>
@@ -28694,13 +28694,13 @@
         <v>-0.734919216225661</v>
       </c>
       <c r="P160" t="n">
-        <v>-0.726490025619605</v>
+        <v>-0.726968875794979</v>
       </c>
       <c r="Q160" t="n">
-        <v>1.08694264528675</v>
+        <v>1.11159020119216</v>
       </c>
       <c r="R160" t="n">
-        <v>-0.250135832438398</v>
+        <v>-0.256208657788521</v>
       </c>
       <c r="S160" t="n">
         <v>0.132104872302236</v>
@@ -28870,13 +28870,13 @@
         <v>0.0135508798549395</v>
       </c>
       <c r="P161" t="n">
-        <v>0.796581996474214</v>
+        <v>0.805460471139472</v>
       </c>
       <c r="Q161" t="n">
-        <v>-1.57440715261827</v>
+        <v>-1.6101084736404</v>
       </c>
       <c r="R161" t="n">
-        <v>-0.0577208343722595</v>
+        <v>-0.0597159923772142</v>
       </c>
       <c r="S161" t="n">
         <v>-1.30225145066205</v>
@@ -29046,13 +29046,13 @@
         <v>0.126293204565613</v>
       </c>
       <c r="P162" t="n">
-        <v>-0.163864132330293</v>
+        <v>-0.160886367735723</v>
       </c>
       <c r="Q162" t="n">
-        <v>-0.70651782205771</v>
+        <v>-0.722538849103472</v>
       </c>
       <c r="R162" t="n">
-        <v>0.267552138549071</v>
+        <v>0.272450180103804</v>
       </c>
       <c r="S162" t="n">
         <v>-0.83723182084258</v>
@@ -29222,13 +29222,13 @@
         <v>0.554635945727097</v>
       </c>
       <c r="P163" t="n">
-        <v>0.583215691782818</v>
+        <v>0.590783304063316</v>
       </c>
       <c r="Q163" t="n">
-        <v>0.970691620436618</v>
+        <v>0.992703063345187</v>
       </c>
       <c r="R163" t="n">
-        <v>1.39180548439265</v>
+        <v>1.4205287537213</v>
       </c>
       <c r="S163" t="n">
         <v>0.0600595775414719</v>
@@ -29398,13 +29398,13 @@
         <v>0.402769972205429</v>
       </c>
       <c r="P164" t="n">
-        <v>0.619903038483746</v>
+        <v>0.627696047472766</v>
       </c>
       <c r="Q164" t="n">
-        <v>0.883725204899876</v>
+        <v>0.903764593810813</v>
       </c>
       <c r="R164" t="n">
-        <v>0.0018361888386882</v>
+        <v>0.00110316596438066</v>
       </c>
       <c r="S164" t="n">
         <v>-1.13196257213661</v>
@@ -29574,13 +29574,13 @@
         <v>1.03440194210403</v>
       </c>
       <c r="P165" t="n">
-        <v>0.126120285652777</v>
+        <v>0.130879632705976</v>
       </c>
       <c r="Q165" t="n">
-        <v>1.48272857721928</v>
+        <v>1.51635099111391</v>
       </c>
       <c r="R165" t="n">
-        <v>1.13983346311557</v>
+        <v>1.16321692996839</v>
       </c>
       <c r="S165" t="n">
         <v>2.14937312560361</v>
@@ -29750,13 +29750,13 @@
         <v>-0.56079681206736</v>
       </c>
       <c r="P166" t="n">
-        <v>0.6060028130353</v>
+        <v>0.61371042296046</v>
       </c>
       <c r="Q166" t="n">
-        <v>0.0602064945111259</v>
+        <v>0.0615717394444866</v>
       </c>
       <c r="R166" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S166" t="n">
         <v>-0.673492514568118</v>
@@ -29926,13 +29926,13 @@
         <v>-0.0624959921503804</v>
       </c>
       <c r="P167" t="n">
-        <v>0.318705683697462</v>
+        <v>0.324648221107338</v>
       </c>
       <c r="Q167" t="n">
-        <v>-0.320493426562984</v>
+        <v>-0.327760948619257</v>
       </c>
       <c r="R167" t="n">
-        <v>-0.0353640441207653</v>
+        <v>-0.0368854160151386</v>
       </c>
       <c r="S167" t="n">
         <v>-0.542501069548548</v>
@@ -30102,13 +30102,13 @@
         <v>0.852824121762078</v>
       </c>
       <c r="P168" t="n">
-        <v>0.137684284548116</v>
+        <v>0.14251467754829</v>
       </c>
       <c r="Q168" t="n">
-        <v>-0.984277904333226</v>
+        <v>-1.00659743037142</v>
       </c>
       <c r="R168" t="n">
-        <v>-0.531428234373183</v>
+        <v>-0.543462221032669</v>
       </c>
       <c r="S168" t="n">
         <v>1.02939627068629</v>
@@ -30278,13 +30278,13 @@
         <v>-2.08043677385266</v>
       </c>
       <c r="P169" t="n">
-        <v>-0.0130598765069946</v>
+        <v>-0.00915561310697129</v>
       </c>
       <c r="Q169" t="n">
-        <v>-1.21323030441975</v>
+        <v>-1.24074156445172</v>
       </c>
       <c r="R169" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S169" t="n">
         <v>0.400637334592353</v>
@@ -30454,13 +30454,13 @@
         <v>0.720818921412681</v>
       </c>
       <c r="P170" t="n">
-        <v>0.0119001629172489</v>
+        <v>0.015957773758194</v>
       </c>
       <c r="Q170" t="n">
-        <v>-1.12537647647957</v>
+        <v>-1.15089555951393</v>
       </c>
       <c r="R170" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S170" t="n">
         <v>2.26726542612122</v>
@@ -30630,13 +30630,13 @@
         <v>0.785184421197898</v>
       </c>
       <c r="P171" t="n">
-        <v>0.0321673781274179</v>
+        <v>0.0363495050211731</v>
       </c>
       <c r="Q171" t="n">
-        <v>1.36647755236914</v>
+        <v>1.39746385326693</v>
       </c>
       <c r="R171" t="n">
-        <v>1.0280495118581</v>
+        <v>1.04906404815802</v>
       </c>
       <c r="S171" t="n">
         <v>0.931152686921611</v>
@@ -30806,13 +30806,13 @@
         <v>0.805362446122666</v>
       </c>
       <c r="P172" t="n">
-        <v>-0.0093598042826433</v>
+        <v>-0.00543280868267485</v>
       </c>
       <c r="Q172" t="n">
-        <v>0.0557694324939453</v>
+        <v>0.0570340624274267</v>
       </c>
       <c r="R172" t="n">
-        <v>-0.32893435545596</v>
+        <v>-0.336677082671247</v>
       </c>
       <c r="S172" t="n">
         <v>1.13418942670194</v>
@@ -30982,13 +30982,13 @@
         <v>-2.74123963566024</v>
       </c>
       <c r="P173" t="n">
-        <v>-1.22481214031877</v>
+        <v>-1.22835254098871</v>
       </c>
       <c r="Q173" t="n">
-        <v>-0.544121352228894</v>
+        <v>-0.556459870279078</v>
       </c>
       <c r="R173" t="n">
-        <v>-1.26352148892006</v>
+        <v>-1.29107002895474</v>
       </c>
       <c r="S173" t="n">
         <v>-0.195373740246688</v>
@@ -31158,13 +31158,13 @@
         <v>0.729311506787186</v>
       </c>
       <c r="P174" t="n">
-        <v>0.937619664152377</v>
+        <v>0.947364634460707</v>
       </c>
       <c r="Q174" t="n">
-        <v>0.901473452968599</v>
+        <v>0.921915301879052</v>
       </c>
       <c r="R174" t="n">
-        <v>1.11417813004008</v>
+        <v>1.13701790791355</v>
       </c>
       <c r="S174" t="n">
         <v>0.217249311564956</v>
@@ -31334,13 +31334,13 @@
         <v>-2.6503958165321</v>
       </c>
       <c r="P175" t="n">
-        <v>-0.880534645666542</v>
+        <v>-0.881959902531042</v>
       </c>
       <c r="Q175" t="n">
-        <v>-0.189156390854433</v>
+        <v>-0.193445708914283</v>
       </c>
       <c r="R175" t="n">
-        <v>-0.407732878473522</v>
+        <v>-0.417145507553972</v>
       </c>
       <c r="S175" t="n">
         <v>-0.352563474270172</v>
@@ -31510,13 +31510,13 @@
         <v>0.526823542091628</v>
       </c>
       <c r="P176" t="n">
-        <v>0.890089455774362</v>
+        <v>0.89954241389083</v>
       </c>
       <c r="Q176" t="n">
-        <v>-1.91783575274806</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R176" t="n">
-        <v>0.427897970270853</v>
+        <v>0.436194067946559</v>
       </c>
       <c r="S176" t="n">
         <v>-1.014070271619</v>
@@ -31686,13 +31686,13 @@
         <v>0.745300181646945</v>
       </c>
       <c r="P177" t="n">
-        <v>0.0897914704501892</v>
+        <v>0.094327623511249</v>
       </c>
       <c r="Q177" t="n">
-        <v>-0.245063372270911</v>
+        <v>-0.250620439329238</v>
       </c>
       <c r="R177" t="n">
-        <v>-0.0540557867900473</v>
+        <v>-0.0559732749408083</v>
       </c>
       <c r="S177" t="n">
         <v>1.04904498743922</v>
@@ -31862,13 +31862,13 @@
         <v>-2.42554567061574</v>
       </c>
       <c r="P178" t="n">
-        <v>0.267045572719245</v>
+        <v>0.27267072498074</v>
       </c>
       <c r="Q178" t="n">
-        <v>-1.25405127497782</v>
+        <v>-1.28248819300867</v>
       </c>
       <c r="R178" t="n">
-        <v>0.172260901411554</v>
+        <v>0.175139526757252</v>
       </c>
       <c r="S178" t="n">
         <v>-0.909277115603344</v>
@@ -32038,13 +32038,13 @@
         <v>-0.614143914448586</v>
       </c>
       <c r="P179" t="n">
-        <v>0.640745737490967</v>
+        <v>0.648666798142901</v>
       </c>
       <c r="Q179" t="n">
-        <v>-0.00546202334314964</v>
+        <v>-0.00558588040800091</v>
       </c>
       <c r="R179" t="n">
-        <v>-1.02346087228517</v>
+        <v>-1.04592203687015</v>
       </c>
       <c r="S179" t="n">
         <v>-1.19090872239542</v>
@@ -32214,13 +32214,13 @@
         <v>0.635274833483287</v>
       </c>
       <c r="P180" t="n">
-        <v>0.880193511094314</v>
+        <v>0.889585671318343</v>
       </c>
       <c r="Q180" t="n">
-        <v>-0.518386392529246</v>
+        <v>-0.530141343580131</v>
       </c>
       <c r="R180" t="n">
-        <v>1.0747788685313</v>
+        <v>1.09678369547219</v>
       </c>
       <c r="S180" t="n">
         <v>0.276195461823763</v>
@@ -32390,13 +32390,13 @@
         <v>0.0263100945674971</v>
       </c>
       <c r="P181" t="n">
-        <v>0.488441489092225</v>
+        <v>0.495426835407475</v>
       </c>
       <c r="Q181" t="n">
-        <v>-0.848503806607495</v>
+        <v>-0.86774451364939</v>
       </c>
       <c r="R181" t="n">
-        <v>0.234566710309161</v>
+        <v>0.238765723176151</v>
       </c>
       <c r="S181" t="n">
         <v>-0.83723182084258</v>
@@ -32566,13 +32566,13 @@
         <v>0.378768656930069</v>
       </c>
       <c r="P182" t="n">
-        <v>0.793042856001958</v>
+        <v>0.801899587186557</v>
       </c>
       <c r="Q182" t="n">
-        <v>-1.91783575274806</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R182" t="n">
-        <v>-0.63313330477957</v>
+        <v>-0.647322629892931</v>
       </c>
       <c r="S182" t="n">
         <v>-1.44634204018358</v>
@@ -32742,13 +32742,13 @@
         <v>-0.93741531558154</v>
       </c>
       <c r="P183" t="n">
-        <v>0.145527161074315</v>
+        <v>0.150405738495367</v>
       </c>
       <c r="Q183" t="n">
-        <v>0.342403638803823</v>
+        <v>0.350167997729499</v>
       </c>
       <c r="R183" t="n">
-        <v>0.906186679749541</v>
+        <v>0.924618693397521</v>
       </c>
       <c r="S183" t="n">
         <v>-0.830682248591602</v>
@@ -32918,13 +32918,13 @@
         <v>-0.920129162400676</v>
       </c>
       <c r="P184" t="n">
-        <v>-0.312135240891169</v>
+        <v>-0.310068412159879</v>
       </c>
       <c r="Q184" t="n">
-        <v>-0.915947149268642</v>
+        <v>-0.936717204308702</v>
       </c>
       <c r="R184" t="n">
-        <v>0.389414970657625</v>
+        <v>0.396895534864298</v>
       </c>
       <c r="S184" t="n">
         <v>-1.11231385538368</v>
@@ -33094,13 +33094,13 @@
         <v>0.509106251913782</v>
       </c>
       <c r="P185" t="n">
-        <v>0.870717211236187</v>
+        <v>0.88005115174718</v>
       </c>
       <c r="Q185" t="n">
-        <v>1.35849084073822</v>
+        <v>1.38929603463623</v>
       </c>
       <c r="R185" t="n">
-        <v>1.12792205847338</v>
+        <v>1.15105309830007</v>
       </c>
       <c r="S185" t="n">
         <v>1.17348686020781</v>
@@ -33270,13 +33270,13 @@
         <v>0.471259744773091</v>
       </c>
       <c r="P186" t="n">
-        <v>-2.62837739766886</v>
+        <v>-2.64054090733006</v>
       </c>
       <c r="Q186" t="n">
-        <v>-0.219328412571262</v>
+        <v>-0.22430191263029</v>
       </c>
       <c r="R186" t="n">
-        <v>-0.502107853715485</v>
+        <v>-0.513520481541422</v>
       </c>
       <c r="S186" t="n">
         <v>-0.10367972873299</v>
@@ -33446,13 +33446,13 @@
         <v>0.256882974019259</v>
       </c>
       <c r="P187" t="n">
-        <v>0.790693048710278</v>
+        <v>0.799535343341764</v>
       </c>
       <c r="Q187" t="n">
-        <v>-0.186494153644125</v>
+        <v>-0.190723102704046</v>
       </c>
       <c r="R187" t="n">
-        <v>1.11509439193564</v>
+        <v>1.13795358727265</v>
       </c>
       <c r="S187" t="n">
         <v>-0.326365185266258</v>
@@ -33622,13 +33622,13 @@
         <v>0.481175895703667</v>
       </c>
       <c r="P188" t="n">
-        <v>0.79108145783348</v>
+        <v>0.799926138741048</v>
       </c>
       <c r="Q188" t="n">
-        <v>-0.674570975534009</v>
+        <v>-0.689867574580641</v>
       </c>
       <c r="R188" t="n">
-        <v>1.17648393893769</v>
+        <v>1.20064410433245</v>
       </c>
       <c r="S188" t="n">
         <v>-1.12541299988563</v>
@@ -33798,13 +33798,13 @@
         <v>0.728331280218577</v>
       </c>
       <c r="P189" t="n">
-        <v>-0.309148157441927</v>
+        <v>-0.30706297691259</v>
       </c>
       <c r="Q189" t="n">
-        <v>-0.520161217336118</v>
+        <v>-0.531956414386954</v>
       </c>
       <c r="R189" t="n">
-        <v>-1.13524482354264</v>
+        <v>-1.16007491868053</v>
       </c>
       <c r="S189" t="n">
         <v>1.40272188899206</v>
@@ -33974,13 +33974,13 @@
         <v>-0.25660525671592</v>
       </c>
       <c r="P190" t="n">
-        <v>0.27393949513762</v>
+        <v>0.279607001713658</v>
       </c>
       <c r="Q190" t="n">
-        <v>-1.91783575274806</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R190" t="n">
-        <v>-0.773321374799186</v>
+        <v>-0.790481571835455</v>
       </c>
       <c r="S190" t="n">
         <v>-0.83723182084258</v>
@@ -34150,13 +34150,13 @@
         <v>-0.0376568068620193</v>
       </c>
       <c r="P191" t="n">
-        <v>0.560688302155553</v>
+        <v>0.568117512509225</v>
       </c>
       <c r="Q191" t="n">
-        <v>-0.695868873216477</v>
+        <v>-0.711648424262529</v>
       </c>
       <c r="R191" t="n">
-        <v>-1.21129456087354</v>
+        <v>-1.23773630548595</v>
       </c>
       <c r="S191" t="n">
         <v>-0.647294225564204</v>
@@ -34326,13 +34326,13 @@
         <v>0.205776970556305</v>
       </c>
       <c r="P192" t="n">
-        <v>0.314164284718482</v>
+        <v>0.320078921054173</v>
       </c>
       <c r="Q192" t="n">
-        <v>-0.0693557163905523</v>
+        <v>-0.0709284294536638</v>
       </c>
       <c r="R192" t="n">
-        <v>0.0897973308117804</v>
+        <v>0.0909283844381209</v>
       </c>
       <c r="S192" t="n">
         <v>0.191051022561042</v>
@@ -34502,13 +34502,13 @@
         <v>-1.06823692285432</v>
       </c>
       <c r="P193" t="n">
-        <v>-0.354954630576499</v>
+        <v>-0.35315087209596</v>
       </c>
       <c r="Q193" t="n">
-        <v>0.73730215833291</v>
+        <v>0.754021252247834</v>
       </c>
       <c r="R193" t="n">
-        <v>-0.356422212322552</v>
+        <v>-0.36474746344429</v>
       </c>
       <c r="S193" t="n">
         <v>0.125555300051257</v>
@@ -34678,13 +34678,13 @@
         <v>0.127818453375689</v>
       </c>
       <c r="P194" t="n">
-        <v>0.796177969501652</v>
+        <v>0.805053961939168</v>
       </c>
       <c r="Q194" t="n">
-        <v>-1.91162386592401</v>
+        <v>-1.95497192693695</v>
       </c>
       <c r="R194" t="n">
-        <v>0.82738815673198</v>
+        <v>0.844150268514796</v>
       </c>
       <c r="S194" t="n">
         <v>-1.29570187841107</v>
@@ -34854,13 +34854,13 @@
         <v>0.196942729448344</v>
       </c>
       <c r="P195" t="n">
-        <v>0.115191865322679</v>
+        <v>0.119884071244309</v>
       </c>
       <c r="Q195" t="n">
-        <v>-0.737577256177975</v>
+        <v>-0.754302588222892</v>
       </c>
       <c r="R195" t="n">
-        <v>0.411405256150898</v>
+        <v>0.419351839482733</v>
       </c>
       <c r="S195" t="n">
         <v>-0.62109593656029</v>
@@ -35030,13 +35030,13 @@
         <v>0.65175158796227</v>
       </c>
       <c r="P196" t="n">
-        <v>0.608196441833386</v>
+        <v>0.615917528795051</v>
       </c>
       <c r="Q196" t="n">
-        <v>1.25200135232588</v>
+        <v>1.28039178622679</v>
       </c>
       <c r="R196" t="n">
-        <v>1.15815870102663</v>
+        <v>1.18193051715042</v>
       </c>
       <c r="S196" t="n">
         <v>0.171402305808106</v>
@@ -35206,13 +35206,13 @@
         <v>0.523386648106256</v>
       </c>
       <c r="P197" t="n">
-        <v>0.693776144991251</v>
+        <v>0.702023009506832</v>
       </c>
       <c r="Q197" t="n">
-        <v>0.74883851957758</v>
+        <v>0.76581921249219</v>
       </c>
       <c r="R197" t="n">
-        <v>0.484706207795142</v>
+        <v>0.49420618821085</v>
       </c>
       <c r="S197" t="n">
         <v>-1.03371898837193</v>
@@ -35382,13 +35382,13 @@
         <v>0.991979688533111</v>
       </c>
       <c r="P198" t="n">
-        <v>0.424798752952141</v>
+        <v>0.43139309625035</v>
       </c>
       <c r="Q198" t="n">
-        <v>1.34606706709011</v>
+        <v>1.37659053898846</v>
       </c>
       <c r="R198" t="n">
-        <v>1.27452396176186</v>
+        <v>1.30076179575631</v>
       </c>
       <c r="S198" t="n">
         <v>2.86327650096026</v>
@@ -35558,13 +35558,13 @@
         <v>-2.00103435446517</v>
       </c>
       <c r="P199" t="n">
-        <v>0.646768116011388</v>
+        <v>0.65472617645802</v>
       </c>
       <c r="Q199" t="n">
-        <v>-0.179394854416635</v>
+        <v>-0.183462819476751</v>
       </c>
       <c r="R199" t="n">
-        <v>-1.97454071986922</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S199" t="n">
         <v>-0.948574549109214</v>
@@ -35732,13 +35732,13 @@
         <v>1.97544228013687</v>
       </c>
       <c r="P200" t="n">
-        <v>1.92354779252317</v>
+        <v>1.14245010770843</v>
       </c>
       <c r="Q200" t="n">
-        <v>2.59807612914943</v>
+        <v>1.66881693888712</v>
       </c>
       <c r="R200" t="n">
-        <v>2.50594640955528</v>
+        <v>1.72556022478837</v>
       </c>
       <c r="S200" t="n">
         <v>4.60546271972054</v>
@@ -35906,13 +35906,13 @@
         <v>-4.53979112403857</v>
       </c>
       <c r="P201" t="n">
-        <v>-5.42548307093489</v>
+        <v>-5.45483120878088</v>
       </c>
       <c r="Q201" t="n">
-        <v>-2.88409802090094</v>
+        <v>-1.96132467476084</v>
       </c>
       <c r="R201" t="n">
-        <v>-2.94116347984781</v>
+        <v>-2.01715721161747</v>
       </c>
       <c r="S201" t="n">
         <v>-1.94410953125794</v>

</xml_diff>

<commit_message>
correcciones en uto y disto
</commit_message>
<xml_diff>
--- a/03_ips_clean/00_ips_wide_norm_complete.xlsx
+++ b/03_ips_clean/00_ips_wide_norm_complete.xlsx
@@ -1049,7 +1049,7 @@
         <v>-0.27019013997832</v>
       </c>
       <c r="AW2" t="n">
-        <v>-1.31685283767894</v>
+        <v>-0.86845896678918</v>
       </c>
       <c r="AX2" t="n">
         <v>-0.421093375844313</v>
@@ -1061,7 +1061,7 @@
         <v>-0.322998232950349</v>
       </c>
       <c r="BA2" t="n">
-        <v>-0.235182389877304</v>
+        <v>-0.232865055298747</v>
       </c>
       <c r="BB2" t="n">
         <v>-0.230029511693985</v>
@@ -1225,7 +1225,7 @@
         <v>0.933520905271153</v>
       </c>
       <c r="AW3" t="n">
-        <v>-0.91557986472448</v>
+        <v>-0.544695702503086</v>
       </c>
       <c r="AX3" t="n">
         <v>-1.48018928185944</v>
@@ -1237,7 +1237,7 @@
         <v>-0.089007934221616</v>
       </c>
       <c r="BA3" t="n">
-        <v>1.40601737491567</v>
+        <v>1.41127832948073</v>
       </c>
       <c r="BB3" t="n">
         <v>0.0401013050719827</v>
@@ -1401,7 +1401,7 @@
         <v>-0.112561312624221</v>
       </c>
       <c r="AW4" t="n">
-        <v>-0.626533276356229</v>
+        <v>-0.311481224359092</v>
       </c>
       <c r="AX4" t="n">
         <v>-0.298495013354791</v>
@@ -1413,7 +1413,7 @@
         <v>0.887080528320713</v>
       </c>
       <c r="BA4" t="n">
-        <v>-0.354542372771339</v>
+        <v>-0.352439119646346</v>
       </c>
       <c r="BB4" t="n">
         <v>-0.025355367522779</v>
@@ -1577,7 +1577,7 @@
         <v>0.159706661896491</v>
       </c>
       <c r="AW5" t="n">
-        <v>-0.482009982172104</v>
+        <v>-0.194873985287095</v>
       </c>
       <c r="AX5" t="n">
         <v>0.0707890154062104</v>
@@ -1589,7 +1589,7 @@
         <v>0.272674457325076</v>
       </c>
       <c r="BA5" t="n">
-        <v>0.660017481827952</v>
+        <v>0.663940427308241</v>
       </c>
       <c r="BB5" t="n">
         <v>-0.180992123131013</v>
@@ -1753,7 +1753,7 @@
         <v>-0.857715769207228</v>
       </c>
       <c r="AW6" t="n">
-        <v>-1.50973131372437</v>
+        <v>-1.02408112233884</v>
       </c>
       <c r="AX6" t="n">
         <v>-2.58803472108311</v>
@@ -1765,7 +1765,7 @@
         <v>-0.810761768614631</v>
       </c>
       <c r="BA6" t="n">
-        <v>0.466057509625146</v>
+        <v>0.469632572743393</v>
       </c>
       <c r="BB6" t="n">
         <v>-0.278384513132874</v>
@@ -1929,7 +1929,7 @@
         <v>0.517953996792167</v>
       </c>
       <c r="AW7" t="n">
-        <v>0.577827893906935</v>
+        <v>0.660246078860188</v>
       </c>
       <c r="AX7" t="n">
         <v>-0.029927227732005</v>
@@ -1941,7 +1941,7 @@
         <v>-0.114050864018276</v>
       </c>
       <c r="BA7" t="n">
-        <v>0.0532709021166116</v>
+        <v>0.0561056002079489</v>
       </c>
       <c r="BB7" t="n">
         <v>-0.0389926117409979</v>
@@ -2075,7 +2075,7 @@
         <v>-0.930871283144079</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.424580335738454</v>
+        <v>0.424580335738455</v>
       </c>
       <c r="AN8" t="n">
         <v>-0.20239981194563</v>
@@ -2105,7 +2105,7 @@
         <v>0.546613783583822</v>
       </c>
       <c r="AW8" t="n">
-        <v>-1.14268839395083</v>
+        <v>-0.727936049412472</v>
       </c>
       <c r="AX8" t="n">
         <v>1.73255385071203</v>
@@ -2117,7 +2117,7 @@
         <v>0.291127142438405</v>
       </c>
       <c r="BA8" t="n">
-        <v>0.849004121410173</v>
+        <v>0.853266029191938</v>
       </c>
       <c r="BB8" t="n">
         <v>-0.0229092721395262</v>
@@ -2281,7 +2281,7 @@
         <v>-0.671427155061477</v>
       </c>
       <c r="AW9" t="n">
-        <v>0.0238215474723357</v>
+        <v>0.213251351464895</v>
       </c>
       <c r="AX9" t="n">
         <v>-1.28883373754431</v>
@@ -2293,7 +2293,7 @@
         <v>-2.01636160433239</v>
       </c>
       <c r="BA9" t="n">
-        <v>-2.27424876431705</v>
+        <v>-2.27558865457022</v>
       </c>
       <c r="BB9" t="n">
         <v>-1.69617499170907</v>
@@ -2457,7 +2457,7 @@
         <v>0.962180692062807</v>
       </c>
       <c r="AW10" t="n">
-        <v>0.0516139550371198</v>
+        <v>0.235675389967397</v>
       </c>
       <c r="AX10" t="n">
         <v>-0.946616534420768</v>
@@ -2469,7 +2469,7 @@
         <v>1.69188364988053</v>
       </c>
       <c r="BA10" t="n">
-        <v>0.510817503210409</v>
+        <v>0.514472846873743</v>
       </c>
       <c r="BB10" t="n">
         <v>0.241426503203457</v>
@@ -2633,7 +2633,7 @@
         <v>-0.0409118456450861</v>
       </c>
       <c r="AW11" t="n">
-        <v>-0.482009982172104</v>
+        <v>-0.194873985287095</v>
       </c>
       <c r="AX11" t="n">
         <v>1.09533350696566</v>
@@ -2645,7 +2645,7 @@
         <v>0.782686170874012</v>
       </c>
       <c r="BA11" t="n">
-        <v>0.0532709021166116</v>
+        <v>0.0561056002079489</v>
       </c>
       <c r="BB11" t="n">
         <v>3.18172763824401</v>
@@ -2809,7 +2809,7 @@
         <v>0.56094367697965</v>
       </c>
       <c r="AW12" t="n">
-        <v>-3.95056904259112</v>
+        <v>-2.99344772301502</v>
       </c>
       <c r="AX12" t="n">
         <v>0.403141982467375</v>
@@ -2821,7 +2821,7 @@
         <v>0.68521157034481</v>
       </c>
       <c r="BA12" t="n">
-        <v>-0.986155615585603</v>
+        <v>-0.985185210152387</v>
       </c>
       <c r="BB12" t="n">
         <v>-0.534384667298594</v>
@@ -2985,7 +2985,7 @@
         <v>0.102387088313184</v>
       </c>
       <c r="AW13" t="n">
-        <v>-3.5651739768289</v>
+        <v>-2.68249539644234</v>
       </c>
       <c r="AX13" t="n">
         <v>-0.78383005115421</v>
@@ -2997,7 +2997,7 @@
         <v>-2.33772146174255</v>
       </c>
       <c r="BA13" t="n">
-        <v>-0.21031572677438</v>
+        <v>-0.207953791892998</v>
       </c>
       <c r="BB13" t="n">
         <v>-1.20512921721871</v>
@@ -3161,7 +3161,7 @@
         <v>-1.33060225126952</v>
       </c>
       <c r="AW14" t="n">
-        <v>-2.92284771103885</v>
+        <v>-2.16424058596328</v>
       </c>
       <c r="AX14" t="n">
         <v>-0.940720592785103</v>
@@ -3173,7 +3173,7 @@
         <v>-2.11891313409912</v>
       </c>
       <c r="BA14" t="n">
-        <v>-1.52327553860876</v>
+        <v>-1.52326849971658</v>
       </c>
       <c r="BB14" t="n">
         <v>-1.41203949150422</v>
@@ -3337,7 +3337,7 @@
         <v>-0.65709726166565</v>
       </c>
       <c r="AW15" t="n">
-        <v>-0.867405047934321</v>
+        <v>-0.505826311859783</v>
       </c>
       <c r="AX15" t="n">
         <v>-1.51872228486052</v>
@@ -3349,7 +3349,7 @@
         <v>-1.32626535273301</v>
       </c>
       <c r="BA15" t="n">
-        <v>0.0134842411519336</v>
+        <v>0.0162475787587495</v>
       </c>
       <c r="BB15" t="n">
         <v>-0.0250824126731455</v>
@@ -3513,7 +3513,7 @@
         <v>0.388984956229725</v>
       </c>
       <c r="AW16" t="n">
-        <v>-2.02359140140733</v>
+        <v>-1.43868422443576</v>
       </c>
       <c r="AX16" t="n">
         <v>-0.413894610577768</v>
@@ -3525,7 +3525,7 @@
         <v>0.322540642095618</v>
       </c>
       <c r="BA16" t="n">
-        <v>-0.831982304347475</v>
+        <v>-0.830735377036739</v>
       </c>
       <c r="BB16" t="n">
         <v>-0.284053575394489</v>
@@ -3689,7 +3689,7 @@
         <v>-0.857715769207228</v>
       </c>
       <c r="AW17" t="n">
-        <v>-4.89653990564837</v>
+        <v>-3.75669527564226</v>
       </c>
       <c r="AX17" t="n">
         <v>-0.0485190527094064</v>
@@ -3701,7 +3701,7 @@
         <v>0.145922084582332</v>
       </c>
       <c r="BA17" t="n">
-        <v>-0.130742404845025</v>
+        <v>-0.128237748994599</v>
       </c>
       <c r="BB17" t="n">
         <v>-0.690682813504017</v>
@@ -3865,7 +3865,7 @@
         <v>0.345995276042245</v>
       </c>
       <c r="AW18" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX18" t="n">
         <v>0.2722148546233</v>
@@ -3877,7 +3877,7 @@
         <v>-1.03747838987806</v>
       </c>
       <c r="BA18" t="n">
-        <v>-0.593262338559407</v>
+        <v>-0.591587248341543</v>
       </c>
       <c r="BB18" t="n">
         <v>-1.01218163331829</v>
@@ -4041,7 +4041,7 @@
         <v>-0.843385875811401</v>
       </c>
       <c r="AW19" t="n">
-        <v>-2.79438268911811</v>
+        <v>-2.06058981043905</v>
       </c>
       <c r="AX19" t="n">
         <v>-1.73341565452269</v>
@@ -4053,7 +4053,7 @@
         <v>0.0573199060619862</v>
       </c>
       <c r="BA19" t="n">
-        <v>-0.707648988832856</v>
+        <v>-0.706179060007991</v>
       </c>
       <c r="BB19" t="n">
         <v>-0.223930020631025</v>
@@ -4217,7 +4217,7 @@
         <v>0.159706661896491</v>
       </c>
       <c r="AW20" t="n">
-        <v>0.509007057402808</v>
+        <v>0.604718644472016</v>
       </c>
       <c r="AX20" t="n">
         <v>0.624708411488371</v>
@@ -4229,7 +4229,7 @@
         <v>0.531951768986889</v>
       </c>
       <c r="BA20" t="n">
-        <v>-0.0213290871921598</v>
+        <v>-0.0186281900093001</v>
       </c>
       <c r="BB20" t="n">
         <v>-0.335274602754528</v>
@@ -4342,7 +4342,7 @@
         <v>-0.0233975024599997</v>
       </c>
       <c r="AF21" t="n">
-        <v>0.811860917151266</v>
+        <v>0.811860917151267</v>
       </c>
       <c r="AG21" t="n">
         <v>1.06779523188794</v>
@@ -4393,7 +4393,7 @@
         <v>0.618263250562957</v>
       </c>
       <c r="AW21" t="n">
-        <v>-0.0195354407829019</v>
+        <v>0.178269179743296</v>
       </c>
       <c r="AX21" t="n">
         <v>-0.172393650592444</v>
@@ -4405,7 +4405,7 @@
         <v>1.3300670126088</v>
       </c>
       <c r="BA21" t="n">
-        <v>-0.52363568187122</v>
+        <v>-0.521835710805443</v>
       </c>
       <c r="BB21" t="n">
         <v>0.370250693966941</v>
@@ -4569,7 +4569,7 @@
         <v>-1.45957129183196</v>
       </c>
       <c r="AW22" t="n">
-        <v>0.353013238405877</v>
+        <v>0.478856522049352</v>
       </c>
       <c r="AX22" t="n">
         <v>-0.651719746747396</v>
@@ -4581,7 +4581,7 @@
         <v>-2.97579139281408</v>
       </c>
       <c r="BA22" t="n">
-        <v>-1.38402222523238</v>
+        <v>-1.38376542464438</v>
       </c>
       <c r="BB22" t="n">
         <v>-1.3873370776124</v>
@@ -4745,7 +4745,7 @@
         <v>-1.20163321070708</v>
       </c>
       <c r="AW23" t="n">
-        <v>-0.659884627908512</v>
+        <v>-0.338390443705258</v>
       </c>
       <c r="AX23" t="n">
         <v>-0.574075446582567</v>
@@ -4757,7 +4757,7 @@
         <v>-1.12117449735637</v>
       </c>
       <c r="BA23" t="n">
-        <v>0.610284155622104</v>
+        <v>0.614117900496742</v>
       </c>
       <c r="BB23" t="n">
         <v>0.0972748478067178</v>
@@ -4852,7 +4852,7 @@
         <v>0.151295911614618</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.670401706181884</v>
+        <v>0.670401706181885</v>
       </c>
       <c r="AA24" t="n">
         <v>-0.426786682628269</v>
@@ -4921,7 +4921,7 @@
         <v>0.618263250562957</v>
       </c>
       <c r="AW24" t="n">
-        <v>0.585239048432697</v>
+        <v>0.6662256980798</v>
       </c>
       <c r="AX24" t="n">
         <v>0.0707890154062104</v>
@@ -4933,7 +4933,7 @@
         <v>-0.0577286802894332</v>
       </c>
       <c r="BA24" t="n">
-        <v>0.560550829416257</v>
+        <v>0.564295373685242</v>
       </c>
       <c r="BB24" t="n">
         <v>-0.211006658327232</v>
@@ -5097,7 +5097,7 @@
         <v>-0.972354916373844</v>
       </c>
       <c r="AW25" t="n">
-        <v>-0.225079938330626</v>
+        <v>0.0124275657613642</v>
       </c>
       <c r="AX25" t="n">
         <v>0.347752036976961</v>
@@ -5109,7 +5109,7 @@
         <v>-0.095427320709454</v>
       </c>
       <c r="BA25" t="n">
-        <v>-0.0760357460185918</v>
+        <v>-0.0734329695019491</v>
       </c>
       <c r="BB25" t="n">
         <v>-1.06442099223273</v>
@@ -5273,7 +5273,7 @@
         <v>-0.427818967332417</v>
       </c>
       <c r="AW26" t="n">
-        <v>-0.482009982172104</v>
+        <v>-0.194873985287095</v>
       </c>
       <c r="AX26" t="n">
         <v>0.440073044167211</v>
@@ -5285,7 +5285,7 @@
         <v>-0.0805504535446741</v>
       </c>
       <c r="BA26" t="n">
-        <v>-0.677808993109348</v>
+        <v>-0.676285543921092</v>
       </c>
       <c r="BB26" t="n">
         <v>-0.539749279920234</v>
@@ -5449,7 +5449,7 @@
         <v>0.360325169438071</v>
       </c>
       <c r="AW27" t="n">
-        <v>-0.570947305040308</v>
+        <v>-0.266632214496176</v>
       </c>
       <c r="AX27" t="n">
         <v>-2.14489521598177</v>
@@ -5461,7 +5461,7 @@
         <v>-1.11202137974063</v>
       </c>
       <c r="BA27" t="n">
-        <v>0.590390825139765</v>
+        <v>0.594188889772142</v>
       </c>
       <c r="BB27" t="n">
         <v>0.578158303279958</v>
@@ -5625,7 +5625,7 @@
         <v>0.116716981709011</v>
       </c>
       <c r="AW28" t="n">
-        <v>0.0516139550371198</v>
+        <v>0.235675389967397</v>
       </c>
       <c r="AX28" t="n">
         <v>-0.166604061906238</v>
@@ -5637,7 +5637,7 @@
         <v>0.409299992935996</v>
       </c>
       <c r="BA28" t="n">
-        <v>1.2319507331952</v>
+        <v>1.23689948564048</v>
       </c>
       <c r="BB28" t="n">
         <v>0.447769871262806</v>
@@ -5801,7 +5801,7 @@
         <v>-1.33060225126952</v>
       </c>
       <c r="AW29" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX29" t="n">
         <v>-1.59097581989961</v>
@@ -5813,7 +5813,7 @@
         <v>-0.478589028261079</v>
       </c>
       <c r="BA29" t="n">
-        <v>-0.23020905725672</v>
+        <v>-0.227882802617598</v>
       </c>
       <c r="BB29" t="n">
         <v>-0.198314257819282</v>
@@ -5977,7 +5977,7 @@
         <v>-0.27019013997832</v>
       </c>
       <c r="AW30" t="n">
-        <v>-0.289311871197818</v>
+        <v>-0.0393973555717942</v>
       </c>
       <c r="AX30" t="n">
         <v>-2.47073406488854</v>
@@ -5989,7 +5989,7 @@
         <v>1.342393210998</v>
       </c>
       <c r="BA30" t="n">
-        <v>0.232310876457663</v>
+        <v>0.235466696729347</v>
       </c>
       <c r="BB30" t="n">
         <v>0.17803798850784</v>
@@ -6153,7 +6153,7 @@
         <v>-0.485138540915725</v>
       </c>
       <c r="AW31" t="n">
-        <v>-1.14268839395083</v>
+        <v>-0.727936049412472</v>
       </c>
       <c r="AX31" t="n">
         <v>0.372931097761515</v>
@@ -6165,7 +6165,7 @@
         <v>0.851969169146741</v>
       </c>
       <c r="BA31" t="n">
-        <v>-0.916528958897416</v>
+        <v>-0.915433672616288</v>
       </c>
       <c r="BB31" t="n">
         <v>-0.889120989187447</v>
@@ -6329,7 +6329,7 @@
         <v>-0.485138540915725</v>
       </c>
       <c r="AW32" t="n">
-        <v>-1.83089444661939</v>
+        <v>-1.28320852757837</v>
       </c>
       <c r="AX32" t="n">
         <v>-1.60680246819107</v>
@@ -6341,7 +6341,7 @@
         <v>-1.14602216064389</v>
       </c>
       <c r="BA32" t="n">
-        <v>-0.613155669041745</v>
+        <v>-0.611516259066142</v>
       </c>
       <c r="BB32" t="n">
         <v>-0.856376905494895</v>
@@ -6505,7 +6505,7 @@
         <v>-0.542458114499033</v>
       </c>
       <c r="AW33" t="n">
-        <v>-0.225079938330626</v>
+        <v>0.0124275657613642</v>
       </c>
       <c r="AX33" t="n">
         <v>-2.64846313755417</v>
@@ -6517,7 +6517,7 @@
         <v>-0.633960148749031</v>
       </c>
       <c r="BA33" t="n">
-        <v>1.66960400380666</v>
+        <v>1.67533772158168</v>
       </c>
       <c r="BB33" t="n">
         <v>0.00324190210803601</v>
@@ -6681,7 +6681,7 @@
         <v>0.474964316604687</v>
       </c>
       <c r="AW34" t="n">
-        <v>-0.166686746548472</v>
+        <v>0.0595415546360138</v>
       </c>
       <c r="AX34" t="n">
         <v>-1.13776601989633</v>
@@ -6693,7 +6693,7 @@
         <v>-0.363027867323178</v>
       </c>
       <c r="BA34" t="n">
-        <v>0.545630831554503</v>
+        <v>0.549348615641793</v>
       </c>
       <c r="BB34" t="n">
         <v>-0.328167278400614</v>
@@ -6856,7 +6856,9 @@
       <c r="AV35" t="n">
         <v>0.116716981709011</v>
       </c>
-      <c r="AW35"/>
+      <c r="AW35" t="n">
+        <v>-0.86845896678918</v>
+      </c>
       <c r="AX35" t="n">
         <v>-0.421093375844313</v>
       </c>
@@ -6867,7 +6869,7 @@
         <v>-0.1671633545032</v>
       </c>
       <c r="BA35" t="n">
-        <v>-0.384382368494847</v>
+        <v>-0.382332635733245</v>
       </c>
       <c r="BB35" t="n">
         <v>-0.125676773026474</v>
@@ -6962,7 +6964,7 @@
         <v>0.638341786256426</v>
       </c>
       <c r="Z36" t="n">
-        <v>0.979830685993454</v>
+        <v>0.979830685993455</v>
       </c>
       <c r="AA36" t="n">
         <v>-0.208431277111013</v>
@@ -6980,7 +6982,7 @@
         <v>1.50225413447672</v>
       </c>
       <c r="AF36" t="n">
-        <v>0.906641102081318</v>
+        <v>0.906641102081319</v>
       </c>
       <c r="AG36" t="n">
         <v>-1.28973696994947</v>
@@ -7030,7 +7032,9 @@
       <c r="AV36" t="n">
         <v>0.646923037354612</v>
       </c>
-      <c r="AW36"/>
+      <c r="AW36" t="n">
+        <v>-0.544695702503086</v>
+      </c>
       <c r="AX36" t="n">
         <v>-1.48018928185944</v>
       </c>
@@ -7041,7 +7045,7 @@
         <v>0.419661322077012</v>
       </c>
       <c r="BA36" t="n">
-        <v>1.00815076526889</v>
+        <v>1.01269811498874</v>
       </c>
       <c r="BB36" t="n">
         <v>0.20706568694</v>
@@ -7204,7 +7208,9 @@
       <c r="AV37" t="n">
         <v>0.31733548925059</v>
       </c>
-      <c r="AW37"/>
+      <c r="AW37" t="n">
+        <v>-0.311481224359092</v>
+      </c>
       <c r="AX37" t="n">
         <v>-0.298495013354791</v>
       </c>
@@ -7215,7 +7221,7 @@
         <v>0.819188803925576</v>
       </c>
       <c r="BA37" t="n">
-        <v>-0.638022332144669</v>
+        <v>-0.636427522471892</v>
       </c>
       <c r="BB37" t="n">
         <v>0.200882209769461</v>
@@ -7378,7 +7384,9 @@
       <c r="AV38" t="n">
         <v>0.876201331687844</v>
       </c>
-      <c r="AW38"/>
+      <c r="AW38" t="n">
+        <v>-0.194873985287095</v>
+      </c>
       <c r="AX38" t="n">
         <v>0.0707890154062104</v>
       </c>
@@ -7389,7 +7397,7 @@
         <v>0.0602244953853806</v>
       </c>
       <c r="BA38" t="n">
-        <v>0.466057509625146</v>
+        <v>0.469632572743393</v>
       </c>
       <c r="BB38" t="n">
         <v>-0.0392445700637361</v>
@@ -7552,7 +7560,9 @@
       <c r="AV39" t="n">
         <v>-0.198540672999185</v>
       </c>
-      <c r="AW39"/>
+      <c r="AW39" t="n">
+        <v>-1.02408112233884</v>
+      </c>
       <c r="AX39" t="n">
         <v>-2.58803472108311</v>
       </c>
@@ -7563,7 +7573,7 @@
         <v>-0.728603384895764</v>
       </c>
       <c r="BA39" t="n">
-        <v>0.68985747755146</v>
+        <v>0.69383394339514</v>
       </c>
       <c r="BB39" t="n">
         <v>-0.219699220461709</v>
@@ -7726,7 +7736,9 @@
       <c r="AV40" t="n">
         <v>0.575273570375476</v>
       </c>
-      <c r="AW40"/>
+      <c r="AW40" t="n">
+        <v>0.660246078860188</v>
+      </c>
       <c r="AX40" t="n">
         <v>-0.029927227732005</v>
       </c>
@@ -7737,7 +7749,7 @@
         <v>1.02604926204126</v>
       </c>
       <c r="BA40" t="n">
-        <v>0.540657498933918</v>
+        <v>0.544366362960642</v>
       </c>
       <c r="BB40" t="n">
         <v>0.0850548691539024</v>
@@ -7832,7 +7844,7 @@
         <v>0.334964425028935</v>
       </c>
       <c r="Z41" t="n">
-        <v>0.720309606151492</v>
+        <v>0.720309606151493</v>
       </c>
       <c r="AA41" t="n">
         <v>0.253234437411183</v>
@@ -7871,7 +7883,7 @@
         <v>-0.957499020107757</v>
       </c>
       <c r="AM41" t="n">
-        <v>0.424580335738454</v>
+        <v>0.424580335738455</v>
       </c>
       <c r="AN41" t="n">
         <v>-0.20239981194563</v>
@@ -7900,7 +7912,9 @@
       <c r="AV41" t="n">
         <v>0.474964316604687</v>
       </c>
-      <c r="AW41"/>
+      <c r="AW41" t="n">
+        <v>-0.727936049412472</v>
+      </c>
       <c r="AX41" t="n">
         <v>1.73255385071203</v>
       </c>
@@ -7911,7 +7925,7 @@
         <v>-0.0521391764654224</v>
       </c>
       <c r="BA41" t="n">
-        <v>-0.309782379186076</v>
+        <v>-0.307598845515996</v>
       </c>
       <c r="BB41" t="n">
         <v>-0.071306266632205</v>
@@ -8074,7 +8088,9 @@
       <c r="AV42" t="n">
         <v>-0.212870566395011</v>
       </c>
-      <c r="AW42"/>
+      <c r="AW42" t="n">
+        <v>0.213251351464895</v>
+      </c>
       <c r="AX42" t="n">
         <v>-1.28883373754431</v>
       </c>
@@ -8085,7 +8101,7 @@
         <v>-2.25623430664884</v>
       </c>
       <c r="BA42" t="n">
-        <v>-2.33392875576407</v>
+        <v>-2.33537568674402</v>
       </c>
       <c r="BB42" t="n">
         <v>-1.6335948432989</v>
@@ -8248,7 +8264,9 @@
       <c r="AV43" t="n">
         <v>1.03383015904194</v>
       </c>
-      <c r="AW43"/>
+      <c r="AW43" t="n">
+        <v>0.235675389967397</v>
+      </c>
       <c r="AX43" t="n">
         <v>-0.946616534420768</v>
       </c>
@@ -8259,7 +8277,7 @@
         <v>0.555493587494568</v>
       </c>
       <c r="BA43" t="n">
-        <v>0.376537522454621</v>
+        <v>0.379952024482695</v>
       </c>
       <c r="BB43" t="n">
         <v>0.305066976221813</v>
@@ -8422,7 +8440,9 @@
       <c r="AV44" t="n">
         <v>0.761562184521228</v>
       </c>
-      <c r="AW44"/>
+      <c r="AW44" t="n">
+        <v>-0.194873985287095</v>
+      </c>
       <c r="AX44" t="n">
         <v>1.09533350696566</v>
       </c>
@@ -8433,7 +8453,7 @@
         <v>1.14688261872583</v>
       </c>
       <c r="BA44" t="n">
-        <v>1.04793742623356</v>
+        <v>1.05255613643794</v>
       </c>
       <c r="BB44" t="n">
         <v>3.28108320351055</v>
@@ -8596,7 +8616,9 @@
       <c r="AV45" t="n">
         <v>0.56094367697965</v>
       </c>
-      <c r="AW45"/>
+      <c r="AW45" t="n">
+        <v>-2.99344772301502</v>
+      </c>
       <c r="AX45" t="n">
         <v>0.403141982467375</v>
       </c>
@@ -8607,7 +8629,7 @@
         <v>0.968140537925691</v>
       </c>
       <c r="BA45" t="n">
-        <v>-1.11048893110022</v>
+        <v>-1.10974152718114</v>
       </c>
       <c r="BB45" t="n">
         <v>-0.435134084666537</v>
@@ -8770,7 +8792,9 @@
       <c r="AV46" t="n">
         <v>0.102387088313184</v>
       </c>
-      <c r="AW46"/>
+      <c r="AW46" t="n">
+        <v>-2.68249539644234</v>
+      </c>
       <c r="AX46" t="n">
         <v>-0.78383005115421</v>
       </c>
@@ -8781,7 +8805,7 @@
         <v>-0.919464193419139</v>
       </c>
       <c r="BA46" t="n">
-        <v>-0.797168976003382</v>
+        <v>-0.79585960826869</v>
       </c>
       <c r="BB46" t="n">
         <v>-1.05458411938248</v>
@@ -8944,7 +8968,9 @@
       <c r="AV47" t="n">
         <v>-1.01534459656133</v>
       </c>
-      <c r="AW47"/>
+      <c r="AW47" t="n">
+        <v>-2.16424058596328</v>
+      </c>
       <c r="AX47" t="n">
         <v>-0.940720592785103</v>
       </c>
@@ -8955,7 +8981,7 @@
         <v>-1.88497165199767</v>
       </c>
       <c r="BA47" t="n">
-        <v>-1.40391555571472</v>
+        <v>-1.40369443536898</v>
       </c>
       <c r="BB47" t="n">
         <v>-1.28393968091861</v>
@@ -9118,7 +9144,9 @@
       <c r="AV48" t="n">
         <v>-0.599777688082342</v>
       </c>
-      <c r="AW48"/>
+      <c r="AW48" t="n">
+        <v>-0.505826311859783</v>
+      </c>
       <c r="AX48" t="n">
         <v>-1.51872228486052</v>
       </c>
@@ -9129,7 +9157,7 @@
         <v>-0.977299692593783</v>
       </c>
       <c r="BA48" t="n">
-        <v>0.0482975694960271</v>
+        <v>0.0511233475267992</v>
       </c>
       <c r="BB48" t="n">
         <v>0.126302546238877</v>
@@ -9292,7 +9320,9 @@
       <c r="AV49" t="n">
         <v>0.603933357167131</v>
       </c>
-      <c r="AW49"/>
+      <c r="AW49" t="n">
+        <v>-1.43868422443576</v>
+      </c>
       <c r="AX49" t="n">
         <v>-0.413894610577768</v>
       </c>
@@ -9303,7 +9333,7 @@
         <v>0.286794666766955</v>
       </c>
       <c r="BA49" t="n">
-        <v>-1.32434223378537</v>
+        <v>-1.32397839247058</v>
       </c>
       <c r="BB49" t="n">
         <v>-0.244107682976997</v>
@@ -9398,7 +9428,7 @@
         <v>0.110684808151251</v>
       </c>
       <c r="Z50" t="n">
-        <v>0.720309606151492</v>
+        <v>0.720309606151493</v>
       </c>
       <c r="AA50" t="n">
         <v>-0.308250891061759</v>
@@ -9466,7 +9496,9 @@
       <c r="AV50" t="n">
         <v>-0.399159180540762</v>
       </c>
-      <c r="AW50"/>
+      <c r="AW50" t="n">
+        <v>-3.75669527564226</v>
+      </c>
       <c r="AX50" t="n">
         <v>-0.0485190527094064</v>
       </c>
@@ -9477,7 +9509,7 @@
         <v>0.688030730570458</v>
       </c>
       <c r="BA50" t="n">
-        <v>-0.155609067947948</v>
+        <v>-0.153149012400349</v>
       </c>
       <c r="BB50" t="n">
         <v>-0.591810168356067</v>
@@ -9641,7 +9673,7 @@
         <v>0.761562184521228</v>
       </c>
       <c r="AW51" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX51" t="n">
         <v>0.2722148546233</v>
@@ -9653,7 +9685,7 @@
         <v>-0.945044106115922</v>
       </c>
       <c r="BA51" t="n">
-        <v>-1.00604894606794</v>
+        <v>-1.00511422087699</v>
       </c>
       <c r="BB51" t="n">
         <v>-0.85135873556702</v>
@@ -9742,7 +9774,7 @@
         <v>0.839259893560454</v>
       </c>
       <c r="X52" t="n">
-        <v>0.696256592980103</v>
+        <v>0.696256592980104</v>
       </c>
       <c r="Y52" t="n">
         <v>0.148124612405577</v>
@@ -9817,7 +9849,7 @@
         <v>-0.370499393749109</v>
       </c>
       <c r="AW52" t="n">
-        <v>-2.79438268911811</v>
+        <v>-2.06058981043905</v>
       </c>
       <c r="AX52" t="n">
         <v>-1.73341565452269</v>
@@ -9829,7 +9861,7 @@
         <v>-0.328868432381243</v>
       </c>
       <c r="BA52" t="n">
-        <v>-0.090955743880346</v>
+        <v>-0.0883797275453988</v>
       </c>
       <c r="BB52" t="n">
         <v>-0.145707459684182</v>
@@ -9942,7 +9974,7 @@
         <v>0.441202379850438</v>
       </c>
       <c r="AF53" t="n">
-        <v>0.5195318049108</v>
+        <v>0.519531804910801</v>
       </c>
       <c r="AG53" t="n">
         <v>-0.519930536696439</v>
@@ -9993,7 +10025,7 @@
         <v>1.04816005243777</v>
       </c>
       <c r="AW53" t="n">
-        <v>0.509007057402808</v>
+        <v>0.604718644472016</v>
       </c>
       <c r="AX53" t="n">
         <v>0.624708411488371</v>
@@ -10005,7 +10037,7 @@
         <v>-0.135896304727838</v>
       </c>
       <c r="BA53" t="n">
-        <v>-0.125769072224439</v>
+        <v>-0.123255496313448</v>
       </c>
       <c r="BB53" t="n">
         <v>-0.358979681618838</v>
@@ -10169,7 +10201,7 @@
         <v>0.532283890187996</v>
       </c>
       <c r="AW54" t="n">
-        <v>-0.0195354407829019</v>
+        <v>0.178269179743296</v>
       </c>
       <c r="AX54" t="n">
         <v>-0.172393650592444</v>
@@ -10181,7 +10213,7 @@
         <v>0.0639589673726018</v>
       </c>
       <c r="BA54" t="n">
-        <v>-0.881715630553323</v>
+        <v>-0.880557903848239</v>
       </c>
       <c r="BB54" t="n">
         <v>0.494739101926634</v>
@@ -10345,7 +10377,7 @@
         <v>-0.685757048457303</v>
       </c>
       <c r="AW55" t="n">
-        <v>0.353013238405877</v>
+        <v>0.478856522049352</v>
       </c>
       <c r="AX55" t="n">
         <v>-0.651719746747396</v>
@@ -10357,7 +10389,7 @@
         <v>-2.27334453451186</v>
       </c>
       <c r="BA55" t="n">
-        <v>-1.59787552791753</v>
+        <v>-1.59800228993383</v>
       </c>
       <c r="BB55" t="n">
         <v>-1.29449043568328</v>
@@ -10521,7 +10553,7 @@
         <v>-0.585447794686514</v>
       </c>
       <c r="AW56" t="n">
-        <v>-0.659884627908512</v>
+        <v>-0.338390443705258</v>
       </c>
       <c r="AX56" t="n">
         <v>-0.574075446582567</v>
@@ -10533,7 +10565,7 @@
         <v>-1.0188914590397</v>
       </c>
       <c r="BA56" t="n">
-        <v>0.0781375652195353</v>
+        <v>0.0810168636136985</v>
       </c>
       <c r="BB56" t="n">
         <v>0.224881240010299</v>
@@ -10697,7 +10729,7 @@
         <v>0.331665382646416</v>
       </c>
       <c r="AW57" t="n">
-        <v>0.585239048432697</v>
+        <v>0.6662256980798</v>
       </c>
       <c r="AX57" t="n">
         <v>0.0707890154062104</v>
@@ -10709,7 +10741,7 @@
         <v>-0.322888395538961</v>
       </c>
       <c r="BA57" t="n">
-        <v>-0.250102387739058</v>
+        <v>-0.247811813342197</v>
       </c>
       <c r="BB57" t="n">
         <v>-0.0160539061083506</v>
@@ -10873,7 +10905,7 @@
         <v>-0.943695129582191</v>
       </c>
       <c r="AW58" t="n">
-        <v>0.358853135677269</v>
+        <v>0.483568387365774</v>
       </c>
       <c r="AX58" t="n">
         <v>0.347752036976961</v>
@@ -10885,7 +10917,7 @@
         <v>0.443398407093826</v>
       </c>
       <c r="BA58" t="n">
-        <v>-0.53358234711239</v>
+        <v>-0.531800216167743</v>
       </c>
       <c r="BB58" t="n">
         <v>-0.982775997402021</v>
@@ -11049,7 +11081,7 @@
         <v>0.231356128875627</v>
       </c>
       <c r="AW59" t="n">
-        <v>-0.482009982172104</v>
+        <v>-0.194873985287095</v>
       </c>
       <c r="AX59" t="n">
         <v>0.440073044167211</v>
@@ -11061,7 +11093,7 @@
         <v>-0.869659029432702</v>
       </c>
       <c r="BA59" t="n">
-        <v>-0.846902302209229</v>
+        <v>-0.845682135080189</v>
       </c>
       <c r="BB59" t="n">
         <v>-0.452676682887202</v>
@@ -11225,7 +11257,7 @@
         <v>1.13413941281273</v>
       </c>
       <c r="AW60" t="n">
-        <v>0.417246327459423</v>
+        <v>0.530682376240423</v>
       </c>
       <c r="AX60" t="n">
         <v>-2.14489521598177</v>
@@ -11237,7 +11269,7 @@
         <v>0.200230582435713</v>
       </c>
       <c r="BA60" t="n">
-        <v>0.436217513901638</v>
+        <v>0.439739056656494</v>
       </c>
       <c r="BB60" t="n">
         <v>0.770790939276956</v>
@@ -11401,7 +11433,7 @@
         <v>0.360325169438071</v>
       </c>
       <c r="AW61" t="n">
-        <v>0.0516139550371198</v>
+        <v>0.235675389967397</v>
       </c>
       <c r="AX61" t="n">
         <v>-0.166604061906238</v>
@@ -11413,7 +11445,7 @@
         <v>0.581610483091474</v>
       </c>
       <c r="BA61" t="n">
-        <v>0.973337436924792</v>
+        <v>0.977822346220687</v>
       </c>
       <c r="BB61" t="n">
         <v>0.542632179773835</v>
@@ -11577,7 +11609,7 @@
         <v>-0.485138540915725</v>
       </c>
       <c r="AW62" t="n">
-        <v>-0.126260690699288</v>
+        <v>0.0921589315492328</v>
       </c>
       <c r="AX62" t="n">
         <v>-1.59097581989961</v>
@@ -11589,7 +11621,7 @@
         <v>-0.261318424377095</v>
       </c>
       <c r="BA62" t="n">
-        <v>-0.717595654074026</v>
+        <v>-0.716143565370291</v>
       </c>
       <c r="BB62" t="n">
         <v>-0.127335498651169</v>
@@ -11753,7 +11785,7 @@
         <v>0.589603463771303</v>
       </c>
       <c r="AW63" t="n">
-        <v>0.38512978293265</v>
+        <v>0.504769449144888</v>
       </c>
       <c r="AX63" t="n">
         <v>-2.47073406488854</v>
@@ -11765,7 +11797,7 @@
         <v>0.237245790073758</v>
       </c>
       <c r="BA63" t="n">
-        <v>0.560550829416257</v>
+        <v>0.564295373685242</v>
       </c>
       <c r="BB63" t="n">
         <v>0.258192229929012</v>
@@ -11929,7 +11961,7 @@
         <v>-0.0122520588534316</v>
       </c>
       <c r="AW64" t="n">
-        <v>-1.14268839395083</v>
+        <v>-0.727936049412472</v>
       </c>
       <c r="AX64" t="n">
         <v>0.372931097761515</v>
@@ -11941,7 +11973,7 @@
         <v>-0.151908158476969</v>
       </c>
       <c r="BA64" t="n">
-        <v>-0.384382368494847</v>
+        <v>-0.382332635733245</v>
       </c>
       <c r="BB64" t="n">
         <v>-0.715332736078596</v>
@@ -12105,7 +12137,7 @@
         <v>-0.313179820165801</v>
       </c>
       <c r="AW65" t="n">
-        <v>-0.0560466496392259</v>
+        <v>0.148810459722059</v>
       </c>
       <c r="AX65" t="n">
         <v>-1.60680246819107</v>
@@ -12117,7 +12149,7 @@
         <v>-0.622903182669219</v>
       </c>
       <c r="BA65" t="n">
-        <v>-1.03588894179145</v>
+        <v>-1.03500773696389</v>
       </c>
       <c r="BB65" t="n">
         <v>-0.764748062125676</v>
@@ -12281,7 +12313,7 @@
         <v>0.17403655529232</v>
       </c>
       <c r="AW66" t="n">
-        <v>-0.225079938330626</v>
+        <v>0.0124275657613642</v>
       </c>
       <c r="AX66" t="n">
         <v>-2.64846313755417</v>
@@ -12293,7 +12325,7 @@
         <v>-0.602741915600953</v>
       </c>
       <c r="BA66" t="n">
-        <v>0.863924119271927</v>
+        <v>0.868212787235388</v>
       </c>
       <c r="BB66" t="n">
         <v>0.0954691464937586</v>
@@ -12457,7 +12489,7 @@
         <v>0.962180692062807</v>
       </c>
       <c r="AW67" t="n">
-        <v>0.529653077116775</v>
+        <v>0.621376688216885</v>
       </c>
       <c r="AX67" t="n">
         <v>-1.13776601989633</v>
@@ -12469,7 +12501,7 @@
         <v>-0.140729150828948</v>
       </c>
       <c r="BA67" t="n">
-        <v>0.0234309063931033</v>
+        <v>0.0262120841210496</v>
       </c>
       <c r="BB67" t="n">
         <v>-0.172016107883456</v>
@@ -12632,7 +12664,9 @@
       <c r="AV68" t="n">
         <v>-0.27019013997832</v>
       </c>
-      <c r="AW68"/>
+      <c r="AW68" t="n">
+        <v>-0.86845896678918</v>
+      </c>
       <c r="AX68" t="n">
         <v>0.11067137145355</v>
       </c>
@@ -12643,7 +12677,7 @@
         <v>-0.1671633545032</v>
       </c>
       <c r="BA68" t="n">
-        <v>-0.334649042288999</v>
+        <v>-0.332510108921746</v>
       </c>
       <c r="BB68" t="n">
         <v>-0.0312763881071327</v>
@@ -12738,7 +12772,7 @@
         <v>0.0324389014530642</v>
       </c>
       <c r="Z69" t="n">
-        <v>0.810852518276355</v>
+        <v>0.810852518276356</v>
       </c>
       <c r="AA69" t="n">
         <v>0.150881900756438</v>
@@ -12806,7 +12840,9 @@
       <c r="AV69" t="n">
         <v>0.0164077279382209</v>
       </c>
-      <c r="AW69"/>
+      <c r="AW69" t="n">
+        <v>-0.544695702503086</v>
+      </c>
       <c r="AX69" t="n">
         <v>0.977208615412783</v>
       </c>
@@ -12817,7 +12853,7 @@
         <v>0.419661322077012</v>
       </c>
       <c r="BA69" t="n">
-        <v>1.03301742837181</v>
+        <v>1.03760937839449</v>
       </c>
       <c r="BB69" t="n">
         <v>0.425650030179059</v>
@@ -12980,7 +13016,9 @@
       <c r="AV70" t="n">
         <v>0.331665382646416</v>
       </c>
-      <c r="AW70"/>
+      <c r="AW70" t="n">
+        <v>-0.311481224359092</v>
+      </c>
       <c r="AX70" t="n">
         <v>0.545581817090449</v>
       </c>
@@ -12991,7 +13029,7 @@
         <v>0.819188803925576</v>
       </c>
       <c r="BA70" t="n">
-        <v>-0.558449010215313</v>
+        <v>-0.556711479573493</v>
       </c>
       <c r="BB70" t="n">
         <v>0.250664975037201</v>
@@ -13154,7 +13192,9 @@
       <c r="AV71" t="n">
         <v>0.704242610937921</v>
       </c>
-      <c r="AW71"/>
+      <c r="AW71" t="n">
+        <v>-0.194873985287095</v>
+      </c>
       <c r="AX71" t="n">
         <v>0.229055498320737</v>
       </c>
@@ -13165,7 +13205,7 @@
         <v>0.0602244953853806</v>
       </c>
       <c r="BA71" t="n">
-        <v>0.351670859351697</v>
+        <v>0.355040761076945</v>
       </c>
       <c r="BB71" t="n">
         <v>-0.00194424003499707</v>
@@ -13328,7 +13368,9 @@
       <c r="AV72" t="n">
         <v>-0.485138540915725</v>
       </c>
-      <c r="AW72"/>
+      <c r="AW72" t="n">
+        <v>-1.02408112233884</v>
+      </c>
       <c r="AX72" t="n">
         <v>-0.593916918716119</v>
       </c>
@@ -13339,7 +13381,7 @@
         <v>-0.728603384895764</v>
       </c>
       <c r="BA72" t="n">
-        <v>0.40637751817813</v>
+        <v>0.409845540569595</v>
       </c>
       <c r="BB72" t="n">
         <v>-0.187123108984316</v>
@@ -13502,7 +13544,9 @@
       <c r="AV73" t="n">
         <v>0.188366448688146</v>
       </c>
-      <c r="AW73"/>
+      <c r="AW73" t="n">
+        <v>0.660246078860188</v>
+      </c>
       <c r="AX73" t="n">
         <v>0.0707890154062104</v>
       </c>
@@ -13513,7 +13557,7 @@
         <v>1.02604926204126</v>
       </c>
       <c r="BA73" t="n">
-        <v>0.227337543837078</v>
+        <v>0.230484444048197</v>
       </c>
       <c r="BB73" t="n">
         <v>0.157818333108079</v>
@@ -13602,7 +13646,7 @@
         <v>-0.149119952415086</v>
       </c>
       <c r="X74" t="n">
-        <v>-0.246060022294722</v>
+        <v>-0.246060022294723</v>
       </c>
       <c r="Y74" t="n">
         <v>0.358282197853998</v>
@@ -13647,7 +13691,7 @@
         <v>-1.01380605226383</v>
       </c>
       <c r="AM74" t="n">
-        <v>0.424580335738454</v>
+        <v>0.424580335738455</v>
       </c>
       <c r="AN74" t="n">
         <v>-0.518259888082547</v>
@@ -13676,7 +13720,9 @@
       <c r="AV74" t="n">
         <v>0.489294210000515</v>
       </c>
-      <c r="AW74"/>
+      <c r="AW74" t="n">
+        <v>-0.727936049412472</v>
+      </c>
       <c r="AX74" t="n">
         <v>1.17863445462987</v>
       </c>
@@ -13687,7 +13733,7 @@
         <v>-0.0521391764654224</v>
       </c>
       <c r="BA74" t="n">
-        <v>-0.473902355665372</v>
+        <v>-0.472013183993944</v>
       </c>
       <c r="BB74" t="n">
         <v>-0.136080552102883</v>
@@ -13850,7 +13896,9 @@
       <c r="AV75" t="n">
         <v>-0.198540672999185</v>
       </c>
-      <c r="AW75"/>
+      <c r="AW75" t="n">
+        <v>0.213251351464895</v>
+      </c>
       <c r="AX75" t="n">
         <v>-0.707056515763081</v>
       </c>
@@ -13861,7 +13909,7 @@
         <v>-2.25623430664884</v>
       </c>
       <c r="BA75" t="n">
-        <v>-2.23943543597296</v>
+        <v>-2.24071288580217</v>
       </c>
       <c r="BB75" t="n">
         <v>-1.60358030810268</v>
@@ -14024,7 +14072,9 @@
       <c r="AV76" t="n">
         <v>0.790221971312882</v>
       </c>
-      <c r="AW76"/>
+      <c r="AW76" t="n">
+        <v>0.235675389967397</v>
+      </c>
       <c r="AX76" t="n">
         <v>-0.00306646093412165</v>
       </c>
@@ -14035,7 +14085,7 @@
         <v>0.555493587494568</v>
       </c>
       <c r="BA76" t="n">
-        <v>0.371564189834036</v>
+        <v>0.374969771801545</v>
       </c>
       <c r="BB76" t="n">
         <v>0.428054132508522</v>
@@ -14198,7 +14248,9 @@
       <c r="AV77" t="n">
         <v>0.0450675147298754</v>
       </c>
-      <c r="AW77"/>
+      <c r="AW77" t="n">
+        <v>-0.194873985287095</v>
+      </c>
       <c r="AX77" t="n">
         <v>0.913376904559016</v>
       </c>
@@ -14209,7 +14261,7 @@
         <v>1.14688261872583</v>
       </c>
       <c r="BA77" t="n">
-        <v>1.19216407223052</v>
+        <v>1.19704146419128</v>
       </c>
       <c r="BB77" t="n">
         <v>3.64831245890185</v>
@@ -14372,7 +14424,9 @@
       <c r="AV78" t="n">
         <v>0.46063442320886</v>
       </c>
-      <c r="AW78"/>
+      <c r="AW78" t="n">
+        <v>-2.99344772301502</v>
+      </c>
       <c r="AX78" t="n">
         <v>-0.48313038067595</v>
       </c>
@@ -14383,7 +14437,7 @@
         <v>0.968140537925691</v>
       </c>
       <c r="BA78" t="n">
-        <v>-0.881715630553323</v>
+        <v>-0.880557903848239</v>
       </c>
       <c r="BB78" t="n">
         <v>-0.351210966667736</v>
@@ -14546,7 +14600,9 @@
       <c r="AV79" t="n">
         <v>0.646923037354612</v>
       </c>
-      <c r="AW79"/>
+      <c r="AW79" t="n">
+        <v>-2.68249539644234</v>
+      </c>
       <c r="AX79" t="n">
         <v>-0.11912411703188</v>
       </c>
@@ -14557,7 +14613,7 @@
         <v>-0.919464193419139</v>
       </c>
       <c r="BA79" t="n">
-        <v>-0.787222310762212</v>
+        <v>-0.78589510290639</v>
       </c>
       <c r="BB79" t="n">
         <v>-0.851778666104918</v>
@@ -14720,7 +14776,9 @@
       <c r="AV80" t="n">
         <v>-0.929365236186363</v>
       </c>
-      <c r="AW80"/>
+      <c r="AW80" t="n">
+        <v>-2.16424058596328</v>
+      </c>
       <c r="AX80" t="n">
         <v>0.0000775981342769585</v>
       </c>
@@ -14731,7 +14789,7 @@
         <v>-1.88497165199767</v>
       </c>
       <c r="BA80" t="n">
-        <v>-1.4437022166794</v>
+        <v>-1.44355245681818</v>
       </c>
       <c r="BB80" t="n">
         <v>-1.20061496393631</v>
@@ -14820,13 +14878,13 @@
         <v>0.938392535955357</v>
       </c>
       <c r="X81" t="n">
-        <v>-0.246060022294722</v>
+        <v>-0.246060022294723</v>
       </c>
       <c r="Y81" t="n">
         <v>-0.69114073652467</v>
       </c>
       <c r="Z81" t="n">
-        <v>-0.568761542163513</v>
+        <v>-0.568761542163514</v>
       </c>
       <c r="AA81" t="n">
         <v>-1.07185222160734</v>
@@ -14894,7 +14952,9 @@
       <c r="AV81" t="n">
         <v>-1.11565385033211</v>
       </c>
-      <c r="AW81"/>
+      <c r="AW81" t="n">
+        <v>-0.505826311859783</v>
+      </c>
       <c r="AX81" t="n">
         <v>-0.651719746747396</v>
       </c>
@@ -14905,7 +14965,7 @@
         <v>-0.977299692593783</v>
       </c>
       <c r="BA81" t="n">
-        <v>0.137817556666553</v>
+        <v>0.140803895787498</v>
       </c>
       <c r="BB81" t="n">
         <v>0.251210884736468</v>
@@ -15068,7 +15128,9 @@
       <c r="AV82" t="n">
         <v>0.675582824146266</v>
       </c>
-      <c r="AW82"/>
+      <c r="AW82" t="n">
+        <v>-1.43868422443576</v>
+      </c>
       <c r="AX82" t="n">
         <v>-0.393787256070568</v>
       </c>
@@ -15079,7 +15141,7 @@
         <v>0.286794666766955</v>
       </c>
       <c r="BA82" t="n">
-        <v>-1.22487558137367</v>
+        <v>-1.22433333884758</v>
       </c>
       <c r="BB82" t="n">
         <v>-0.224559916437871</v>
@@ -15242,7 +15304,9 @@
       <c r="AV83" t="n">
         <v>-0.470808647519897</v>
       </c>
-      <c r="AW83"/>
+      <c r="AW83" t="n">
+        <v>-3.75669527564226</v>
+      </c>
       <c r="AX83" t="n">
         <v>0.473640693840389</v>
       </c>
@@ -15253,7 +15317,7 @@
         <v>0.688030730570458</v>
       </c>
       <c r="BA83" t="n">
-        <v>-0.120795739603855</v>
+        <v>-0.118273243632299</v>
       </c>
       <c r="BB83" t="n">
         <v>-0.481021994195278</v>
@@ -15417,7 +15481,7 @@
         <v>1.04816005243777</v>
       </c>
       <c r="AW84" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX84" t="n">
         <v>-0.574075446582567</v>
@@ -15429,7 +15493,7 @@
         <v>-0.945044106115922</v>
       </c>
       <c r="BA84" t="n">
-        <v>-0.563422342835898</v>
+        <v>-0.561693732254643</v>
       </c>
       <c r="BB84" t="n">
         <v>-0.824745637727771</v>
@@ -15542,7 +15606,7 @@
         <v>-0.0857491358744569</v>
       </c>
       <c r="AF85" t="n">
-        <v>-0.991294457660341</v>
+        <v>-0.991294457660342</v>
       </c>
       <c r="AG85" t="n">
         <v>-0.904833753322954</v>
@@ -15593,7 +15657,7 @@
         <v>-0.642767368269822</v>
       </c>
       <c r="AW85" t="n">
-        <v>-2.79438268911811</v>
+        <v>-2.06058981043905</v>
       </c>
       <c r="AX85" t="n">
         <v>-0.320217603281908</v>
@@ -15605,7 +15669,7 @@
         <v>-0.328868432381243</v>
       </c>
       <c r="BA85" t="n">
-        <v>-0.667862327868178</v>
+        <v>-0.666321038558792</v>
       </c>
       <c r="BB85" t="n">
         <v>0.0335398904173353</v>
@@ -15769,7 +15833,7 @@
         <v>0.575273570375476</v>
       </c>
       <c r="AW86" t="n">
-        <v>-0.166686746548472</v>
+        <v>0.0595415546360138</v>
       </c>
       <c r="AX86" t="n">
         <v>1.17863445462987</v>
@@ -15781,7 +15845,7 @@
         <v>-0.135896304727838</v>
       </c>
       <c r="BA86" t="n">
-        <v>-1.51332887336759</v>
+        <v>-1.51330399435428</v>
       </c>
       <c r="BB86" t="n">
         <v>-0.284599485093756</v>
@@ -15945,7 +16009,7 @@
         <v>0.56094367697965</v>
       </c>
       <c r="AW87" t="n">
-        <v>-0.0195354407829019</v>
+        <v>0.178269179743296</v>
       </c>
       <c r="AX87" t="n">
         <v>0.347752036976961</v>
@@ -15957,7 +16021,7 @@
         <v>0.0639589673726018</v>
       </c>
       <c r="BA87" t="n">
-        <v>0.326804196248773</v>
+        <v>0.330129497671195</v>
       </c>
       <c r="BB87" t="n">
         <v>0.609128180449893</v>
@@ -16121,7 +16185,7 @@
         <v>-0.771736408832266</v>
       </c>
       <c r="AW88" t="n">
-        <v>0.353013238405877</v>
+        <v>0.478856522049352</v>
       </c>
       <c r="AX88" t="n">
         <v>-0.507219323728544</v>
@@ -16133,7 +16197,7 @@
         <v>-2.27334453451186</v>
       </c>
       <c r="BA88" t="n">
-        <v>-0.0263024198127443</v>
+        <v>-0.0236104426904498</v>
       </c>
       <c r="BB88" t="n">
         <v>-1.33815271336117</v>
@@ -16297,7 +16361,7 @@
         <v>-0.585447794686514</v>
       </c>
       <c r="AW89" t="n">
-        <v>-0.659884627908512</v>
+        <v>-0.338390443705258</v>
       </c>
       <c r="AX89" t="n">
         <v>-0.0696434072958139</v>
@@ -16309,7 +16373,7 @@
         <v>-1.0188914590397</v>
       </c>
       <c r="BA89" t="n">
-        <v>0.326804196248773</v>
+        <v>0.330129497671195</v>
       </c>
       <c r="BB89" t="n">
         <v>0.386638483208388</v>
@@ -16473,7 +16537,7 @@
         <v>0.116716981709011</v>
       </c>
       <c r="AW90" t="n">
-        <v>0.585239048432697</v>
+        <v>0.6662256980798</v>
       </c>
       <c r="AX90" t="n">
         <v>0.624708411488371</v>
@@ -16485,7 +16549,7 @@
         <v>-0.322888395538961</v>
       </c>
       <c r="BA90" t="n">
-        <v>-0.0263024198127443</v>
+        <v>-0.0236104426904498</v>
       </c>
       <c r="BB90" t="n">
         <v>0.102838927433858</v>
@@ -16649,7 +16713,7 @@
         <v>-0.70008694185313</v>
       </c>
       <c r="AW91" t="n">
-        <v>0.358853135677269</v>
+        <v>0.483568387365774</v>
       </c>
       <c r="AX91" t="n">
         <v>0.624708411488371</v>
@@ -16661,7 +16725,7 @@
         <v>0.443398407093826</v>
       </c>
       <c r="BA91" t="n">
-        <v>-0.279942383462567</v>
+        <v>-0.277705329429097</v>
       </c>
       <c r="BB91" t="n">
         <v>-0.965800305407517</v>
@@ -16825,7 +16889,7 @@
         <v>0.489294210000515</v>
       </c>
       <c r="AW92" t="n">
-        <v>-0.482009982172104</v>
+        <v>-0.194873985287095</v>
       </c>
       <c r="AX92" t="n">
         <v>0.0707890154062104</v>
@@ -16837,7 +16901,7 @@
         <v>-0.869659029432702</v>
       </c>
       <c r="BA92" t="n">
-        <v>-0.807115641244551</v>
+        <v>-0.80582411363099</v>
       </c>
       <c r="BB92" t="n">
         <v>-0.390684437230094</v>
@@ -17001,7 +17065,7 @@
         <v>0.517953996792167</v>
       </c>
       <c r="AW93" t="n">
-        <v>0.417246327459423</v>
+        <v>0.530682376240423</v>
       </c>
       <c r="AX93" t="n">
         <v>1.24380222441123</v>
@@ -17013,7 +17077,7 @@
         <v>0.200230582435713</v>
       </c>
       <c r="BA93" t="n">
-        <v>0.90868411285719</v>
+        <v>0.913053061365738</v>
       </c>
       <c r="BB93" t="n">
         <v>0.893820088617455</v>
@@ -17177,7 +17241,7 @@
         <v>-0.0409118456450861</v>
       </c>
       <c r="AW94" t="n">
-        <v>0.0516139550371198</v>
+        <v>0.235675389967397</v>
       </c>
       <c r="AX94" t="n">
         <v>0.852795605723107</v>
@@ -17189,7 +17253,7 @@
         <v>0.581610483091474</v>
       </c>
       <c r="BA94" t="n">
-        <v>1.11756408292175</v>
+        <v>1.12230767397404</v>
       </c>
       <c r="BB94" t="n">
         <v>0.58301899925612</v>
@@ -17353,7 +17417,7 @@
         <v>-0.614107581478168</v>
       </c>
       <c r="AW95" t="n">
-        <v>-0.126260690699288</v>
+        <v>0.0921589315492328</v>
       </c>
       <c r="AX95" t="n">
         <v>-1.29772085588352</v>
@@ -17365,7 +17429,7 @@
         <v>-0.261318424377095</v>
       </c>
       <c r="BA95" t="n">
-        <v>-0.886688963173907</v>
+        <v>-0.885540156529389</v>
       </c>
       <c r="BB95" t="n">
         <v>-0.162473186409736</v>
@@ -17454,7 +17518,7 @@
         <v>-0.94032305832988</v>
       </c>
       <c r="X96" t="n">
-        <v>0.574460567876554</v>
+        <v>0.574460567876555</v>
       </c>
       <c r="Y96" t="n">
         <v>0.359513770362364</v>
@@ -17529,7 +17593,7 @@
         <v>0.431974636417206</v>
       </c>
       <c r="AW96" t="n">
-        <v>0.38512978293265</v>
+        <v>0.504769449144888</v>
       </c>
       <c r="AX96" t="n">
         <v>-0.298495013354791</v>
@@ -17541,7 +17605,7 @@
         <v>0.237245790073758</v>
       </c>
       <c r="BA96" t="n">
-        <v>0.704777475413215</v>
+        <v>0.708780701438591</v>
       </c>
       <c r="BB96" t="n">
         <v>0.275535361144176</v>
@@ -17636,7 +17700,7 @@
         <v>-0.907076449658175</v>
       </c>
       <c r="Z97" t="n">
-        <v>-0.837605417719798</v>
+        <v>-0.837605417719799</v>
       </c>
       <c r="AA97" t="n">
         <v>-1.40955445305446</v>
@@ -17705,7 +17769,7 @@
         <v>-0.198540672999185</v>
       </c>
       <c r="AW97" t="n">
-        <v>-1.14268839395083</v>
+        <v>-0.727936049412472</v>
       </c>
       <c r="AX97" t="n">
         <v>0.372931097761515</v>
@@ -17717,7 +17781,7 @@
         <v>-0.151908158476969</v>
       </c>
       <c r="BA97" t="n">
-        <v>-0.822035639106305</v>
+        <v>-0.820770871674439</v>
       </c>
       <c r="BB97" t="n">
         <v>-0.587715845611568</v>
@@ -17881,7 +17945,7 @@
         <v>-0.456478754124071</v>
       </c>
       <c r="AW98" t="n">
-        <v>-0.0560466496392259</v>
+        <v>0.148810459722059</v>
       </c>
       <c r="AX98" t="n">
         <v>-0.0937389974077486</v>
@@ -17893,7 +17957,7 @@
         <v>-0.622903182669219</v>
       </c>
       <c r="BA98" t="n">
-        <v>-1.508355540747</v>
+        <v>-1.50832174167313</v>
       </c>
       <c r="BB98" t="n">
         <v>-0.734534059923956</v>
@@ -18057,7 +18121,7 @@
         <v>0.0737273015215299</v>
       </c>
       <c r="AW99" t="n">
-        <v>-0.225079938330626</v>
+        <v>0.0124275657613642</v>
       </c>
       <c r="AX99" t="n">
         <v>-1.43990810225163</v>
@@ -18069,7 +18133,7 @@
         <v>-0.602741915600953</v>
       </c>
       <c r="BA99" t="n">
-        <v>0.799270795204325</v>
+        <v>0.803443502380439</v>
       </c>
       <c r="BB99" t="n">
         <v>0.132821967839735</v>
@@ -18233,7 +18297,7 @@
         <v>1.10547962602108</v>
       </c>
       <c r="AW100" t="n">
-        <v>0.529653077116775</v>
+        <v>0.621376688216885</v>
       </c>
       <c r="AX100" t="n">
         <v>0.901671433059122</v>
@@ -18245,7 +18309,7 @@
         <v>-0.140729150828948</v>
       </c>
       <c r="BA100" t="n">
-        <v>0.0532709021166116</v>
+        <v>0.0561056002079489</v>
       </c>
       <c r="BB100" t="n">
         <v>-0.0942239757379571</v>
@@ -18409,7 +18473,7 @@
         <v>0.0164077279382209</v>
       </c>
       <c r="AW101" t="n">
-        <v>0.665659902621219</v>
+        <v>0.731112495904847</v>
       </c>
       <c r="AX101" t="n">
         <v>0.11067137145355</v>
@@ -18421,7 +18485,7 @@
         <v>0.0387695876940898</v>
       </c>
       <c r="BA101" t="n">
-        <v>1.27173739415988</v>
+        <v>1.27675750708968</v>
       </c>
       <c r="BB101" t="n">
         <v>0.119394688890465</v>
@@ -18585,7 +18649,7 @@
         <v>0.345995276042245</v>
       </c>
       <c r="AW102" t="n">
-        <v>0.591591136258678</v>
+        <v>0.671350819451493</v>
       </c>
       <c r="AX102" t="n">
         <v>0.977208615412783</v>
@@ -18597,7 +18661,7 @@
         <v>0.669870945220833</v>
       </c>
       <c r="BA102" t="n">
-        <v>1.4607240337421</v>
+        <v>1.46608310897338</v>
       </c>
       <c r="BB102" t="n">
         <v>0.609044194342313</v>
@@ -18761,7 +18825,7 @@
         <v>0.403314849625552</v>
       </c>
       <c r="AW103" t="n">
-        <v>0.577827893906935</v>
+        <v>0.660246078860188</v>
       </c>
       <c r="AX103" t="n">
         <v>0.545581817090449</v>
@@ -18773,7 +18837,7 @@
         <v>0.789837806771109</v>
       </c>
       <c r="BA103" t="n">
-        <v>1.69944399953017</v>
+        <v>1.70523123766858</v>
       </c>
       <c r="BB103" t="n">
         <v>0.397588171984064</v>
@@ -18937,7 +19001,7 @@
         <v>1.0624899458336</v>
       </c>
       <c r="AW104" t="n">
-        <v>0.229489756959881</v>
+        <v>0.379192781243473</v>
       </c>
       <c r="AX104" t="n">
         <v>0.229055498320737</v>
@@ -18949,7 +19013,7 @@
         <v>1.02492647961373</v>
       </c>
       <c r="BA104" t="n">
-        <v>1.46569736636268</v>
+        <v>1.47106536165453</v>
       </c>
       <c r="BB104" t="n">
         <v>0.225574125397829</v>
@@ -19044,7 +19108,7 @@
         <v>-0.133063917462853</v>
       </c>
       <c r="Z105" t="n">
-        <v>-0.00576050418635905</v>
+        <v>-0.00576050418635906</v>
       </c>
       <c r="AA105" t="n">
         <v>0.0662723004814374</v>
@@ -19113,7 +19177,7 @@
         <v>-0.80039619562392</v>
       </c>
       <c r="AW105" t="n">
-        <v>0.288781305538684</v>
+        <v>0.427031600716194</v>
       </c>
       <c r="AX105" t="n">
         <v>-0.593916918716119</v>
@@ -19125,7 +19189,7 @@
         <v>-0.576954532238213</v>
       </c>
       <c r="BA105" t="n">
-        <v>1.32644405298631</v>
+        <v>1.33156228658233</v>
       </c>
       <c r="BB105" t="n">
         <v>-0.177422713558885</v>
@@ -19259,7 +19323,7 @@
         <v>0.488227846605137</v>
       </c>
       <c r="AM106" t="n">
-        <v>0.735932552866716</v>
+        <v>0.735932552866717</v>
       </c>
       <c r="AN106" t="n">
         <v>-1.24972532755751</v>
@@ -19289,7 +19353,7 @@
         <v>0.56094367697965</v>
       </c>
       <c r="AW106" t="n">
-        <v>0.426421822360585</v>
+        <v>0.538085536634626</v>
       </c>
       <c r="AX106" t="n">
         <v>0.0707890154062104</v>
@@ -19301,7 +19365,7 @@
         <v>1.1275024176941</v>
       </c>
       <c r="BA106" t="n">
-        <v>1.61987067760081</v>
+        <v>1.62551519477018</v>
       </c>
       <c r="BB106" t="n">
         <v>0.373190207732223</v>
@@ -19396,7 +19460,7 @@
         <v>0.533083389208079</v>
       </c>
       <c r="Z107" t="n">
-        <v>0.581785238995848</v>
+        <v>0.581785238995849</v>
       </c>
       <c r="AA107" t="n">
         <v>0.66064819175115</v>
@@ -19465,7 +19529,7 @@
         <v>0.374655062833897</v>
       </c>
       <c r="AW107" t="n">
-        <v>0.426421822360585</v>
+        <v>0.538085536634626</v>
       </c>
       <c r="AX107" t="n">
         <v>1.17863445462987</v>
@@ -19477,7 +19541,7 @@
         <v>0.165473143809549</v>
       </c>
       <c r="BA107" t="n">
-        <v>2.14207060276221</v>
+        <v>2.14865172629092</v>
       </c>
       <c r="BB107" t="n">
         <v>-0.240590764722106</v>
@@ -19566,7 +19630,7 @@
         <v>-1.11366442242669</v>
       </c>
       <c r="X108" t="n">
-        <v>-2.83582813502281</v>
+        <v>-2.83582813502282</v>
       </c>
       <c r="Y108" t="n">
         <v>-1.50034545314655</v>
@@ -19590,7 +19654,7 @@
         <v>1.25485796944927</v>
       </c>
       <c r="AF108" t="n">
-        <v>0.534845580603878</v>
+        <v>0.534845580603879</v>
       </c>
       <c r="AG108" t="n">
         <v>0.779117819418051</v>
@@ -19611,7 +19675,7 @@
         <v>-0.651079869922987</v>
       </c>
       <c r="AM108" t="n">
-        <v>1.17876488514591</v>
+        <v>1.17876488514592</v>
       </c>
       <c r="AN108" t="n">
         <v>-0.933865251420596</v>
@@ -19641,7 +19705,7 @@
         <v>0.0307376213340492</v>
       </c>
       <c r="AW108" t="n">
-        <v>0.288781305538684</v>
+        <v>0.427031600716194</v>
       </c>
       <c r="AX108" t="n">
         <v>-0.707056515763081</v>
@@ -19653,7 +19717,7 @@
         <v>-1.37373952276664</v>
       </c>
       <c r="BA108" t="n">
-        <v>0.714724140654384</v>
+        <v>0.71874520680089</v>
       </c>
       <c r="BB108" t="n">
         <v>-1.65452838061309</v>
@@ -19817,7 +19881,7 @@
         <v>0.847541544896191</v>
       </c>
       <c r="AW109" t="n">
-        <v>0.4429391006063</v>
+        <v>0.551412344773687</v>
       </c>
       <c r="AX109" t="n">
         <v>-0.00306646093412165</v>
@@ -19829,7 +19893,7 @@
         <v>1.30413317936421</v>
       </c>
       <c r="BA109" t="n">
-        <v>1.44580403588034</v>
+        <v>1.45113635092993</v>
       </c>
       <c r="BB109" t="n">
         <v>0.513058571642409</v>
@@ -19993,7 +20057,7 @@
         <v>0.847541544896191</v>
       </c>
       <c r="AW110" t="n">
-        <v>0.674176371300901</v>
+        <v>0.737983927288882</v>
       </c>
       <c r="AX110" t="n">
         <v>0.913376904559016</v>
@@ -20005,7 +20069,7 @@
         <v>1.53651252939257</v>
       </c>
       <c r="BA110" t="n">
-        <v>2.59961720385601</v>
+        <v>2.60701897295672</v>
       </c>
       <c r="BB110" t="n">
         <v>3.77814448295628</v>
@@ -20169,7 +20233,7 @@
         <v>-0.427818967332417</v>
       </c>
       <c r="AW111" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX111" t="n">
         <v>-0.48313038067595</v>
@@ -20181,7 +20245,7 @@
         <v>0.759425047973216</v>
       </c>
       <c r="BA111" t="n">
-        <v>1.8188039824242</v>
+        <v>1.82480530201618</v>
       </c>
       <c r="BB111" t="n">
         <v>-0.263728937360254</v>
@@ -20345,7 +20409,7 @@
         <v>0.861871438292017</v>
       </c>
       <c r="AW112" t="n">
-        <v>0.538154515373862</v>
+        <v>0.628235992448056</v>
       </c>
       <c r="AX112" t="n">
         <v>-0.11912411703188</v>
@@ -20357,7 +20421,7 @@
         <v>-0.82711533875475</v>
       </c>
       <c r="BA112" t="n">
-        <v>1.04793742623356</v>
+        <v>1.05255613643794</v>
       </c>
       <c r="BB112" t="n">
         <v>-0.592440064162914</v>
@@ -20521,7 +20585,7 @@
         <v>0.31733548925059</v>
       </c>
       <c r="AW113" t="n">
-        <v>0.187360638612032</v>
+        <v>0.345201304625029</v>
       </c>
       <c r="AX113" t="n">
         <v>0.0000775981342769585</v>
@@ -20533,7 +20597,7 @@
         <v>-1.77391382492672</v>
       </c>
       <c r="BA113" t="n">
-        <v>0.471030842245731</v>
+        <v>0.474614825424544</v>
       </c>
       <c r="BB113" t="n">
         <v>-1.06171244026329</v>
@@ -20697,7 +20761,7 @@
         <v>-0.728746728644785</v>
       </c>
       <c r="AW114" t="n">
-        <v>0.529653077116775</v>
+        <v>0.621376688216885</v>
       </c>
       <c r="AX114" t="n">
         <v>-0.651719746747396</v>
@@ -20709,7 +20773,7 @@
         <v>-0.418764251524614</v>
       </c>
       <c r="BA114" t="n">
-        <v>1.07777742195707</v>
+        <v>1.08244965252484</v>
       </c>
       <c r="BB114" t="n">
         <v>0.522895444492656</v>
@@ -20873,7 +20937,7 @@
         <v>0.646923037354612</v>
       </c>
       <c r="AW115" t="n">
-        <v>0.0575440348440829</v>
+        <v>0.240460018200999</v>
       </c>
       <c r="AX115" t="n">
         <v>-0.393787256070568</v>
@@ -20885,7 +20949,7 @@
         <v>0.347998513224192</v>
       </c>
       <c r="BA115" t="n">
-        <v>2.08736394393578</v>
+        <v>2.09384694679827</v>
       </c>
       <c r="BB115" t="n">
         <v>-0.0971739877666864</v>
@@ -21049,7 +21113,7 @@
         <v>-0.513798327707379</v>
       </c>
       <c r="AW116" t="n">
-        <v>0.642928122725586</v>
+        <v>0.712771576485691</v>
       </c>
       <c r="AX116" t="n">
         <v>0.473640693840389</v>
@@ -21061,7 +21125,7 @@
         <v>0.641532893082507</v>
       </c>
       <c r="BA116" t="n">
-        <v>0.769430799480817</v>
+        <v>0.77354998629354</v>
       </c>
       <c r="BB116" t="n">
         <v>-0.3218788185956</v>
@@ -21225,7 +21289,7 @@
         <v>0.962180692062807</v>
       </c>
       <c r="AW117" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX117" t="n">
         <v>-0.574075446582567</v>
@@ -21237,7 +21301,7 @@
         <v>-0.2244496666209</v>
       </c>
       <c r="BA117" t="n">
-        <v>1.47067069898327</v>
+        <v>1.47604761433568</v>
       </c>
       <c r="BB117" t="n">
         <v>-0.657193353106697</v>
@@ -21401,7 +21465,7 @@
         <v>-0.599777688082342</v>
       </c>
       <c r="AW118" t="n">
-        <v>0.0134979595221753</v>
+        <v>0.204921863163504</v>
       </c>
       <c r="AX118" t="n">
         <v>-0.320217603281908</v>
@@ -21413,7 +21477,7 @@
         <v>-0.0466473058959796</v>
       </c>
       <c r="BA118" t="n">
-        <v>1.75912399097718</v>
+        <v>1.76501826984238</v>
       </c>
       <c r="BB118" t="n">
         <v>0.224681773004798</v>
@@ -21577,7 +21641,7 @@
         <v>1.24877855997935</v>
       </c>
       <c r="AW119" t="n">
-        <v>-0.166686746548472</v>
+        <v>0.0595415546360138</v>
       </c>
       <c r="AX119" t="n">
         <v>1.17863445462987</v>
@@ -21589,7 +21653,7 @@
         <v>0.157223133798564</v>
       </c>
       <c r="BA119" t="n">
-        <v>1.74917732573601</v>
+        <v>1.75505376448008</v>
       </c>
       <c r="BB119" t="n">
         <v>-0.282489334140822</v>
@@ -21753,7 +21817,7 @@
         <v>0.661252930750438</v>
       </c>
       <c r="AW120" t="n">
-        <v>0.674176371300901</v>
+        <v>0.737983927288882</v>
       </c>
       <c r="AX120" t="n">
         <v>0.347752036976961</v>
@@ -21765,7 +21829,7 @@
         <v>1.08924238606032</v>
       </c>
       <c r="BA120" t="n">
-        <v>1.21703073533344</v>
+        <v>1.22195272759703</v>
       </c>
       <c r="BB120" t="n">
         <v>0.942206584846686</v>
@@ -21929,7 +21993,7 @@
         <v>-0.413489073936589</v>
       </c>
       <c r="AW121" t="n">
-        <v>0.569068626093024</v>
+        <v>0.653178747314513</v>
       </c>
       <c r="AX121" t="n">
         <v>-0.507219323728544</v>
@@ -21941,7 +22005,7 @@
         <v>-1.9469809728051</v>
       </c>
       <c r="BA121" t="n">
-        <v>0.301937533145849</v>
+        <v>0.305218234265446</v>
       </c>
       <c r="BB121" t="n">
         <v>-1.22334370430001</v>
@@ -22105,7 +22169,7 @@
         <v>-0.829055982415574</v>
       </c>
       <c r="AW122" t="n">
-        <v>0.353013238405877</v>
+        <v>0.478856522049352</v>
       </c>
       <c r="AX122" t="n">
         <v>-0.0696434072958139</v>
@@ -22117,7 +22181,7 @@
         <v>0.125004159791165</v>
       </c>
       <c r="BA122" t="n">
-        <v>1.01312409788947</v>
+        <v>1.01768036766989</v>
       </c>
       <c r="BB122" t="n">
         <v>0.662186403913233</v>
@@ -22281,7 +22345,7 @@
         <v>0.345995276042245</v>
       </c>
       <c r="AW123" t="n">
-        <v>0.585239048432697</v>
+        <v>0.6662256980798</v>
       </c>
       <c r="AX123" t="n">
         <v>0.624708411488371</v>
@@ -22293,7 +22357,7 @@
         <v>-0.649727919361742</v>
       </c>
       <c r="BA123" t="n">
-        <v>1.18221740698935</v>
+        <v>1.18707695882898</v>
       </c>
       <c r="BB123" t="n">
         <v>0.400737651018294</v>
@@ -22382,7 +22446,7 @@
         <v>-0.0106120196482577</v>
       </c>
       <c r="X124" t="n">
-        <v>-0.085802094526895</v>
+        <v>-0.0858020945268951</v>
       </c>
       <c r="Y124" t="n">
         <v>0.809509838710827</v>
@@ -22457,7 +22521,7 @@
         <v>-0.900705449394709</v>
       </c>
       <c r="AW124" t="n">
-        <v>0.358853135677269</v>
+        <v>0.483568387365774</v>
       </c>
       <c r="AX124" t="n">
         <v>0.624708411488371</v>
@@ -22469,7 +22533,7 @@
         <v>-0.242109081540865</v>
       </c>
       <c r="BA124" t="n">
-        <v>1.0678307567159</v>
+        <v>1.07248514716254</v>
       </c>
       <c r="BB124" t="n">
         <v>-0.897866042639161</v>
@@ -22564,7 +22628,7 @@
         <v>-0.664271929633818</v>
       </c>
       <c r="Z125" t="n">
-        <v>-0.333835075426574</v>
+        <v>-0.333835075426575</v>
       </c>
       <c r="AA125" t="n">
         <v>-0.831935779476728</v>
@@ -22633,7 +22697,7 @@
         <v>-0.0695716324367406</v>
       </c>
       <c r="AW125" t="n">
-        <v>0.38512978293265</v>
+        <v>0.504769449144888</v>
       </c>
       <c r="AX125" t="n">
         <v>0.0707890154062104</v>
@@ -22645,7 +22709,7 @@
         <v>-0.292439024270604</v>
       </c>
       <c r="BA125" t="n">
-        <v>0.684884144930876</v>
+        <v>0.688851690713991</v>
       </c>
       <c r="BB125" t="n">
         <v>-0.339221949810764</v>
@@ -22809,7 +22873,7 @@
         <v>0.517953996792167</v>
       </c>
       <c r="AW126" t="n">
-        <v>0.552472727175272</v>
+        <v>0.639788504837397</v>
       </c>
       <c r="AX126" t="n">
         <v>1.24380222441123</v>
@@ -22821,7 +22885,7 @@
         <v>0.198753879460374</v>
       </c>
       <c r="BA126" t="n">
-        <v>1.74917732573601</v>
+        <v>1.75505376448008</v>
       </c>
       <c r="BB126" t="n">
         <v>1.08498296773181</v>
@@ -22985,7 +23049,7 @@
         <v>0.532283890187996</v>
       </c>
       <c r="AW127" t="n">
-        <v>0.261252508462492</v>
+        <v>0.40482025381776</v>
       </c>
       <c r="AX127" t="n">
         <v>0.852795605723107</v>
@@ -22997,7 +23061,7 @@
         <v>0.854226938158623</v>
       </c>
       <c r="BA127" t="n">
-        <v>0.978310769545377</v>
+        <v>0.982804598901837</v>
       </c>
       <c r="BB127" t="n">
         <v>0.607647925303804</v>
@@ -23161,7 +23225,7 @@
         <v>-0.786066302228093</v>
       </c>
       <c r="AW128" t="n">
-        <v>-0.126260690699288</v>
+        <v>0.0921589315492328</v>
       </c>
       <c r="AX128" t="n">
         <v>-1.29772085588352</v>
@@ -23173,7 +23237,7 @@
         <v>-0.567410881604203</v>
       </c>
       <c r="BA128" t="n">
-        <v>1.29163072464222</v>
+        <v>1.29668651781428</v>
       </c>
       <c r="BB128" t="n">
         <v>-0.179060442656685</v>
@@ -23337,7 +23401,7 @@
         <v>0.747232291125401</v>
       </c>
       <c r="AW129" t="n">
-        <v>0.38512978293265</v>
+        <v>0.504769449144888</v>
       </c>
       <c r="AX129" t="n">
         <v>-0.298495013354791</v>
@@ -23349,7 +23413,7 @@
         <v>0.346192298014686</v>
       </c>
       <c r="BA129" t="n">
-        <v>1.56019068615379</v>
+        <v>1.56572816259638</v>
       </c>
       <c r="BB129" t="n">
         <v>0.631709945125328</v>
@@ -23513,7 +23577,7 @@
         <v>0.202696342083974</v>
       </c>
       <c r="AW130" t="n">
-        <v>0.288781305538684</v>
+        <v>0.427031600716194</v>
       </c>
       <c r="AX130" t="n">
         <v>0.372931097761515</v>
@@ -23525,7 +23589,7 @@
         <v>0.567990644079256</v>
       </c>
       <c r="BA130" t="n">
-        <v>0.719697473274969</v>
+        <v>0.72372745948204</v>
       </c>
       <c r="BB130" t="n">
         <v>-0.434063261794898</v>
@@ -23689,7 +23753,7 @@
         <v>-0.327509713561627</v>
       </c>
       <c r="AW131" t="n">
-        <v>0.674176371300901</v>
+        <v>0.737983927288882</v>
       </c>
       <c r="AX131" t="n">
         <v>-0.0937389974077486</v>
@@ -23701,7 +23765,7 @@
         <v>-0.804330177969972</v>
       </c>
       <c r="BA131" t="n">
-        <v>1.21205740271286</v>
+        <v>1.21697047491588</v>
       </c>
       <c r="BB131" t="n">
         <v>-0.65058994539826</v>
@@ -23865,7 +23929,7 @@
         <v>0.245686022271455</v>
       </c>
       <c r="AW132" t="n">
-        <v>0.577827893906935</v>
+        <v>0.660246078860188</v>
       </c>
       <c r="AX132" t="n">
         <v>-1.43990810225163</v>
@@ -23877,7 +23941,7 @@
         <v>-0.627906886965822</v>
       </c>
       <c r="BA132" t="n">
-        <v>1.52040402518911</v>
+        <v>1.52587014114718</v>
       </c>
       <c r="BB132" t="n">
         <v>0.340908047631358</v>
@@ -23972,7 +24036,7 @@
         <v>-0.687117599664007</v>
       </c>
       <c r="Z133" t="n">
-        <v>-0.583703967414414</v>
+        <v>-0.583703967414415</v>
       </c>
       <c r="AA133" t="n">
         <v>-0.559534291731016</v>
@@ -24041,7 +24105,7 @@
         <v>1.23444866658352</v>
       </c>
       <c r="AW133" t="n">
-        <v>0.509007057402808</v>
+        <v>0.604718644472016</v>
       </c>
       <c r="AX133" t="n">
         <v>0.901671433059122</v>
@@ -24053,7 +24117,7 @@
         <v>0.155819655764151</v>
       </c>
       <c r="BA133" t="n">
-        <v>1.00815076526889</v>
+        <v>1.01269811498874</v>
       </c>
       <c r="BB133" t="n">
         <v>0.0898210807590383</v>
@@ -24217,7 +24281,7 @@
         <v>-0.155550992811702</v>
       </c>
       <c r="AW134" t="n">
-        <v>0.665659902621219</v>
+        <v>0.731112495904847</v>
       </c>
       <c r="AX134" t="n">
         <v>0.556024347315511</v>
@@ -24229,7 +24293,7 @@
         <v>0.0387695876940898</v>
       </c>
       <c r="BA134" t="n">
-        <v>-0.424169029459525</v>
+        <v>-0.422190657182445</v>
       </c>
       <c r="BB134" t="n">
         <v>0.220461471098928</v>
@@ -24393,7 +24457,7 @@
         <v>0.303005595854762</v>
       </c>
       <c r="AW135" t="n">
-        <v>0.591591136258678</v>
+        <v>0.671350819451493</v>
       </c>
       <c r="AX135" t="n">
         <v>-0.48313038067595</v>
@@ -24405,7 +24469,7 @@
         <v>0.669870945220833</v>
       </c>
       <c r="BA135" t="n">
-        <v>0.50087083796924</v>
+        <v>0.504508341511443</v>
       </c>
       <c r="BB135" t="n">
         <v>0.636108717509803</v>
@@ -24569,7 +24633,7 @@
         <v>-0.184210779603357</v>
       </c>
       <c r="AW136" t="n">
-        <v>0.577827893906935</v>
+        <v>0.660246078860188</v>
       </c>
       <c r="AX136" t="n">
         <v>0.624708411488371</v>
@@ -24581,7 +24645,7 @@
         <v>0.789837806771109</v>
       </c>
       <c r="BA136" t="n">
-        <v>-0.822035639106305</v>
+        <v>-0.820770871674439</v>
       </c>
       <c r="BB136" t="n">
         <v>0.600897541907104</v>
@@ -24745,7 +24809,7 @@
         <v>0.56094367697965</v>
       </c>
       <c r="AW137" t="n">
-        <v>0.229489756959881</v>
+        <v>0.379192781243473</v>
       </c>
       <c r="AX137" t="n">
         <v>1.37129946963523</v>
@@ -24757,7 +24821,7 @@
         <v>1.02492647961373</v>
       </c>
       <c r="BA137" t="n">
-        <v>-0.265022385600812</v>
+        <v>-0.262758571385647</v>
       </c>
       <c r="BB137" t="n">
         <v>0.284563867708971</v>
@@ -24852,7 +24916,7 @@
         <v>-0.133063917462853</v>
       </c>
       <c r="Z138" t="n">
-        <v>-0.00576050418635905</v>
+        <v>-0.00576050418635906</v>
       </c>
       <c r="AA138" t="n">
         <v>0.0662723004814374</v>
@@ -24921,7 +24985,7 @@
         <v>-0.65709726166565</v>
       </c>
       <c r="AW138" t="n">
-        <v>0.288781305538684</v>
+        <v>0.427031600716194</v>
       </c>
       <c r="AX138" t="n">
         <v>-0.593916918716119</v>
@@ -24933,7 +24997,7 @@
         <v>-0.576954532238213</v>
       </c>
       <c r="BA138" t="n">
-        <v>0.416324183419299</v>
+        <v>0.419810045931894</v>
       </c>
       <c r="BB138" t="n">
         <v>-0.13707788713039</v>
@@ -25067,7 +25131,7 @@
         <v>0.488227846605137</v>
       </c>
       <c r="AM139" t="n">
-        <v>0.735932552866716</v>
+        <v>0.735932552866717</v>
       </c>
       <c r="AN139" t="n">
         <v>0.645435129263989</v>
@@ -25097,7 +25161,7 @@
         <v>0.646923037354612</v>
       </c>
       <c r="AW139" t="n">
-        <v>0.426421822360585</v>
+        <v>0.538085536634626</v>
       </c>
       <c r="AX139" t="n">
         <v>0.73549494952854</v>
@@ -25109,7 +25173,7 @@
         <v>1.1275024176941</v>
       </c>
       <c r="BA139" t="n">
-        <v>0.227337543837078</v>
+        <v>0.230484444048197</v>
       </c>
       <c r="BB139" t="n">
         <v>0.564059135470051</v>
@@ -25204,7 +25268,7 @@
         <v>0.533083389208079</v>
       </c>
       <c r="Z140" t="n">
-        <v>0.581785238995848</v>
+        <v>0.581785238995849</v>
       </c>
       <c r="AA140" t="n">
         <v>0.66064819175115</v>
@@ -25273,7 +25337,7 @@
         <v>0.403314849625552</v>
       </c>
       <c r="AW140" t="n">
-        <v>0.426421822360585</v>
+        <v>0.538085536634626</v>
       </c>
       <c r="AX140" t="n">
         <v>0.977208615412783</v>
@@ -25285,7 +25349,7 @@
         <v>0.165473143809549</v>
       </c>
       <c r="BA140" t="n">
-        <v>-0.409249031597771</v>
+        <v>-0.407243899138995</v>
       </c>
       <c r="BB140" t="n">
         <v>-0.23205567653934</v>
@@ -25419,7 +25483,7 @@
         <v>-0.651079869922987</v>
       </c>
       <c r="AM141" t="n">
-        <v>1.17876488514591</v>
+        <v>1.17876488514592</v>
       </c>
       <c r="AN141" t="n">
         <v>0.0635876205907209</v>
@@ -25449,7 +25513,7 @@
         <v>-0.771736408832266</v>
       </c>
       <c r="AW141" t="n">
-        <v>0.288781305538684</v>
+        <v>0.427031600716194</v>
       </c>
       <c r="AX141" t="n">
         <v>0.221856733054192</v>
@@ -25461,7 +25525,7 @@
         <v>-1.37373952276664</v>
       </c>
       <c r="BA141" t="n">
-        <v>-2.44334207341694</v>
+        <v>-2.44498524572932</v>
       </c>
       <c r="BB141" t="n">
         <v>-1.66460671352263</v>
@@ -25625,7 +25689,7 @@
         <v>0.890531225083672</v>
       </c>
       <c r="AW142" t="n">
-        <v>0.4429391006063</v>
+        <v>0.551412344773687</v>
       </c>
       <c r="AX142" t="n">
         <v>1.37129946963523</v>
@@ -25637,7 +25701,7 @@
         <v>1.30413317936421</v>
       </c>
       <c r="BA142" t="n">
-        <v>0.222364211216494</v>
+        <v>0.225502191367047</v>
       </c>
       <c r="BB142" t="n">
         <v>0.591417610014069</v>
@@ -25801,7 +25865,7 @@
         <v>-0.55678800789486</v>
       </c>
       <c r="AW143" t="n">
-        <v>0.674176371300901</v>
+        <v>0.737983927288882</v>
       </c>
       <c r="AX143" t="n">
         <v>1.17863445462987</v>
@@ -25813,7 +25877,7 @@
         <v>1.53651252939257</v>
       </c>
       <c r="BA143" t="n">
-        <v>1.07280408933649</v>
+        <v>1.07746739984369</v>
       </c>
       <c r="BB143" t="n">
         <v>4.05757676113668</v>
@@ -25902,7 +25966,7 @@
         <v>-0.958922158786782</v>
       </c>
       <c r="X144" t="n">
-        <v>0.388561371665874</v>
+        <v>0.388561371665875</v>
       </c>
       <c r="Y144" t="n">
         <v>0.160019550215545</v>
@@ -25926,7 +25990,7 @@
         <v>-1.01969793490601</v>
       </c>
       <c r="AF144" t="n">
-        <v>0.67942911045338</v>
+        <v>0.679429110453381</v>
       </c>
       <c r="AG144" t="n">
         <v>0.365346861544547</v>
@@ -25977,7 +26041,7 @@
         <v>0.474964316604687</v>
       </c>
       <c r="AW144" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX144" t="n">
         <v>0.347752036976961</v>
@@ -25989,7 +26053,7 @@
         <v>0.759425047973216</v>
       </c>
       <c r="BA144" t="n">
-        <v>-0.503742351388881</v>
+        <v>-0.501906700080844</v>
       </c>
       <c r="BB144" t="n">
         <v>-0.198891662308891</v>
@@ -26153,7 +26217,7 @@
         <v>0.532283890187996</v>
       </c>
       <c r="AW145" t="n">
-        <v>0.538154515373862</v>
+        <v>0.628235992448056</v>
       </c>
       <c r="AX145" t="n">
         <v>0.207372790749667</v>
@@ -26164,7 +26228,9 @@
       <c r="AZ145" t="n">
         <v>-0.82711533875475</v>
       </c>
-      <c r="BA145"/>
+      <c r="BA145" t="n">
+        <v>-0.546746974211193</v>
+      </c>
       <c r="BB145" t="n">
         <v>-0.492549087460563</v>
       </c>
@@ -26327,7 +26393,7 @@
         <v>-1.80348873333181</v>
       </c>
       <c r="AW146" t="n">
-        <v>0.187360638612032</v>
+        <v>0.345201304625029</v>
       </c>
       <c r="AX146" t="n">
         <v>1.08229862359752</v>
@@ -26339,7 +26405,7 @@
         <v>-1.77391382492672</v>
       </c>
       <c r="BA146" t="n">
-        <v>-1.17514225516782</v>
+        <v>-1.17451081203608</v>
       </c>
       <c r="BB146" t="n">
         <v>-0.973663504729646</v>
@@ -26503,7 +26569,7 @@
         <v>-0.499468434311552</v>
       </c>
       <c r="AW147" t="n">
-        <v>0.529653077116775</v>
+        <v>0.621376688216885</v>
       </c>
       <c r="AX147" t="n">
         <v>-0.124714293937849</v>
@@ -26515,7 +26581,7 @@
         <v>-0.418764251524614</v>
       </c>
       <c r="BA147" t="n">
-        <v>0.088084230460705</v>
+        <v>0.0909813689759986</v>
       </c>
       <c r="BB147" t="n">
         <v>0.627857082440118</v>
@@ -26679,7 +26745,7 @@
         <v>0.288675702458936</v>
       </c>
       <c r="AW148" t="n">
-        <v>0.0575440348440829</v>
+        <v>0.240460018200999</v>
       </c>
       <c r="AX148" t="n">
         <v>0.72104424252072</v>
@@ -26691,7 +26757,7 @@
         <v>0.347998513224192</v>
       </c>
       <c r="BA148" t="n">
-        <v>-1.45364888192057</v>
+        <v>-1.45351696218048</v>
       </c>
       <c r="BB148" t="n">
         <v>-0.0310349280478415</v>
@@ -26855,7 +26921,7 @@
         <v>-0.528128221103206</v>
       </c>
       <c r="AW149" t="n">
-        <v>0.642928122725586</v>
+        <v>0.712771576485691</v>
       </c>
       <c r="AX149" t="n">
         <v>0.484162988777546</v>
@@ -26867,7 +26933,7 @@
         <v>0.641532893082507</v>
       </c>
       <c r="BA149" t="n">
-        <v>-0.633048999524085</v>
+        <v>-0.631445269790742</v>
       </c>
       <c r="BB149" t="n">
         <v>-0.309711331260022</v>
@@ -27031,7 +27097,7 @@
         <v>0.431974636417206</v>
       </c>
       <c r="AW150" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX150" t="n">
         <v>0.2722148546233</v>
@@ -27043,7 +27109,7 @@
         <v>-0.2244496666209</v>
       </c>
       <c r="BA150" t="n">
-        <v>-0.652942330006424</v>
+        <v>-0.651374280515342</v>
       </c>
       <c r="BB150" t="n">
         <v>-0.638327973691655</v>
@@ -27207,7 +27273,7 @@
         <v>-0.413489073936589</v>
       </c>
       <c r="AW151" t="n">
-        <v>0.0134979595221753</v>
+        <v>0.204921863163504</v>
       </c>
       <c r="AX151" t="n">
         <v>0.809350425868872</v>
@@ -27219,7 +27285,7 @@
         <v>-0.0466473058959796</v>
       </c>
       <c r="BA151" t="n">
-        <v>-0.508715684009466</v>
+        <v>-0.506888952761994</v>
       </c>
       <c r="BB151" t="n">
         <v>0.280490541491366</v>
@@ -27383,7 +27449,7 @@
         <v>0.790221971312882</v>
       </c>
       <c r="AW152" t="n">
-        <v>-0.166686746548472</v>
+        <v>0.0595415546360138</v>
       </c>
       <c r="AX152" t="n">
         <v>1.53314207047533</v>
@@ -27395,7 +27461,7 @@
         <v>0.157223133798564</v>
       </c>
       <c r="BA152" t="n">
-        <v>-0.891662295794492</v>
+        <v>-0.890522409210539</v>
       </c>
       <c r="BB152" t="n">
         <v>-0.208907005637745</v>
@@ -27559,7 +27625,7 @@
         <v>0.374655062833897</v>
       </c>
       <c r="AW153" t="n">
-        <v>0.674176371300901</v>
+        <v>0.737983927288882</v>
       </c>
       <c r="AX153" t="n">
         <v>1.13148686272258</v>
@@ -27571,7 +27637,7 @@
         <v>1.08924238606032</v>
       </c>
       <c r="BA153" t="n">
-        <v>-0.389355701115431</v>
+        <v>-0.387314888414395</v>
       </c>
       <c r="BB153" t="n">
         <v>1.17146766201179</v>
@@ -27735,7 +27801,7 @@
         <v>-1.0010147031655</v>
       </c>
       <c r="AW154" t="n">
-        <v>0.569068626093024</v>
+        <v>0.653178747314513</v>
       </c>
       <c r="AX154" t="n">
         <v>-0.141351883468931</v>
@@ -27747,7 +27813,7 @@
         <v>-1.9469809728051</v>
       </c>
       <c r="BA154" t="n">
-        <v>-1.508355540747</v>
+        <v>-1.50832174167313</v>
       </c>
       <c r="BB154" t="n">
         <v>-1.1771093520775</v>
@@ -27911,7 +27977,7 @@
         <v>-0.198540672999185</v>
       </c>
       <c r="AW155" t="n">
-        <v>0.353013238405877</v>
+        <v>0.478856522049352</v>
       </c>
       <c r="AX155" t="n">
         <v>0.255431029786711</v>
@@ -27923,7 +27989,7 @@
         <v>0.125004159791165</v>
       </c>
       <c r="BA155" t="n">
-        <v>0.282044202663511</v>
+        <v>0.285289223540846</v>
       </c>
       <c r="BB155" t="n">
         <v>0.811083274388214</v>
@@ -28087,7 +28153,7 @@
         <v>0.159706661896491</v>
       </c>
       <c r="AW156" t="n">
-        <v>0.585239048432697</v>
+        <v>0.6662256980798</v>
       </c>
       <c r="AX156" t="n">
         <v>1.08229862359752</v>
@@ -28099,7 +28165,7 @@
         <v>-0.649727919361742</v>
       </c>
       <c r="BA156" t="n">
-        <v>-0.0263024198127443</v>
+        <v>-0.0236104426904498</v>
       </c>
       <c r="BB156" t="n">
         <v>0.618114693960898</v>
@@ -28263,7 +28329,7 @@
         <v>-0.757406515436438</v>
       </c>
       <c r="AW157" t="n">
-        <v>0.585239048432697</v>
+        <v>0.6662256980798</v>
       </c>
       <c r="AX157" t="n">
         <v>-0.48313038067595</v>
@@ -28275,7 +28341,7 @@
         <v>-0.242109081540865</v>
       </c>
       <c r="BA157" t="n">
-        <v>-0.692728990971102</v>
+        <v>-0.691232301964541</v>
       </c>
       <c r="BB157" t="n">
         <v>-0.826887283471048</v>
@@ -28370,7 +28436,7 @@
         <v>-0.664271929633818</v>
       </c>
       <c r="Z158" t="n">
-        <v>-0.333835075426574</v>
+        <v>-0.333835075426575</v>
       </c>
       <c r="AA158" t="n">
         <v>-0.831935779476728</v>
@@ -28439,7 +28505,7 @@
         <v>0.345995276042245</v>
       </c>
       <c r="AW158" t="n">
-        <v>0.38512978293265</v>
+        <v>0.504769449144888</v>
       </c>
       <c r="AX158" t="n">
         <v>0.274268795959738</v>
@@ -28451,7 +28517,7 @@
         <v>-0.292439024270604</v>
       </c>
       <c r="BA158" t="n">
-        <v>-0.812088973865136</v>
+        <v>-0.810806366312139</v>
       </c>
       <c r="BB158" t="n">
         <v>-0.261776260359031</v>
@@ -28615,7 +28681,7 @@
         <v>0.388984956229725</v>
       </c>
       <c r="AW159" t="n">
-        <v>0.552472727175272</v>
+        <v>0.639788504837397</v>
       </c>
       <c r="AX159" t="n">
         <v>1.73255385071203</v>
@@ -28627,7 +28693,7 @@
         <v>0.198753879460374</v>
       </c>
       <c r="BA159" t="n">
-        <v>1.22200406795403</v>
+        <v>1.22693498027818</v>
       </c>
       <c r="BB159" t="n">
         <v>1.14195704346104</v>
@@ -28791,7 +28857,7 @@
         <v>-0.399159180540762</v>
       </c>
       <c r="AW160" t="n">
-        <v>0.261252508462492</v>
+        <v>0.40482025381776</v>
       </c>
       <c r="AX160" t="n">
         <v>0.770478422841398</v>
@@ -28803,7 +28869,7 @@
         <v>0.854226938158623</v>
       </c>
       <c r="BA160" t="n">
-        <v>0.674937479689706</v>
+        <v>0.678887185351691</v>
       </c>
       <c r="BB160" t="n">
         <v>0.89289624143408</v>
@@ -28967,7 +29033,7 @@
         <v>-0.829055982415574</v>
       </c>
       <c r="AW161" t="n">
-        <v>0.609943282247355</v>
+        <v>0.686158073097811</v>
       </c>
       <c r="AX161" t="n">
         <v>-0.320217603281908</v>
@@ -28979,7 +29045,7 @@
         <v>-0.567410881604203</v>
       </c>
       <c r="BA161" t="n">
-        <v>-0.757382315038704</v>
+        <v>-0.75600158681949</v>
       </c>
       <c r="BB161" t="n">
         <v>-0.0759360008125242</v>
@@ -29143,7 +29209,7 @@
         <v>0.102387088313184</v>
       </c>
       <c r="AW162" t="n">
-        <v>0.491620327019281</v>
+        <v>0.590690327182698</v>
       </c>
       <c r="AX162" t="n">
         <v>1.11532786146406</v>
@@ -29155,7 +29221,7 @@
         <v>0.346192298014686</v>
       </c>
       <c r="BA162" t="n">
-        <v>0.655044149207368</v>
+        <v>0.658958174627091</v>
       </c>
       <c r="BB162" t="n">
         <v>0.916895271674918</v>
@@ -29319,7 +29385,7 @@
         <v>0.0450675147298754</v>
       </c>
       <c r="AW163" t="n">
-        <v>0.288781305538684</v>
+        <v>0.427031600716194</v>
       </c>
       <c r="AX163" t="n">
         <v>0.0707890154062104</v>
@@ -29331,7 +29397,7 @@
         <v>0.567990644079256</v>
       </c>
       <c r="BA163" t="n">
-        <v>-0.747435649797534</v>
+        <v>-0.74603708145719</v>
       </c>
       <c r="BB163" t="n">
         <v>-0.324093952183009</v>
@@ -29495,7 +29561,7 @@
         <v>-0.413489073936589</v>
       </c>
       <c r="AW164" t="n">
-        <v>0.674176371300901</v>
+        <v>0.737983927288882</v>
       </c>
       <c r="AX164" t="n">
         <v>0.133497373231311</v>
@@ -29507,7 +29573,7 @@
         <v>-0.804330177969972</v>
       </c>
       <c r="BA164" t="n">
-        <v>-1.30942223592361</v>
+        <v>-1.30903163442713</v>
       </c>
       <c r="BB164" t="n">
         <v>-0.592933482544943</v>
@@ -29671,7 +29737,7 @@
         <v>0.0880571949173561</v>
       </c>
       <c r="AW165" t="n">
-        <v>0.577827893906935</v>
+        <v>0.660246078860188</v>
       </c>
       <c r="AX165" t="n">
         <v>-0.835630584600363</v>
@@ -29683,7 +29749,7 @@
         <v>-0.627906886965822</v>
       </c>
       <c r="BA165" t="n">
-        <v>0.60531082300152</v>
+        <v>0.609135647815592</v>
       </c>
       <c r="BB165" t="n">
         <v>0.539566686847184</v>
@@ -29778,7 +29844,7 @@
         <v>-0.687117599664007</v>
       </c>
       <c r="Z166" t="n">
-        <v>-0.583703967414414</v>
+        <v>-0.583703967414415</v>
       </c>
       <c r="AA166" t="n">
         <v>-0.559534291731016</v>
@@ -29847,7 +29913,7 @@
         <v>0.933520905271153</v>
       </c>
       <c r="AW166" t="n">
-        <v>0.509007057402808</v>
+        <v>0.604718644472016</v>
       </c>
       <c r="AX166" t="n">
         <v>1.08229862359752</v>
@@ -29859,7 +29925,7 @@
         <v>0.155819655764151</v>
       </c>
       <c r="BA166" t="n">
-        <v>-0.359515705391923</v>
+        <v>-0.357421372327496</v>
       </c>
       <c r="BB166" t="n">
         <v>0.149640185882527</v>
@@ -30023,7 +30089,7 @@
         <v>-0.284520033374146</v>
       </c>
       <c r="AW167" t="n">
-        <v>0.665659902621219</v>
+        <v>0.731112495904847</v>
       </c>
       <c r="AX167" t="n">
         <v>0.556024347315511</v>
@@ -30035,7 +30101,7 @@
         <v>0.544302375689725</v>
       </c>
       <c r="BA167" t="n">
-        <v>-0.424169029459525</v>
+        <v>-0.422190657182445</v>
       </c>
       <c r="BB167" t="n">
         <v>0.199664411209558</v>
@@ -30199,7 +30265,7 @@
         <v>0.260015915667281</v>
       </c>
       <c r="AW168" t="n">
-        <v>0.591591136258678</v>
+        <v>0.671350819451493</v>
       </c>
       <c r="AX168" t="n">
         <v>-0.48313038067595</v>
@@ -30211,7 +30277,7 @@
         <v>1.49384679714641</v>
       </c>
       <c r="BA168" t="n">
-        <v>0.50087083796924</v>
+        <v>0.504508341511443</v>
       </c>
       <c r="BB168" t="n">
         <v>0.543041612048286</v>
@@ -30375,7 +30441,7 @@
         <v>0.46063442320886</v>
       </c>
       <c r="AW169" t="n">
-        <v>0.577827893906935</v>
+        <v>0.660246078860188</v>
       </c>
       <c r="AX169" t="n">
         <v>0.624708411488371</v>
@@ -30387,7 +30453,7 @@
         <v>1.88165828844683</v>
       </c>
       <c r="BA169" t="n">
-        <v>-0.822035639106305</v>
+        <v>-0.820770871674439</v>
       </c>
       <c r="BB169" t="n">
         <v>0.552259087355134</v>
@@ -30551,7 +30617,7 @@
         <v>0.575273570375476</v>
       </c>
       <c r="AW170" t="n">
-        <v>0.229489756959881</v>
+        <v>0.379192781243473</v>
       </c>
       <c r="AX170" t="n">
         <v>1.37129946963523</v>
@@ -30563,7 +30629,7 @@
         <v>1.10105600986303</v>
       </c>
       <c r="BA170" t="n">
-        <v>-0.265022385600812</v>
+        <v>-0.262758571385647</v>
       </c>
       <c r="BB170" t="n">
         <v>0.050704551153893</v>
@@ -30652,7 +30718,7 @@
         <v>-1.58682478732974</v>
       </c>
       <c r="X171" t="n">
-        <v>-1.47043059044092</v>
+        <v>-1.47043059044093</v>
       </c>
       <c r="Y171" t="n">
         <v>-0.182347344005966</v>
@@ -30727,7 +30793,7 @@
         <v>-0.12689120602005</v>
       </c>
       <c r="AW171" t="n">
-        <v>0.288781305538684</v>
+        <v>0.427031600716194</v>
       </c>
       <c r="AX171" t="n">
         <v>-0.593916918716119</v>
@@ -30739,7 +30805,7 @@
         <v>0.416768936910438</v>
       </c>
       <c r="BA171" t="n">
-        <v>0.416324183419299</v>
+        <v>0.419810045931894</v>
       </c>
       <c r="BB171" t="n">
         <v>-0.122621778363271</v>
@@ -30834,7 +30900,7 @@
         <v>0.594282279769633</v>
       </c>
       <c r="Z172" t="n">
-        <v>0.201267446467568</v>
+        <v>0.201267446467569</v>
       </c>
       <c r="AA172" t="n">
         <v>0.914539379834871</v>
@@ -30873,7 +30939,7 @@
         <v>1.07847749874522</v>
       </c>
       <c r="AM172" t="n">
-        <v>0.735932552866716</v>
+        <v>0.735932552866717</v>
       </c>
       <c r="AN172" t="n">
         <v>0.645435129263989</v>
@@ -30903,7 +30969,7 @@
         <v>0.661252930750438</v>
       </c>
       <c r="AW172" t="n">
-        <v>0.426421822360585</v>
+        <v>0.538085536634626</v>
       </c>
       <c r="AX172" t="n">
         <v>0.73549494952854</v>
@@ -30915,7 +30981,7 @@
         <v>1.52264860724394</v>
       </c>
       <c r="BA172" t="n">
-        <v>0.227337543837078</v>
+        <v>0.230484444048197</v>
       </c>
       <c r="BB172" t="n">
         <v>0.683508376974975</v>
@@ -31028,7 +31094,7 @@
         <v>-0.332376729255229</v>
       </c>
       <c r="AF173" t="n">
-        <v>-0.758893769777108</v>
+        <v>-0.758893769777109</v>
       </c>
       <c r="AG173" t="n">
         <v>0.0959146099059861</v>
@@ -31079,7 +31145,7 @@
         <v>0.761562184521228</v>
       </c>
       <c r="AW173" t="n">
-        <v>0.426421822360585</v>
+        <v>0.538085536634626</v>
       </c>
       <c r="AX173" t="n">
         <v>0.977208615412783</v>
@@ -31091,7 +31157,7 @@
         <v>1.13455642033663</v>
       </c>
       <c r="BA173" t="n">
-        <v>-0.409249031597771</v>
+        <v>-0.407243899138995</v>
       </c>
       <c r="BB173" t="n">
         <v>-0.21740010076672</v>
@@ -31225,7 +31291,7 @@
         <v>-0.13706579347344</v>
       </c>
       <c r="AM174" t="n">
-        <v>1.17876488514591</v>
+        <v>1.17876488514592</v>
       </c>
       <c r="AN174" t="n">
         <v>0.0635876205907209</v>
@@ -31255,7 +31321,7 @@
         <v>-0.571117901290687</v>
       </c>
       <c r="AW174" t="n">
-        <v>0.288781305538684</v>
+        <v>0.427031600716194</v>
       </c>
       <c r="AX174" t="n">
         <v>0.221856733054192</v>
@@ -31267,7 +31333,7 @@
         <v>-1.05263595264972</v>
       </c>
       <c r="BA174" t="n">
-        <v>-2.44334207341694</v>
+        <v>-2.44498524572932</v>
       </c>
       <c r="BB174" t="n">
         <v>-1.6993244707433</v>
@@ -31362,7 +31428,7 @@
         <v>0.88765311436665</v>
       </c>
       <c r="Z175" t="n">
-        <v>0.510696426279138</v>
+        <v>0.510696426279139</v>
       </c>
       <c r="AA175" t="n">
         <v>0.964449186810243</v>
@@ -31431,7 +31497,7 @@
         <v>0.618263250562957</v>
       </c>
       <c r="AW175" t="n">
-        <v>0.4429391006063</v>
+        <v>0.551412344773687</v>
       </c>
       <c r="AX175" t="n">
         <v>1.37129946963523</v>
@@ -31443,7 +31509,7 @@
         <v>1.49659273243113</v>
       </c>
       <c r="BA175" t="n">
-        <v>0.222364211216494</v>
+        <v>0.225502191367047</v>
       </c>
       <c r="BB175" t="n">
         <v>0.623300836103931</v>
@@ -31607,7 +31673,7 @@
         <v>-0.743076622040612</v>
       </c>
       <c r="AW176" t="n">
-        <v>0.674176371300901</v>
+        <v>0.737983927288882</v>
       </c>
       <c r="AX176" t="n">
         <v>1.17863445462987</v>
@@ -31619,7 +31685,7 @@
         <v>1.50978542595462</v>
       </c>
       <c r="BA176" t="n">
-        <v>1.07280408933649</v>
+        <v>1.07746739984369</v>
       </c>
       <c r="BB176" t="n">
         <v>4.12037737307924</v>
@@ -31783,7 +31849,7 @@
         <v>0.388984956229725</v>
       </c>
       <c r="AW177" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX177" t="n">
         <v>0.347752036976961</v>
@@ -31795,7 +31861,7 @@
         <v>1.44592107331041</v>
       </c>
       <c r="BA177" t="n">
-        <v>-0.503742351388881</v>
+        <v>-0.501906700080844</v>
       </c>
       <c r="BB177" t="n">
         <v>-0.192151777175637</v>
@@ -31959,7 +32025,7 @@
         <v>0.102387088313184</v>
       </c>
       <c r="AW178" t="n">
-        <v>0.538154515373862</v>
+        <v>0.628235992448056</v>
       </c>
       <c r="AX178" t="n">
         <v>0.207372790749667</v>
@@ -31971,7 +32037,7 @@
         <v>-0.434458797196399</v>
       </c>
       <c r="BA178" t="n">
-        <v>-0.548502344974144</v>
+        <v>-0.546746974211193</v>
       </c>
       <c r="BB178" t="n">
         <v>-0.520453471703847</v>
@@ -32135,7 +32201,7 @@
         <v>-1.84647841351929</v>
       </c>
       <c r="AW179" t="n">
-        <v>0.187360638612032</v>
+        <v>0.345201304625029</v>
       </c>
       <c r="AX179" t="n">
         <v>1.08229862359752</v>
@@ -32147,7 +32213,7 @@
         <v>-1.45619080624921</v>
       </c>
       <c r="BA179" t="n">
-        <v>-1.17514225516782</v>
+        <v>-1.17451081203608</v>
       </c>
       <c r="BB179" t="n">
         <v>-0.997032639163638</v>
@@ -32311,7 +32377,7 @@
         <v>-1.0010147031655</v>
       </c>
       <c r="AW180" t="n">
-        <v>0.529653077116775</v>
+        <v>0.621376688216885</v>
       </c>
       <c r="AX180" t="n">
         <v>-0.124714293937849</v>
@@ -32323,7 +32389,7 @@
         <v>0.0368413309163744</v>
       </c>
       <c r="BA180" t="n">
-        <v>0.088084230460705</v>
+        <v>0.0909813689759986</v>
       </c>
       <c r="BB180" t="n">
         <v>0.602178330047691</v>
@@ -32436,7 +32502,7 @@
         <v>-0.206710230711924</v>
       </c>
       <c r="AF181" t="n">
-        <v>-0.0797972038841208</v>
+        <v>-0.0797972038841209</v>
       </c>
       <c r="AG181" t="n">
         <v>0.500062987363828</v>
@@ -32487,7 +32553,7 @@
         <v>0.446304529813032</v>
       </c>
       <c r="AW181" t="n">
-        <v>0.0575440348440829</v>
+        <v>0.240460018200999</v>
       </c>
       <c r="AX181" t="n">
         <v>0.72104424252072</v>
@@ -32499,7 +32565,7 @@
         <v>1.09632079701649</v>
       </c>
       <c r="BA181" t="n">
-        <v>-1.45364888192057</v>
+        <v>-1.45351696218048</v>
       </c>
       <c r="BB181" t="n">
         <v>-0.00651098463463178</v>
@@ -32663,7 +32729,7 @@
         <v>-1.08699406354046</v>
       </c>
       <c r="AW182" t="n">
-        <v>0.642928122725586</v>
+        <v>0.712771576485691</v>
       </c>
       <c r="AX182" t="n">
         <v>0.484162988777546</v>
@@ -32675,7 +32741,7 @@
         <v>1.13469066606166</v>
       </c>
       <c r="BA182" t="n">
-        <v>-0.633048999524085</v>
+        <v>-0.631445269790742</v>
       </c>
       <c r="BB182" t="n">
         <v>-0.381550948030825</v>
@@ -32839,7 +32905,7 @@
         <v>0.260015915667281</v>
       </c>
       <c r="AW183" t="n">
-        <v>0.0960831945643985</v>
+        <v>0.271554971000894</v>
       </c>
       <c r="AX183" t="n">
         <v>0.2722148546233</v>
@@ -32851,7 +32917,7 @@
         <v>0.0827655730337386</v>
       </c>
       <c r="BA183" t="n">
-        <v>-0.652942330006424</v>
+        <v>-0.651374280515342</v>
       </c>
       <c r="BB183" t="n">
         <v>-0.571705993854228</v>
@@ -33015,7 +33081,7 @@
         <v>-0.141221099415876</v>
       </c>
       <c r="AW184" t="n">
-        <v>0.0134979595221753</v>
+        <v>0.204921863163504</v>
       </c>
       <c r="AX184" t="n">
         <v>0.809350425868872</v>
@@ -33027,7 +33093,7 @@
         <v>0.538249113906517</v>
       </c>
       <c r="BA184" t="n">
-        <v>-0.508715684009466</v>
+        <v>-0.506888952761994</v>
       </c>
       <c r="BB184" t="n">
         <v>0.306851681007877</v>
@@ -33191,7 +33257,7 @@
         <v>0.331665382646416</v>
       </c>
       <c r="AW185" t="n">
-        <v>-0.166686746548472</v>
+        <v>0.0595415546360138</v>
       </c>
       <c r="AX185" t="n">
         <v>1.53314207047533</v>
@@ -33203,7 +33269,7 @@
         <v>0.853372647181154</v>
       </c>
       <c r="BA185" t="n">
-        <v>-0.891662295794492</v>
+        <v>-0.890522409210539</v>
       </c>
       <c r="BB185" t="n">
         <v>-0.309921296528971</v>
@@ -33367,7 +33433,7 @@
         <v>0.947850798666979</v>
       </c>
       <c r="AW186" t="n">
-        <v>0.674176371300901</v>
+        <v>0.737983927288882</v>
       </c>
       <c r="AX186" t="n">
         <v>1.13148686272258</v>
@@ -33379,7 +33445,7 @@
         <v>1.73625796408163</v>
       </c>
       <c r="BA186" t="n">
-        <v>-0.389355701115431</v>
+        <v>-0.387314888414395</v>
       </c>
       <c r="BB186" t="n">
         <v>1.35269918390487</v>
@@ -33468,7 +33534,7 @@
         <v>-0.439780163087157</v>
       </c>
       <c r="X187" t="n">
-        <v>-0.496062389612533</v>
+        <v>-0.496062389612534</v>
       </c>
       <c r="Y187" t="n">
         <v>-1.13637472450745</v>
@@ -33543,7 +33609,7 @@
         <v>-1.08699406354046</v>
       </c>
       <c r="AW187" t="n">
-        <v>0.569068626093024</v>
+        <v>0.653178747314513</v>
       </c>
       <c r="AX187" t="n">
         <v>-0.141351883468931</v>
@@ -33555,7 +33621,7 @@
         <v>-1.42884129081338</v>
       </c>
       <c r="BA187" t="n">
-        <v>-1.508355540747</v>
+        <v>-1.50832174167313</v>
       </c>
       <c r="BB187" t="n">
         <v>-1.1787680777022</v>
@@ -33650,7 +33716,7 @@
         <v>-0.347254902876174</v>
       </c>
       <c r="Z188" t="n">
-        <v>-0.916669512851651</v>
+        <v>-0.916669512851652</v>
       </c>
       <c r="AA188" t="n">
         <v>-0.108611663160268</v>
@@ -33719,7 +33785,7 @@
         <v>-0.0265819522492598</v>
       </c>
       <c r="AW188" t="n">
-        <v>0.353013238405877</v>
+        <v>0.478856522049352</v>
       </c>
       <c r="AX188" t="n">
         <v>0.255431029786711</v>
@@ -33731,7 +33797,7 @@
         <v>-0.286873928760236</v>
       </c>
       <c r="BA188" t="n">
-        <v>0.282044202663511</v>
+        <v>0.285289223540846</v>
       </c>
       <c r="BB188" t="n">
         <v>0.596456776468838</v>
@@ -33895,7 +33961,7 @@
         <v>0.274345809063109</v>
       </c>
       <c r="AW189" t="n">
-        <v>0.585239048432697</v>
+        <v>0.6662256980798</v>
       </c>
       <c r="AX189" t="n">
         <v>1.08229862359752</v>
@@ -33907,7 +33973,7 @@
         <v>0.378020739003813</v>
       </c>
       <c r="BA189" t="n">
-        <v>-0.0263024198127443</v>
+        <v>-0.0236104426904498</v>
       </c>
       <c r="BB189" t="n">
         <v>0.72303433885457</v>
@@ -34071,7 +34137,7 @@
         <v>-0.743076622040612</v>
       </c>
       <c r="AW190" t="n">
-        <v>0.585239048432697</v>
+        <v>0.6662256980798</v>
       </c>
       <c r="AX190" t="n">
         <v>-0.48313038067595</v>
@@ -34083,7 +34149,7 @@
         <v>0.593070186346379</v>
       </c>
       <c r="BA190" t="n">
-        <v>-0.692728990971102</v>
+        <v>-0.691232301964541</v>
       </c>
       <c r="BB190" t="n">
         <v>-0.845836648993669</v>
@@ -34247,7 +34313,7 @@
         <v>-0.184210779603357</v>
       </c>
       <c r="AW191" t="n">
-        <v>0.38512978293265</v>
+        <v>0.504769449144888</v>
       </c>
       <c r="AX191" t="n">
         <v>0.274268795959738</v>
@@ -34259,7 +34325,7 @@
         <v>0.198692858676269</v>
       </c>
       <c r="BA191" t="n">
-        <v>-0.812088973865136</v>
+        <v>-0.810806366312139</v>
       </c>
       <c r="BB191" t="n">
         <v>-0.260537465272234</v>
@@ -34423,7 +34489,7 @@
         <v>0.2170262354798</v>
       </c>
       <c r="AW192" t="n">
-        <v>0.552472727175272</v>
+        <v>0.639788504837397</v>
       </c>
       <c r="AX192" t="n">
         <v>1.73255385071203</v>
@@ -34435,7 +34501,7 @@
         <v>1.16673878187357</v>
       </c>
       <c r="BA192" t="n">
-        <v>1.22200406795403</v>
+        <v>1.22693498027818</v>
       </c>
       <c r="BB192" t="n">
         <v>1.20795962575507</v>
@@ -34599,7 +34665,7 @@
         <v>0.861871438292017</v>
       </c>
       <c r="AW193" t="n">
-        <v>0.261252508462492</v>
+        <v>0.40482025381776</v>
       </c>
       <c r="AX193" t="n">
         <v>0.770478422841398</v>
@@ -34611,7 +34677,7 @@
         <v>1.63676967767696</v>
       </c>
       <c r="BA193" t="n">
-        <v>0.674937479689706</v>
+        <v>0.678887185351691</v>
       </c>
       <c r="BB193" t="n">
         <v>0.973491409920044</v>
@@ -34775,7 +34841,7 @@
         <v>-1.73183926635268</v>
       </c>
       <c r="AW194" t="n">
-        <v>0.609943282247355</v>
+        <v>0.686158073097811</v>
       </c>
       <c r="AX194" t="n">
         <v>-0.320217603281908</v>
@@ -34787,7 +34853,7 @@
         <v>0.661437872857533</v>
       </c>
       <c r="BA194" t="n">
-        <v>-0.757382315038704</v>
+        <v>-0.75600158681949</v>
       </c>
       <c r="BB194" t="n">
         <v>-0.312766325923226</v>
@@ -34951,7 +35017,7 @@
         <v>-0.155550992811702</v>
       </c>
       <c r="AW195" t="n">
-        <v>0.491620327019281</v>
+        <v>0.590690327182698</v>
       </c>
       <c r="AX195" t="n">
         <v>1.11532786146406</v>
@@ -34963,7 +35029,7 @@
         <v>1.11139293069041</v>
       </c>
       <c r="BA195" t="n">
-        <v>0.655044149207368</v>
+        <v>0.658958174627091</v>
       </c>
       <c r="BB195" t="n">
         <v>0.872739575615004</v>
@@ -35058,7 +35124,7 @@
         <v>0.202046962063534</v>
       </c>
       <c r="Z196" t="n">
-        <v>-0.746982652954984</v>
+        <v>-0.746982652954985</v>
       </c>
       <c r="AA196" t="n">
         <v>-0.183476373623327</v>
@@ -35127,7 +35193,7 @@
         <v>-0.70008694185313</v>
       </c>
       <c r="AW196" t="n">
-        <v>0.288781305538684</v>
+        <v>0.427031600716194</v>
       </c>
       <c r="AX196" t="n">
         <v>0.0707890154062104</v>
@@ -35139,7 +35205,7 @@
         <v>1.00738910626198</v>
       </c>
       <c r="BA196" t="n">
-        <v>-0.747435649797534</v>
+        <v>-0.74603708145719</v>
       </c>
       <c r="BB196" t="n">
         <v>-0.401088216306503</v>
@@ -35303,7 +35369,7 @@
         <v>-0.915035342790536</v>
       </c>
       <c r="AW197" t="n">
-        <v>0.674176371300901</v>
+        <v>0.737983927288882</v>
       </c>
       <c r="AX197" t="n">
         <v>0.133497373231311</v>
@@ -35315,7 +35381,7 @@
         <v>-0.167541683364651</v>
       </c>
       <c r="BA197" t="n">
-        <v>-1.30942223592361</v>
+        <v>-1.30903163442713</v>
       </c>
       <c r="BB197" t="n">
         <v>-0.675281861026629</v>
@@ -35479,7 +35545,7 @@
         <v>0.833211651500363</v>
       </c>
       <c r="AW198" t="n">
-        <v>0.577827893906935</v>
+        <v>0.660246078860188</v>
       </c>
       <c r="AX198" t="n">
         <v>-0.835630584600363</v>
@@ -35491,7 +35557,7 @@
         <v>0.377276285437733</v>
       </c>
       <c r="BA198" t="n">
-        <v>0.60531082300152</v>
+        <v>0.609135647815592</v>
       </c>
       <c r="BB198" t="n">
         <v>0.540941959358798</v>
@@ -35655,7 +35721,7 @@
         <v>0.503624103396341</v>
       </c>
       <c r="AW199" t="n">
-        <v>0.509007057402808</v>
+        <v>0.604718644472016</v>
       </c>
       <c r="AX199" t="n">
         <v>1.08229862359752</v>
@@ -35667,7 +35733,7 @@
         <v>0.709449025791285</v>
       </c>
       <c r="BA199" t="n">
-        <v>-0.359515705391923</v>
+        <v>-0.357421372327496</v>
       </c>
       <c r="BB199" t="n">
         <v>0.129242060004159</v>
@@ -35754,7 +35820,7 @@
         <v>4.95581700265847</v>
       </c>
       <c r="X200" t="n">
-        <v>2.37447422831194</v>
+        <v>2.37447422831193</v>
       </c>
       <c r="Y200" t="n">
         <v>2.65857227656306</v>
@@ -35799,13 +35865,13 @@
         <v>2.79667962056473</v>
       </c>
       <c r="AM200" t="n">
-        <v>2.7710732043269</v>
+        <v>2.77107320432689</v>
       </c>
       <c r="AN200" t="n">
         <v>4.20978285746912</v>
       </c>
       <c r="AO200" t="n">
-        <v>5.72626295645676</v>
+        <v>5.72626295645677</v>
       </c>
       <c r="AP200" t="n">
         <v>8.96392647649603</v>
@@ -35829,7 +35895,7 @@
         <v>4.87424158912359</v>
       </c>
       <c r="AW200" t="n">
-        <v>1.56503656480595</v>
+        <v>1.67801055144193</v>
       </c>
       <c r="AX200" t="n">
         <v>3.39431868601786</v>
@@ -35841,7 +35907,7 @@
         <v>2.78741419522983</v>
       </c>
       <c r="BA200" t="n">
-        <v>0.958417439063037</v>
+        <v>0.962875588177237</v>
       </c>
       <c r="BB200" t="n">
         <v>5.03396008197187</v>
@@ -35973,7 +36039,7 @@
         <v>-5.96482137994877</v>
       </c>
       <c r="AM201" t="n">
-        <v>-3.20566976828206</v>
+        <v>-3.20566976828205</v>
       </c>
       <c r="AN201" t="n">
         <v>-2.83579152627353</v>
@@ -36003,7 +36069,7 @@
         <v>-9.45565180670346</v>
       </c>
       <c r="AW201" t="n">
-        <v>-5.78740009915341</v>
+        <v>-4.69672189979531</v>
       </c>
       <c r="AX201" t="n">
         <v>-3.58987160122657</v>
@@ -36015,7 +36081,7 @@
         <v>-3.920594899873</v>
       </c>
       <c r="BA201" t="n">
-        <v>-3.41587964117055</v>
+        <v>-3.41761152219376</v>
       </c>
       <c r="BB201" t="n">
         <v>-3.03583739370944</v>

</xml_diff>